<commit_message>
Added ClubList.swift source file.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB16A2-6B13-ED4F-BEF7-62FA7077EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C39EB-445D-AB41-A7C1-5F2F952670C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
                   <c:v>5795</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0</c:v>
+                  <c:v>5891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2663,6 +2663,9 @@
                 </c:pt>
                 <c:pt idx="193">
                   <c:v>4586</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>4665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3887,6 +3890,9 @@
                 </c:pt>
                 <c:pt idx="193">
                   <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5130,6 +5136,9 @@
                 </c:pt>
                 <c:pt idx="193">
                   <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6360,11 +6369,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P203" sqref="P203"/>
+      <selection pane="bottomRight" activeCell="I198" sqref="I198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13665,7 +13674,16 @@
       </c>
       <c r="H197">
         <f t="shared" ref="H197" si="310">SUM(I197:K197)</f>
-        <v>0</v>
+        <v>5891</v>
+      </c>
+      <c r="I197" s="5">
+        <v>4665</v>
+      </c>
+      <c r="J197" s="6">
+        <v>680</v>
+      </c>
+      <c r="K197" s="7">
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -13685,7 +13703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Starting to make first Image in Clubs or Musea view switch Not working reliably yet, but gives camera and "?" icons. No crashes.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055502D0-95EB-224F-85C8-3D0CBA5AC97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8F86CF-31DF-574B-A61D-379D8D81266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1464,7 +1464,7 @@
                   <c:v>6057</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>6292</c:v>
+                  <c:v>6248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2116,7 +2116,7 @@
             <c:numRef>
               <c:f>Table!$I$3:$I$300</c:f>
               <c:numCache>
-                <c:formatCode>_ * #.##0_ ;_ * \-#.##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="298"/>
                 <c:pt idx="0">
                   <c:v>239</c:v>
@@ -2713,7 +2713,7 @@
                   <c:v>4809</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>4969</c:v>
+                  <c:v>4937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3964,7 +3964,7 @@
                   <c:v>693</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>734</c:v>
+                  <c:v>729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5234,7 +5234,7 @@
                   <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>589</c:v>
+                  <c:v>582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6465,11 +6465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K201" sqref="K201"/>
+      <selection pane="bottomRight" activeCell="G202" sqref="G202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13914,20 +13914,20 @@
         <v>197</v>
       </c>
       <c r="G201" s="4">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H201">
         <f t="shared" ref="H201" si="317">SUM(I201:K201)</f>
-        <v>6292</v>
+        <v>6248</v>
       </c>
       <c r="I201" s="5">
-        <v>4969</v>
+        <v>4937</v>
       </c>
       <c r="J201" s="6">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="K201" s="7">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -13947,7 +13947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Prevented OrganizationType getter from returning a nil. More a hack than a solution. Threadsafety issue?
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8F86CF-31DF-574B-A61D-379D8D81266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1FF7F7-64C9-F64E-BB02-C79D6300676D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -860,6 +860,9 @@
                 <c:pt idx="198">
                   <c:v>45288</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>45290</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1465,6 +1468,9 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>6248</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>6193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,6 +2115,9 @@
                 <c:pt idx="198">
                   <c:v>45288</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>45290</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2714,6 +2723,9 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>4937</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>4907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3360,6 +3372,9 @@
                 <c:pt idx="198">
                   <c:v>45288</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>45290</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3965,6 +3980,9 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>718</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4630,6 +4648,9 @@
                 <c:pt idx="198">
                   <c:v>45288</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>45290</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5235,6 +5256,9 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6463,13 +6487,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K201"/>
+  <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G202" sqref="G202"/>
+      <selection pane="bottomRight" activeCell="G203" sqref="G203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13928,6 +13952,43 @@
       </c>
       <c r="K201" s="7">
         <v>582</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>45290</v>
+      </c>
+      <c r="B202" s="2">
+        <v>9</v>
+      </c>
+      <c r="C202">
+        <f t="shared" ref="C202" si="318">SUM(D202:F202)</f>
+        <v>1673</v>
+      </c>
+      <c r="D202">
+        <v>1105</v>
+      </c>
+      <c r="E202">
+        <v>371</v>
+      </c>
+      <c r="F202" s="3">
+        <v>197</v>
+      </c>
+      <c r="G202" s="4">
+        <v>69</v>
+      </c>
+      <c r="H202">
+        <f t="shared" ref="H202" si="319">SUM(I202:K202)</f>
+        <v>6193</v>
+      </c>
+      <c r="I202" s="5">
+        <v>4907</v>
+      </c>
+      <c r="J202" s="6">
+        <v>718</v>
+      </c>
+      <c r="K202" s="7">
+        <v>568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor: fixing a SwiftLint warning on cyclomatic_complexity. In this case really irrelevant because the code is trivial.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEF7843-6AAB-3C46-8DDA-362EC9E79394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB167CD4-1D25-104A-86EC-43054F568ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1488,7 +1488,7 @@
                   <c:v>5826</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>5867</c:v>
+                  <c:v>5880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2761,7 +2761,7 @@
                   <c:v>4637</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>4669</c:v>
+                  <c:v>4697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4036,7 +4036,7 @@
                   <c:v>653</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>659</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5330,7 +5330,7 @@
                   <c:v>536</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>539</c:v>
+                  <c:v>543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14162,16 +14162,16 @@
       </c>
       <c r="H205">
         <f t="shared" ref="H205" si="325">SUM(I205:K205)</f>
-        <v>5867</v>
+        <v>5880</v>
       </c>
       <c r="I205" s="5">
-        <v>4669</v>
+        <v>4697</v>
       </c>
       <c r="J205" s="6">
-        <v>659</v>
+        <v>640</v>
       </c>
       <c r="K205" s="7">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parse PhotoClub.description format (array of language/string pairs).
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB167CD4-1D25-104A-86EC-43054F568ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86311CC5-98D3-A649-8717-F6F56988AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -872,6 +872,9 @@
                 <c:pt idx="202">
                   <c:v>45297</c:v>
                 </c:pt>
+                <c:pt idx="203">
+                  <c:v>45298</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1489,6 +1492,9 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>5880</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>5893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2145,6 +2151,9 @@
                 <c:pt idx="202">
                   <c:v>45297</c:v>
                 </c:pt>
+                <c:pt idx="203">
+                  <c:v>45298</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2762,6 +2771,9 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>4697</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>4690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3420,6 +3432,9 @@
                 <c:pt idx="202">
                   <c:v>45297</c:v>
                 </c:pt>
+                <c:pt idx="203">
+                  <c:v>45298</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4037,6 +4052,9 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4714,6 +4732,9 @@
                 <c:pt idx="202">
                   <c:v>45297</c:v>
                 </c:pt>
+                <c:pt idx="203">
+                  <c:v>45298</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5331,6 +5352,9 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6559,13 +6583,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K205"/>
+  <dimension ref="A1:K206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I206" sqref="I206"/>
+      <selection pane="bottomRight" activeCell="I207" sqref="I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14172,6 +14196,43 @@
       </c>
       <c r="K205" s="7">
         <v>543</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B206" s="2">
+        <v>9</v>
+      </c>
+      <c r="C206">
+        <f t="shared" ref="C206" si="326">SUM(D206:F206)</f>
+        <v>1673</v>
+      </c>
+      <c r="D206">
+        <v>1105</v>
+      </c>
+      <c r="E206">
+        <v>371</v>
+      </c>
+      <c r="F206" s="3">
+        <v>197</v>
+      </c>
+      <c r="G206" s="4">
+        <v>63</v>
+      </c>
+      <c r="H206">
+        <f t="shared" ref="H206" si="327">SUM(I206:K206)</f>
+        <v>5893</v>
+      </c>
+      <c r="I206" s="5">
+        <v>4690</v>
+      </c>
+      <c r="J206" s="6">
+        <v>664</v>
+      </c>
+      <c r="K206" s="7">
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -14192,7 +14253,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Chapter 5 of Readme screen
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAD0DFB-7ABA-754F-A0C3-51C21465E633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E26D7-4C55-7D4E-9C95-8DC7E457AE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -875,6 +875,9 @@
                 <c:pt idx="203">
                   <c:v>45298</c:v>
                 </c:pt>
+                <c:pt idx="204">
+                  <c:v>45305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1495,6 +1498,9 @@
                 </c:pt>
                 <c:pt idx="203">
                   <c:v>5899</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>5912</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,6 +2160,9 @@
                 <c:pt idx="203">
                   <c:v>45298</c:v>
                 </c:pt>
+                <c:pt idx="204">
+                  <c:v>45305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2774,6 +2783,9 @@
                 </c:pt>
                 <c:pt idx="203">
                   <c:v>4706</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>4722</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3435,6 +3447,9 @@
                 <c:pt idx="203">
                   <c:v>45298</c:v>
                 </c:pt>
+                <c:pt idx="204">
+                  <c:v>45305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4055,6 +4070,9 @@
                 </c:pt>
                 <c:pt idx="203">
                   <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4735,6 +4753,9 @@
                 <c:pt idx="203">
                   <c:v>45298</c:v>
                 </c:pt>
+                <c:pt idx="204">
+                  <c:v>45305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5355,6 +5376,9 @@
                 </c:pt>
                 <c:pt idx="203">
                   <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6583,13 +6607,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K206"/>
+  <dimension ref="A1:K207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I207" sqref="I207"/>
+      <selection pane="bottomRight" activeCell="I208" sqref="I208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14233,6 +14257,43 @@
       </c>
       <c r="K206" s="7">
         <v>546</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B207" s="2">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <f t="shared" ref="C207" si="328">SUM(D207:F207)</f>
+        <v>1673</v>
+      </c>
+      <c r="D207">
+        <v>1105</v>
+      </c>
+      <c r="E207">
+        <v>371</v>
+      </c>
+      <c r="F207" s="3">
+        <v>197</v>
+      </c>
+      <c r="G207" s="4">
+        <v>63</v>
+      </c>
+      <c r="H207">
+        <f t="shared" ref="H207" si="329">SUM(I207:K207)</f>
+        <v>5912</v>
+      </c>
+      <c r="I207" s="5">
+        <v>4722</v>
+      </c>
+      <c r="J207" s="6">
+        <v>646</v>
+      </c>
+      <c r="K207" s="7">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -14253,7 +14314,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Preparation for release 4614
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E26D7-4C55-7D4E-9C95-8DC7E457AE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BBA6CC-E0FA-AD47-A206-8B44B18E41ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -878,6 +878,9 @@
                 <c:pt idx="204">
                   <c:v>45305</c:v>
                 </c:pt>
+                <c:pt idx="205">
+                  <c:v>45310</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1501,6 +1504,9 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>5912</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>5901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2163,6 +2169,9 @@
                 <c:pt idx="204">
                   <c:v>45305</c:v>
                 </c:pt>
+                <c:pt idx="205">
+                  <c:v>45310</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2786,6 +2795,9 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>4722</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>4702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3450,6 +3462,9 @@
                 <c:pt idx="204">
                   <c:v>45305</c:v>
                 </c:pt>
+                <c:pt idx="205">
+                  <c:v>45310</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4073,6 +4088,9 @@
                 </c:pt>
                 <c:pt idx="204">
                   <c:v>646</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>655</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4756,6 +4774,9 @@
                 <c:pt idx="204">
                   <c:v>45305</c:v>
                 </c:pt>
+                <c:pt idx="205">
+                  <c:v>45310</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5378,6 +5399,9 @@
                   <c:v>546</c:v>
                 </c:pt>
                 <c:pt idx="204">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="205">
                   <c:v>544</c:v>
                 </c:pt>
               </c:numCache>
@@ -6607,13 +6631,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K207"/>
+  <dimension ref="A1:K208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I208" sqref="I208"/>
+      <selection pane="bottomRight" activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14293,6 +14317,43 @@
         <v>646</v>
       </c>
       <c r="K207" s="7">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>45310</v>
+      </c>
+      <c r="B208" s="2">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <f t="shared" ref="C208" si="330">SUM(D208:F208)</f>
+        <v>1673</v>
+      </c>
+      <c r="D208">
+        <v>1105</v>
+      </c>
+      <c r="E208">
+        <v>371</v>
+      </c>
+      <c r="F208" s="3">
+        <v>197</v>
+      </c>
+      <c r="G208" s="4">
+        <v>63</v>
+      </c>
+      <c r="H208">
+        <f t="shared" ref="H208" si="331">SUM(I208:K208)</f>
+        <v>5901</v>
+      </c>
+      <c r="I208" s="5">
+        <v>4702</v>
+      </c>
+      <c r="J208" s="6">
+        <v>655</v>
+      </c>
+      <c r="K208" s="7">
         <v>544</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hide membercount & show wikipediaURL Membercount is hidden if count is zero (e.g. musea, clubs with no member data). Wikipedia URL is shown if availabe (presumably for musea only, but it will display if a club would have a wikipedia link).
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BBA6CC-E0FA-AD47-A206-8B44B18E41ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861E49B3-3FC5-0240-9DE5-6138409C529C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -879,6 +879,9 @@
                   <c:v>45305</c:v>
                 </c:pt>
                 <c:pt idx="205">
+                  <c:v>45309</c:v>
+                </c:pt>
+                <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
               </c:numCache>
@@ -1507,6 +1510,9 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>5901</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>5912</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,6 +2176,9 @@
                   <c:v>45305</c:v>
                 </c:pt>
                 <c:pt idx="205">
+                  <c:v>45309</c:v>
+                </c:pt>
+                <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
               </c:numCache>
@@ -2798,6 +2807,9 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>4702</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>4724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3463,6 +3475,9 @@
                   <c:v>45305</c:v>
                 </c:pt>
                 <c:pt idx="205">
+                  <c:v>45309</c:v>
+                </c:pt>
+                <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
               </c:numCache>
@@ -4091,6 +4106,9 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4775,6 +4793,9 @@
                   <c:v>45305</c:v>
                 </c:pt>
                 <c:pt idx="205">
+                  <c:v>45309</c:v>
+                </c:pt>
+                <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
               </c:numCache>
@@ -5403,6 +5424,9 @@
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6631,9 +6655,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K208"/>
+  <dimension ref="A1:K209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -14322,7 +14346,7 @@
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>45310</v>
+        <v>45309</v>
       </c>
       <c r="B208" s="2">
         <v>9</v>
@@ -14355,6 +14379,43 @@
       </c>
       <c r="K208" s="7">
         <v>544</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>45310</v>
+      </c>
+      <c r="B209" s="2">
+        <v>9</v>
+      </c>
+      <c r="C209">
+        <f t="shared" ref="C209" si="332">SUM(D209:F209)</f>
+        <v>1673</v>
+      </c>
+      <c r="D209">
+        <v>1105</v>
+      </c>
+      <c r="E209">
+        <v>371</v>
+      </c>
+      <c r="F209" s="3">
+        <v>197</v>
+      </c>
+      <c r="G209" s="4">
+        <v>63</v>
+      </c>
+      <c r="H209">
+        <f t="shared" ref="H209" si="333">SUM(I209:K209)</f>
+        <v>5912</v>
+      </c>
+      <c r="I209" s="5">
+        <v>4724</v>
+      </c>
+      <c r="J209" s="6">
+        <v>643</v>
+      </c>
+      <c r="K209" s="7">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -14374,7 +14435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed EN text "musea" to "museums"
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861E49B3-3FC5-0240-9DE5-6138409C529C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E32E56-386C-8142-BA03-94E97CEE1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -884,6 +884,9 @@
                 <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
+                <c:pt idx="207">
+                  <c:v>45312</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1513,6 +1516,9 @@
                 </c:pt>
                 <c:pt idx="206">
                   <c:v>5912</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>5922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2181,6 +2187,9 @@
                 <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
+                <c:pt idx="207">
+                  <c:v>45312</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2810,6 +2819,9 @@
                 </c:pt>
                 <c:pt idx="206">
                   <c:v>4724</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>4738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3480,6 +3492,9 @@
                 <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
+                <c:pt idx="207">
+                  <c:v>45312</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4109,6 +4124,9 @@
                 </c:pt>
                 <c:pt idx="206">
                   <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4798,6 +4816,9 @@
                 <c:pt idx="206">
                   <c:v>45310</c:v>
                 </c:pt>
+                <c:pt idx="207">
+                  <c:v>45312</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5427,6 +5448,9 @@
                 </c:pt>
                 <c:pt idx="206">
                   <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6655,13 +6679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K209"/>
+  <dimension ref="A1:K210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A209" sqref="A209"/>
+      <selection pane="bottomRight" activeCell="J211" sqref="J211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14416,6 +14440,43 @@
       </c>
       <c r="K209" s="7">
         <v>545</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B210" s="2">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <f t="shared" ref="C210" si="334">SUM(D210:F210)</f>
+        <v>1673</v>
+      </c>
+      <c r="D210">
+        <v>1105</v>
+      </c>
+      <c r="E210">
+        <v>371</v>
+      </c>
+      <c r="F210" s="3">
+        <v>197</v>
+      </c>
+      <c r="G210" s="4">
+        <v>63</v>
+      </c>
+      <c r="H210">
+        <f t="shared" ref="H210" si="335">SUM(I210:K210)</f>
+        <v>5922</v>
+      </c>
+      <c r="I210" s="5">
+        <v>4738</v>
+      </c>
+      <c r="J210" s="6">
+        <v>640</v>
+      </c>
+      <c r="K210" s="7">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -14435,8 +14496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA43" sqref="AA43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Moved SwiftJSON file. Minor updates to organization.swift file
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E32E56-386C-8142-BA03-94E97CEE1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3310658C-C463-C04C-8D7C-43396C30CAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -887,6 +887,9 @@
                 <c:pt idx="207">
                   <c:v>45312</c:v>
                 </c:pt>
+                <c:pt idx="208">
+                  <c:v>45317</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1519,6 +1522,9 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>5922</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>7333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,6 +2196,9 @@
                 <c:pt idx="207">
                   <c:v>45312</c:v>
                 </c:pt>
+                <c:pt idx="208">
+                  <c:v>45317</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2822,6 +2831,9 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>4738</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>6028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3495,6 +3507,9 @@
                 <c:pt idx="207">
                   <c:v>45312</c:v>
                 </c:pt>
+                <c:pt idx="208">
+                  <c:v>45317</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4127,6 +4142,9 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4819,6 +4837,9 @@
                 <c:pt idx="207">
                   <c:v>45312</c:v>
                 </c:pt>
+                <c:pt idx="208">
+                  <c:v>45317</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5451,6 +5472,9 @@
                 </c:pt>
                 <c:pt idx="207">
                   <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6679,13 +6703,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:K211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J211" sqref="J211"/>
+      <selection pane="bottomRight" activeCell="I212" sqref="I212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14477,6 +14501,43 @@
       </c>
       <c r="K210" s="7">
         <v>544</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>45317</v>
+      </c>
+      <c r="B211" s="2">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <f t="shared" ref="C211" si="336">SUM(D211:F211)</f>
+        <v>1673</v>
+      </c>
+      <c r="D211">
+        <v>1105</v>
+      </c>
+      <c r="E211">
+        <v>371</v>
+      </c>
+      <c r="F211" s="3">
+        <v>197</v>
+      </c>
+      <c r="G211" s="4">
+        <v>64</v>
+      </c>
+      <c r="H211">
+        <f t="shared" ref="H211" si="337">SUM(I211:K211)</f>
+        <v>7333</v>
+      </c>
+      <c r="I211" s="5">
+        <v>6028</v>
+      </c>
+      <c r="J211" s="6">
+        <v>740</v>
+      </c>
+      <c r="K211" s="7">
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interim version of English and Dutch Readme screen.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3310658C-C463-C04C-8D7C-43396C30CAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD44054-8136-5945-BBEC-CDB146FF9236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -890,6 +890,12 @@
                 <c:pt idx="208">
                   <c:v>45317</c:v>
                 </c:pt>
+                <c:pt idx="209">
+                  <c:v>45327</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>45329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1525,6 +1531,12 @@
                 </c:pt>
                 <c:pt idx="208">
                   <c:v>7333</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>7314</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>7314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2199,6 +2211,12 @@
                 <c:pt idx="208">
                   <c:v>45317</c:v>
                 </c:pt>
+                <c:pt idx="209">
+                  <c:v>45327</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>45329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2834,6 +2852,12 @@
                 </c:pt>
                 <c:pt idx="208">
                   <c:v>6028</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6008</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>6007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,6 +3534,12 @@
                 <c:pt idx="208">
                   <c:v>45317</c:v>
                 </c:pt>
+                <c:pt idx="209">
+                  <c:v>45327</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>45329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4145,6 +4175,12 @@
                 </c:pt>
                 <c:pt idx="208">
                   <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4840,6 +4876,12 @@
                 <c:pt idx="208">
                   <c:v>45317</c:v>
                 </c:pt>
+                <c:pt idx="209">
+                  <c:v>45327</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>45329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5474,6 +5516,12 @@
                   <c:v>544</c:v>
                 </c:pt>
                 <c:pt idx="208">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="210">
                   <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
@@ -6703,13 +6751,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K211"/>
+  <dimension ref="A1:K213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I212" sqref="I212"/>
+      <selection pane="bottomRight" activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14537,6 +14585,80 @@
         <v>740</v>
       </c>
       <c r="K211" s="7">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>45327</v>
+      </c>
+      <c r="B212" s="2">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <f t="shared" ref="C212" si="338">SUM(D212:F212)</f>
+        <v>1673</v>
+      </c>
+      <c r="D212">
+        <v>1105</v>
+      </c>
+      <c r="E212">
+        <v>371</v>
+      </c>
+      <c r="F212" s="3">
+        <v>197</v>
+      </c>
+      <c r="G212" s="4">
+        <v>64</v>
+      </c>
+      <c r="H212">
+        <f t="shared" ref="H212" si="339">SUM(I212:K212)</f>
+        <v>7314</v>
+      </c>
+      <c r="I212" s="5">
+        <v>6008</v>
+      </c>
+      <c r="J212" s="6">
+        <v>742</v>
+      </c>
+      <c r="K212" s="7">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>45329</v>
+      </c>
+      <c r="B213" s="2">
+        <v>9</v>
+      </c>
+      <c r="C213">
+        <f t="shared" ref="C213" si="340">SUM(D213:F213)</f>
+        <v>1673</v>
+      </c>
+      <c r="D213">
+        <v>1105</v>
+      </c>
+      <c r="E213">
+        <v>371</v>
+      </c>
+      <c r="F213" s="3">
+        <v>197</v>
+      </c>
+      <c r="G213" s="4">
+        <v>64</v>
+      </c>
+      <c r="H213">
+        <f t="shared" ref="H213" si="341">SUM(I213:K213)</f>
+        <v>7314</v>
+      </c>
+      <c r="I213" s="5">
+        <v>6007</v>
+      </c>
+      <c r="J213" s="6">
+        <v>742</v>
+      </c>
+      <c r="K213" s="7">
         <v>565</v>
       </c>
     </row>
@@ -14557,7 +14679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaned up Organization.localizedRemark: String  computed property.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD44054-8136-5945-BBEC-CDB146FF9236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619F440-0087-A041-B447-F5683F50BD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Code</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>SwiftyJSON file</t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -179,6 +182,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -896,6 +900,9 @@
                 <c:pt idx="210">
                   <c:v>45329</c:v>
                 </c:pt>
+                <c:pt idx="211">
+                  <c:v>45337</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1529,14 +1536,17 @@
                 <c:pt idx="207">
                   <c:v>5922</c:v>
                 </c:pt>
-                <c:pt idx="208">
-                  <c:v>7333</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>7314</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>7314</c:v>
+                <c:pt idx="208" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5922</c:v>
+                </c:pt>
+                <c:pt idx="209" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5903</c:v>
+                </c:pt>
+                <c:pt idx="210" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5903</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2217,6 +2227,9 @@
                 <c:pt idx="210">
                   <c:v>45329</c:v>
                 </c:pt>
+                <c:pt idx="211">
+                  <c:v>45337</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2858,6 +2871,9 @@
                 </c:pt>
                 <c:pt idx="210">
                   <c:v>6007</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>6021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3540,6 +3556,9 @@
                 <c:pt idx="210">
                   <c:v>45329</c:v>
                 </c:pt>
+                <c:pt idx="211">
+                  <c:v>45337</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4180,6 +4199,9 @@
                   <c:v>742</c:v>
                 </c:pt>
                 <c:pt idx="210">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="211">
                   <c:v>742</c:v>
                 </c:pt>
               </c:numCache>
@@ -4882,6 +4904,9 @@
                 <c:pt idx="210">
                   <c:v>45329</c:v>
                 </c:pt>
+                <c:pt idx="211">
+                  <c:v>45337</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5522,6 +5547,9 @@
                   <c:v>564</c:v>
                 </c:pt>
                 <c:pt idx="210">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="211">
                   <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
@@ -5549,7 +5577,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45330"/>
+          <c:max val="45430"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6455,9 +6483,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6495,7 +6523,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6601,7 +6629,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6743,7 +6771,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6751,13 +6779,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K213"/>
+  <dimension ref="A1:N214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I214" sqref="I214"/>
+      <selection pane="bottomRight" activeCell="P201" sqref="P201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6771,7 +6799,7 @@
     <col min="11" max="11" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
@@ -6786,8 +6814,13 @@
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -6821,8 +6854,17 @@
       <c r="K2" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44380</v>
       </c>
@@ -6859,7 +6901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>44381</v>
@@ -6897,7 +6939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>44382</v>
@@ -6935,7 +6977,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>44383</v>
@@ -6973,7 +7015,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A27" si="2">A6+1</f>
         <v>44384</v>
@@ -7011,7 +7053,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44387</v>
       </c>
@@ -7048,7 +7090,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44392</v>
       </c>
@@ -7085,7 +7127,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>44393</v>
@@ -7123,7 +7165,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>44394</v>
@@ -7161,7 +7203,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>44395</v>
@@ -7200,7 +7242,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>44396</v>
@@ -7239,7 +7281,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>44397</v>
@@ -7278,7 +7320,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>44398</v>
@@ -7317,7 +7359,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44400</v>
       </c>
@@ -14477,7 +14519,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>45310</v>
       </c>
@@ -14514,7 +14556,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>45312</v>
       </c>
@@ -14551,7 +14593,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>45317</v>
       </c>
@@ -14574,9 +14616,9 @@
       <c r="G211" s="4">
         <v>64</v>
       </c>
-      <c r="H211">
-        <f t="shared" ref="H211" si="337">SUM(I211:K211)</f>
-        <v>7333</v>
+      <c r="H211" s="19">
+        <f t="shared" ref="H211:H212" si="337">SUM(I211:K211)-SUM(L211:N211)</f>
+        <v>5922</v>
       </c>
       <c r="I211" s="5">
         <v>6028</v>
@@ -14587,8 +14629,17 @@
       <c r="K211" s="7">
         <v>565</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L211">
+        <v>1305</v>
+      </c>
+      <c r="M211">
+        <v>86</v>
+      </c>
+      <c r="N211">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>45327</v>
       </c>
@@ -14611,9 +14662,9 @@
       <c r="G212" s="4">
         <v>64</v>
       </c>
-      <c r="H212">
-        <f t="shared" ref="H212" si="339">SUM(I212:K212)</f>
-        <v>7314</v>
+      <c r="H212" s="19">
+        <f t="shared" si="337"/>
+        <v>5903</v>
       </c>
       <c r="I212" s="5">
         <v>6008</v>
@@ -14624,8 +14675,17 @@
       <c r="K212" s="7">
         <v>564</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L212">
+        <v>1305</v>
+      </c>
+      <c r="M212">
+        <v>86</v>
+      </c>
+      <c r="N212">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>45329</v>
       </c>
@@ -14633,7 +14693,7 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <f t="shared" ref="C213" si="340">SUM(D213:F213)</f>
+        <f t="shared" ref="C213" si="339">SUM(D213:F213)</f>
         <v>1673</v>
       </c>
       <c r="D213">
@@ -14648,9 +14708,9 @@
       <c r="G213" s="4">
         <v>64</v>
       </c>
-      <c r="H213">
-        <f t="shared" ref="H213" si="341">SUM(I213:K213)</f>
-        <v>7314</v>
+      <c r="H213" s="19">
+        <f>SUM(I213:K213)-SUM(L213:N213)</f>
+        <v>5903</v>
       </c>
       <c r="I213" s="5">
         <v>6007</v>
@@ -14661,11 +14721,67 @@
       <c r="K213" s="7">
         <v>565</v>
       </c>
+      <c r="L213">
+        <v>1305</v>
+      </c>
+      <c r="M213">
+        <v>86</v>
+      </c>
+      <c r="N213">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>45337</v>
+      </c>
+      <c r="B214" s="2">
+        <v>9</v>
+      </c>
+      <c r="C214">
+        <f t="shared" ref="C214" si="340">SUM(D214:F214)</f>
+        <v>1673</v>
+      </c>
+      <c r="D214">
+        <v>1105</v>
+      </c>
+      <c r="E214">
+        <v>371</v>
+      </c>
+      <c r="F214" s="3">
+        <v>197</v>
+      </c>
+      <c r="G214" s="4">
+        <v>64</v>
+      </c>
+      <c r="H214" s="19">
+        <f>SUM(I214:K214)-SUM(L214:N214)</f>
+        <v>5917</v>
+      </c>
+      <c r="I214" s="5">
+        <v>6021</v>
+      </c>
+      <c r="J214" s="6">
+        <v>742</v>
+      </c>
+      <c r="K214" s="7">
+        <v>565</v>
+      </c>
+      <c r="L214">
+        <v>1305</v>
+      </c>
+      <c r="M214">
+        <v>86</v>
+      </c>
+      <c r="N214">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -14679,7 +14795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated ReleaseNotes and line count.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619F440-0087-A041-B447-F5683F50BD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D980B61B-3291-BD41-8585-DBEE9C7D2CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -173,6 +173,7 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -182,7 +183,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -903,6 +903,9 @@
                 <c:pt idx="211">
                   <c:v>45337</c:v>
                 </c:pt>
+                <c:pt idx="212">
+                  <c:v>45343</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1547,6 +1550,9 @@
                 </c:pt>
                 <c:pt idx="211" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>5917</c:v>
+                </c:pt>
+                <c:pt idx="212" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,6 +2236,9 @@
                 <c:pt idx="211">
                   <c:v>45337</c:v>
                 </c:pt>
+                <c:pt idx="212">
+                  <c:v>45343</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2874,6 +2883,9 @@
                 </c:pt>
                 <c:pt idx="211">
                   <c:v>6021</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>6026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3559,6 +3571,9 @@
                 <c:pt idx="211">
                   <c:v>45337</c:v>
                 </c:pt>
+                <c:pt idx="212">
+                  <c:v>45343</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4203,6 +4218,9 @@
                 </c:pt>
                 <c:pt idx="211">
                   <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>741</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4907,6 +4925,9 @@
                 <c:pt idx="211">
                   <c:v>45337</c:v>
                 </c:pt>
+                <c:pt idx="212">
+                  <c:v>45343</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5551,6 +5572,9 @@
                 </c:pt>
                 <c:pt idx="211">
                   <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6779,13 +6803,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N214"/>
+  <dimension ref="A1:N215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P201" sqref="P201"/>
+      <selection pane="bottomRight" activeCell="M219" sqref="M219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6800,25 +6824,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="16" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -14616,7 +14640,7 @@
       <c r="G211" s="4">
         <v>64</v>
       </c>
-      <c r="H211" s="19">
+      <c r="H211" s="16">
         <f t="shared" ref="H211:H212" si="337">SUM(I211:K211)-SUM(L211:N211)</f>
         <v>5922</v>
       </c>
@@ -14662,7 +14686,7 @@
       <c r="G212" s="4">
         <v>64</v>
       </c>
-      <c r="H212" s="19">
+      <c r="H212" s="16">
         <f t="shared" si="337"/>
         <v>5903</v>
       </c>
@@ -14708,7 +14732,7 @@
       <c r="G213" s="4">
         <v>64</v>
       </c>
-      <c r="H213" s="19">
+      <c r="H213" s="16">
         <f>SUM(I213:K213)-SUM(L213:N213)</f>
         <v>5903</v>
       </c>
@@ -14754,7 +14778,7 @@
       <c r="G214" s="4">
         <v>64</v>
       </c>
-      <c r="H214" s="19">
+      <c r="H214" s="16">
         <f>SUM(I214:K214)-SUM(L214:N214)</f>
         <v>5917</v>
       </c>
@@ -14774,6 +14798,52 @@
         <v>86</v>
       </c>
       <c r="N214">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>45343</v>
+      </c>
+      <c r="B215" s="2">
+        <v>9</v>
+      </c>
+      <c r="C215">
+        <f t="shared" ref="C215" si="341">SUM(D215:F215)</f>
+        <v>1673</v>
+      </c>
+      <c r="D215">
+        <v>1105</v>
+      </c>
+      <c r="E215">
+        <v>371</v>
+      </c>
+      <c r="F215" s="3">
+        <v>197</v>
+      </c>
+      <c r="G215" s="4">
+        <v>64</v>
+      </c>
+      <c r="H215" s="16">
+        <f>SUM(I215:K215)-SUM(L215:N215)</f>
+        <v>5922</v>
+      </c>
+      <c r="I215" s="5">
+        <v>6026</v>
+      </c>
+      <c r="J215" s="6">
+        <v>741</v>
+      </c>
+      <c r="K215" s="7">
+        <v>566</v>
+      </c>
+      <c r="L215">
+        <v>1305</v>
+      </c>
+      <c r="M215">
+        <v>86</v>
+      </c>
+      <c r="N215">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Preparations for the next release.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C7800F-0579-9845-83DA-786634B3AE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B2DF71-365F-2040-853A-3017EF27586D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -907,6 +907,9 @@
                   <c:v>45343</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>45351</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
               </c:numCache>
@@ -1558,6 +1561,9 @@
                   <c:v>5922</c:v>
                 </c:pt>
                 <c:pt idx="213" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5947</c:v>
+                </c:pt>
+                <c:pt idx="214" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>5947</c:v>
                 </c:pt>
               </c:numCache>
@@ -2246,6 +2252,9 @@
                   <c:v>45343</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>45351</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
               </c:numCache>
@@ -2897,6 +2906,9 @@
                   <c:v>6026</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>6052</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>6052</c:v>
                 </c:pt>
               </c:numCache>
@@ -3587,6 +3599,9 @@
                   <c:v>45343</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>45351</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
               </c:numCache>
@@ -4238,6 +4253,9 @@
                   <c:v>741</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>741</c:v>
                 </c:pt>
               </c:numCache>
@@ -4947,6 +4965,9 @@
                   <c:v>45343</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>45351</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
               </c:numCache>
@@ -5598,6 +5619,9 @@
                   <c:v>566</c:v>
                 </c:pt>
                 <c:pt idx="213">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="214">
                   <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
@@ -6827,13 +6851,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N216"/>
+  <dimension ref="A1:N217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N220" sqref="N220"/>
+      <selection pane="bottomRight" activeCell="R205" sqref="R205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14873,7 +14897,7 @@
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>45352</v>
+        <v>45351</v>
       </c>
       <c r="B216" s="2">
         <v>9</v>
@@ -14914,6 +14938,52 @@
         <v>86</v>
       </c>
       <c r="N216">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>45352</v>
+      </c>
+      <c r="B217" s="2">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <f t="shared" ref="C217" si="343">SUM(D217:F217)</f>
+        <v>1673</v>
+      </c>
+      <c r="D217">
+        <v>1105</v>
+      </c>
+      <c r="E217">
+        <v>371</v>
+      </c>
+      <c r="F217" s="3">
+        <v>197</v>
+      </c>
+      <c r="G217" s="4">
+        <v>64</v>
+      </c>
+      <c r="H217" s="16">
+        <f>SUM(I217:K217)-SUM(L217:N217)</f>
+        <v>5947</v>
+      </c>
+      <c r="I217" s="5">
+        <v>6052</v>
+      </c>
+      <c r="J217" s="6">
+        <v>741</v>
+      </c>
+      <c r="K217" s="7">
+        <v>565</v>
+      </c>
+      <c r="L217">
+        <v>1305</v>
+      </c>
+      <c r="M217">
+        <v>86</v>
+      </c>
+      <c r="N217">
         <v>20</v>
       </c>
     </row>
@@ -14935,7 +15005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added a photography museum in Lausanne, Switzerland.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B2DF71-365F-2040-853A-3017EF27586D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E3259-BECF-2244-B201-EFF01284DFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -912,6 +912,9 @@
                 <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
+                <c:pt idx="215">
+                  <c:v>45353</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1565,6 +1568,9 @@
                 </c:pt>
                 <c:pt idx="214" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>5947</c:v>
+                </c:pt>
+                <c:pt idx="215" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2257,6 +2263,9 @@
                 <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
+                <c:pt idx="215">
+                  <c:v>45353</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2910,6 +2919,9 @@
                 </c:pt>
                 <c:pt idx="214">
                   <c:v>6052</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>6125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3604,6 +3616,9 @@
                 <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
+                <c:pt idx="215">
+                  <c:v>45353</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4257,6 +4272,9 @@
                 </c:pt>
                 <c:pt idx="214">
                   <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>756</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4970,6 +4988,9 @@
                 <c:pt idx="214">
                   <c:v>45352</c:v>
                 </c:pt>
+                <c:pt idx="215">
+                  <c:v>45353</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5623,6 +5644,9 @@
                 </c:pt>
                 <c:pt idx="214">
                   <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6851,13 +6875,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N217"/>
+  <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R205" sqref="R205"/>
+      <selection pane="bottomRight" activeCell="I219" sqref="I219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14781,7 +14805,7 @@
         <v>64</v>
       </c>
       <c r="H213" s="16">
-        <f>SUM(I213:K213)-SUM(L213:N213)</f>
+        <f t="shared" ref="H213:H218" si="340">SUM(I213:K213)-SUM(L213:N213)</f>
         <v>5903</v>
       </c>
       <c r="I213" s="5">
@@ -14811,7 +14835,7 @@
         <v>9</v>
       </c>
       <c r="C214">
-        <f t="shared" ref="C214" si="340">SUM(D214:F214)</f>
+        <f t="shared" ref="C214" si="341">SUM(D214:F214)</f>
         <v>1673</v>
       </c>
       <c r="D214">
@@ -14827,7 +14851,7 @@
         <v>64</v>
       </c>
       <c r="H214" s="16">
-        <f>SUM(I214:K214)-SUM(L214:N214)</f>
+        <f t="shared" si="340"/>
         <v>5917</v>
       </c>
       <c r="I214" s="5">
@@ -14857,7 +14881,7 @@
         <v>9</v>
       </c>
       <c r="C215">
-        <f t="shared" ref="C215" si="341">SUM(D215:F215)</f>
+        <f t="shared" ref="C215" si="342">SUM(D215:F215)</f>
         <v>1673</v>
       </c>
       <c r="D215">
@@ -14873,7 +14897,7 @@
         <v>64</v>
       </c>
       <c r="H215" s="16">
-        <f>SUM(I215:K215)-SUM(L215:N215)</f>
+        <f t="shared" si="340"/>
         <v>5922</v>
       </c>
       <c r="I215" s="5">
@@ -14903,7 +14927,7 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <f t="shared" ref="C216" si="342">SUM(D216:F216)</f>
+        <f t="shared" ref="C216" si="343">SUM(D216:F216)</f>
         <v>1673</v>
       </c>
       <c r="D216">
@@ -14919,7 +14943,7 @@
         <v>64</v>
       </c>
       <c r="H216" s="16">
-        <f>SUM(I216:K216)-SUM(L216:N216)</f>
+        <f t="shared" si="340"/>
         <v>5947</v>
       </c>
       <c r="I216" s="5">
@@ -14949,7 +14973,7 @@
         <v>9</v>
       </c>
       <c r="C217">
-        <f t="shared" ref="C217" si="343">SUM(D217:F217)</f>
+        <f t="shared" ref="C217" si="344">SUM(D217:F217)</f>
         <v>1673</v>
       </c>
       <c r="D217">
@@ -14965,7 +14989,7 @@
         <v>64</v>
       </c>
       <c r="H217" s="16">
-        <f>SUM(I217:K217)-SUM(L217:N217)</f>
+        <f t="shared" si="340"/>
         <v>5947</v>
       </c>
       <c r="I217" s="5">
@@ -14984,6 +15008,52 @@
         <v>86</v>
       </c>
       <c r="N217">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B218" s="2">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <f t="shared" ref="C218" si="345">SUM(D218:F218)</f>
+        <v>1673</v>
+      </c>
+      <c r="D218">
+        <v>1105</v>
+      </c>
+      <c r="E218">
+        <v>371</v>
+      </c>
+      <c r="F218" s="3">
+        <v>197</v>
+      </c>
+      <c r="G218" s="4">
+        <v>65</v>
+      </c>
+      <c r="H218" s="16">
+        <f t="shared" si="340"/>
+        <v>6052</v>
+      </c>
+      <c r="I218" s="5">
+        <v>6125</v>
+      </c>
+      <c r="J218" s="6">
+        <v>756</v>
+      </c>
+      <c r="K218" s="7">
+        <v>582</v>
+      </c>
+      <c r="L218">
+        <v>1305</v>
+      </c>
+      <c r="M218">
+        <v>86</v>
+      </c>
+      <c r="N218">
         <v>20</v>
       </c>
     </row>
@@ -15005,7 +15075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merge of two versions: ReleaseNotes.md and LineCount.xlsx
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E3259-BECF-2244-B201-EFF01284DFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177F5FC7-5AA4-EE40-9BC0-A99B5CDFDD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -915,6 +915,12 @@
                 <c:pt idx="215">
                   <c:v>45353</c:v>
                 </c:pt>
+                <c:pt idx="216">
+                  <c:v>45358</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>45359</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1571,6 +1577,12 @@
                 </c:pt>
                 <c:pt idx="215" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6052</c:v>
+                </c:pt>
+                <c:pt idx="216" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6158</c:v>
+                </c:pt>
+                <c:pt idx="217" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2266,6 +2278,12 @@
                 <c:pt idx="215">
                   <c:v>45353</c:v>
                 </c:pt>
+                <c:pt idx="216">
+                  <c:v>45358</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>45359</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2922,6 +2940,12 @@
                 </c:pt>
                 <c:pt idx="215">
                   <c:v>6125</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>6205</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>6212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3619,6 +3643,12 @@
                 <c:pt idx="215">
                   <c:v>45353</c:v>
                 </c:pt>
+                <c:pt idx="216">
+                  <c:v>45358</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>45359</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4275,6 +4305,12 @@
                 </c:pt>
                 <c:pt idx="215">
                   <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4991,6 +5027,12 @@
                 <c:pt idx="215">
                   <c:v>45353</c:v>
                 </c:pt>
+                <c:pt idx="216">
+                  <c:v>45358</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>45359</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5647,6 +5689,12 @@
                 </c:pt>
                 <c:pt idx="215">
                   <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5739,7 +5787,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6500"/>
+          <c:max val="7000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6875,13 +6923,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N218"/>
+  <dimension ref="A1:N220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I219" sqref="I219"/>
+      <selection pane="bottomRight" activeCell="I221" sqref="I221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15054,6 +15102,98 @@
         <v>86</v>
       </c>
       <c r="N218">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>45358</v>
+      </c>
+      <c r="B219" s="2">
+        <v>9</v>
+      </c>
+      <c r="C219">
+        <f t="shared" ref="C219" si="346">SUM(D219:F219)</f>
+        <v>1673</v>
+      </c>
+      <c r="D219">
+        <v>1105</v>
+      </c>
+      <c r="E219">
+        <v>371</v>
+      </c>
+      <c r="F219" s="3">
+        <v>197</v>
+      </c>
+      <c r="G219" s="4">
+        <v>66</v>
+      </c>
+      <c r="H219" s="16">
+        <f t="shared" ref="H219" si="347">SUM(I219:K219)-SUM(L219:N219)</f>
+        <v>6158</v>
+      </c>
+      <c r="I219" s="5">
+        <v>6205</v>
+      </c>
+      <c r="J219" s="6">
+        <v>770</v>
+      </c>
+      <c r="K219" s="7">
+        <v>594</v>
+      </c>
+      <c r="L219">
+        <v>1305</v>
+      </c>
+      <c r="M219">
+        <v>86</v>
+      </c>
+      <c r="N219">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B220" s="2">
+        <v>9</v>
+      </c>
+      <c r="C220">
+        <f t="shared" ref="C220" si="348">SUM(D220:F220)</f>
+        <v>1673</v>
+      </c>
+      <c r="D220">
+        <v>1105</v>
+      </c>
+      <c r="E220">
+        <v>371</v>
+      </c>
+      <c r="F220" s="3">
+        <v>197</v>
+      </c>
+      <c r="G220" s="4">
+        <v>66</v>
+      </c>
+      <c r="H220" s="16">
+        <f t="shared" ref="H220" si="349">SUM(I220:K220)-SUM(L220:N220)</f>
+        <v>6166</v>
+      </c>
+      <c r="I220" s="5">
+        <v>6212</v>
+      </c>
+      <c r="J220" s="6">
+        <v>769</v>
+      </c>
+      <c r="K220" s="7">
+        <v>596</v>
+      </c>
+      <c r="L220">
+        <v>1305</v>
+      </c>
+      <c r="M220">
+        <v>86</v>
+      </c>
+      <c r="N220">
         <v>20</v>
       </c>
     </row>
@@ -15076,7 +15216,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="AA48" sqref="AA48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added search bar to OrganizationView. Renamed to FilteredOrganizationView.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEAC678-4F4B-8F45-92A5-6D0A3BDA4F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B314DA-3E39-C248-940F-C5FAEC4D17EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -924,6 +924,9 @@
                 <c:pt idx="218">
                   <c:v>45369</c:v>
                 </c:pt>
+                <c:pt idx="219">
+                  <c:v>45379</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1589,6 +1592,9 @@
                 </c:pt>
                 <c:pt idx="218" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6192</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2293,6 +2299,9 @@
                 <c:pt idx="218">
                   <c:v>45369</c:v>
                 </c:pt>
+                <c:pt idx="219">
+                  <c:v>45379</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2958,6 +2967,9 @@
                 </c:pt>
                 <c:pt idx="218">
                   <c:v>6236</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>6278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3664,6 +3676,9 @@
                 <c:pt idx="218">
                   <c:v>45369</c:v>
                 </c:pt>
+                <c:pt idx="219">
+                  <c:v>45379</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4329,6 +4344,9 @@
                 </c:pt>
                 <c:pt idx="218">
                   <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5054,6 +5072,9 @@
                 <c:pt idx="218">
                   <c:v>45369</c:v>
                 </c:pt>
+                <c:pt idx="219">
+                  <c:v>45379</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5719,6 +5740,9 @@
                 </c:pt>
                 <c:pt idx="218">
                   <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6947,13 +6971,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N221"/>
+  <dimension ref="A1:N222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L221" sqref="L221"/>
+      <selection pane="bottomRight" activeCell="I222" sqref="I222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15264,6 +15288,52 @@
         <v>86</v>
       </c>
       <c r="N221">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>45379</v>
+      </c>
+      <c r="B222" s="2">
+        <v>9</v>
+      </c>
+      <c r="C222">
+        <f t="shared" ref="C222" si="352">SUM(D222:F222)</f>
+        <v>1673</v>
+      </c>
+      <c r="D222">
+        <v>1105</v>
+      </c>
+      <c r="E222">
+        <v>371</v>
+      </c>
+      <c r="F222" s="3">
+        <v>197</v>
+      </c>
+      <c r="G222" s="4">
+        <v>66</v>
+      </c>
+      <c r="H222" s="16">
+        <f t="shared" ref="H222" si="353">SUM(I222:K222)-SUM(L222:N222)</f>
+        <v>6230</v>
+      </c>
+      <c r="I222" s="5">
+        <v>6278</v>
+      </c>
+      <c r="J222" s="6">
+        <v>768</v>
+      </c>
+      <c r="K222" s="7">
+        <v>595</v>
+      </c>
+      <c r="L222">
+        <v>1305</v>
+      </c>
+      <c r="M222">
+        <v>86</v>
+      </c>
+      <c r="N222">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved 2 .pages files to Documentation directory
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7999C045-8CAF-3045-978C-104E7A65F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECDA06A-22AD-8F49-935A-B38B0778353B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1606,7 +1606,7 @@
                   <c:v>6257</c:v>
                 </c:pt>
                 <c:pt idx="221" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6293</c:v>
+                  <c:v>6296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2993,7 +2993,7 @@
                   <c:v>6293</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>6317</c:v>
+                  <c:v>6321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4382,7 +4382,7 @@
                   <c:v>774</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>781</c:v>
+                  <c:v>779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5790,7 +5790,7 @@
                   <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>606</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15456,16 +15456,16 @@
       </c>
       <c r="H224" s="16">
         <f t="shared" ref="H224" si="357">SUM(I224:K224)-SUM(L224:N224)</f>
-        <v>6293</v>
+        <v>6296</v>
       </c>
       <c r="I224" s="5">
-        <v>6317</v>
+        <v>6321</v>
       </c>
       <c r="J224" s="6">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="K224" s="7">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="L224">
         <v>1305</v>
@@ -15496,7 +15496,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Experimentation with smart scrolling on Who's Who page Border still left visible. Needs more work.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47207C28-92EC-784F-AAE5-0A5DDFEA82C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF6259D-3434-074B-B8C1-0CCE48CBCA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -936,6 +936,9 @@
                 <c:pt idx="222">
                   <c:v>45387</c:v>
                 </c:pt>
+                <c:pt idx="223">
+                  <c:v>45391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1613,6 +1616,9 @@
                 </c:pt>
                 <c:pt idx="222" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6323</c:v>
+                </c:pt>
+                <c:pt idx="223" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2329,6 +2335,9 @@
                 <c:pt idx="222">
                   <c:v>45387</c:v>
                 </c:pt>
+                <c:pt idx="223">
+                  <c:v>45391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3006,6 +3015,9 @@
                 </c:pt>
                 <c:pt idx="222">
                   <c:v>6401</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>6419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3724,6 +3736,9 @@
                 <c:pt idx="222">
                   <c:v>45387</c:v>
                 </c:pt>
+                <c:pt idx="223">
+                  <c:v>45391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4401,6 +4416,9 @@
                 </c:pt>
                 <c:pt idx="222">
                   <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5138,6 +5156,9 @@
                 <c:pt idx="222">
                   <c:v>45387</c:v>
                 </c:pt>
+                <c:pt idx="223">
+                  <c:v>45391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5815,6 +5836,9 @@
                 </c:pt>
                 <c:pt idx="222">
                   <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>604</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7043,13 +7067,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N225"/>
+  <dimension ref="A1:N226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I226" sqref="I226"/>
+      <selection pane="bottomRight" activeCell="I227" sqref="I227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15544,6 +15568,52 @@
         <v>86</v>
       </c>
       <c r="N225">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B226" s="2">
+        <v>9</v>
+      </c>
+      <c r="C226">
+        <f t="shared" ref="C226" si="360">SUM(D226:F226)</f>
+        <v>1673</v>
+      </c>
+      <c r="D226">
+        <v>1105</v>
+      </c>
+      <c r="E226">
+        <v>371</v>
+      </c>
+      <c r="F226" s="3">
+        <v>197</v>
+      </c>
+      <c r="G226" s="4">
+        <v>70</v>
+      </c>
+      <c r="H226" s="16">
+        <f t="shared" ref="H226" si="361">SUM(I226:K226)-SUM(L226:N226)</f>
+        <v>6387</v>
+      </c>
+      <c r="I226" s="5">
+        <v>6419</v>
+      </c>
+      <c r="J226" s="6">
+        <v>775</v>
+      </c>
+      <c r="K226" s="7">
+        <v>604</v>
+      </c>
+      <c r="L226">
+        <v>1305</v>
+      </c>
+      <c r="M226">
+        <v>86</v>
+      </c>
+      <c r="N226">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed enum2objectID dictiorary of type [OrganizationTypeEnum: NSManagedObjectID]
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0D2C1A-841D-DA4A-8329-F1E02462BA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD2336F-DBE3-EB4A-8F89-33FE42AFC56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -960,6 +960,9 @@
                 <c:pt idx="230">
                   <c:v>45438</c:v>
                 </c:pt>
+                <c:pt idx="231">
+                  <c:v>45444</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1661,6 +1664,9 @@
                 </c:pt>
                 <c:pt idx="230" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6394</c:v>
+                </c:pt>
+                <c:pt idx="231" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6369</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2401,6 +2407,9 @@
                 <c:pt idx="230">
                   <c:v>45438</c:v>
                 </c:pt>
+                <c:pt idx="231">
+                  <c:v>45444</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3102,6 +3111,9 @@
                 </c:pt>
                 <c:pt idx="230">
                   <c:v>6426</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>6332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3844,6 +3856,9 @@
                 <c:pt idx="230">
                   <c:v>45438</c:v>
                 </c:pt>
+                <c:pt idx="231">
+                  <c:v>45444</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4545,6 +4560,9 @@
                 </c:pt>
                 <c:pt idx="230">
                   <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>830</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5306,6 +5324,9 @@
                 <c:pt idx="230">
                   <c:v>45438</c:v>
                 </c:pt>
+                <c:pt idx="231">
+                  <c:v>45444</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6007,6 +6028,9 @@
                 </c:pt>
                 <c:pt idx="230">
                   <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7235,13 +7259,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N233"/>
+  <dimension ref="A1:N234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I234" sqref="I234"/>
+      <selection pane="bottomRight" activeCell="I235" sqref="I235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16104,6 +16128,52 @@
         <v>86</v>
       </c>
       <c r="N233">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>45444</v>
+      </c>
+      <c r="B234" s="2">
+        <v>9</v>
+      </c>
+      <c r="C234">
+        <f t="shared" ref="C234" si="376">SUM(D234:F234)</f>
+        <v>1673</v>
+      </c>
+      <c r="D234">
+        <v>1105</v>
+      </c>
+      <c r="E234">
+        <v>371</v>
+      </c>
+      <c r="F234" s="3">
+        <v>197</v>
+      </c>
+      <c r="G234" s="4">
+        <v>70</v>
+      </c>
+      <c r="H234" s="16">
+        <f t="shared" ref="H234" si="377">SUM(I234:K234)-SUM(L234:N234)</f>
+        <v>6369</v>
+      </c>
+      <c r="I234" s="5">
+        <v>6332</v>
+      </c>
+      <c r="J234" s="6">
+        <v>830</v>
+      </c>
+      <c r="K234" s="7">
+        <v>618</v>
+      </c>
+      <c r="L234">
+        <v>1305</v>
+      </c>
+      <c r="M234">
+        <v>86</v>
+      </c>
+      <c r="N234">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added empty data mode  (see PhotoClubHubApp.swift)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF446BB-9627-0A49-B577-60E15F741EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E27C75A-2385-C94D-B168-0FE29CAB5174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -969,6 +969,9 @@
                 <c:pt idx="233">
                   <c:v>45452</c:v>
                 </c:pt>
+                <c:pt idx="234">
+                  <c:v>45459</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1679,6 +1682,9 @@
                 </c:pt>
                 <c:pt idx="233" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6491</c:v>
+                </c:pt>
+                <c:pt idx="234" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2428,6 +2434,9 @@
                 <c:pt idx="233">
                   <c:v>45452</c:v>
                 </c:pt>
+                <c:pt idx="234">
+                  <c:v>45459</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3138,6 +3147,9 @@
                 </c:pt>
                 <c:pt idx="233">
                   <c:v>6424</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>6389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3889,6 +3901,9 @@
                 <c:pt idx="233">
                   <c:v>45452</c:v>
                 </c:pt>
+                <c:pt idx="234">
+                  <c:v>45459</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4599,6 +4614,9 @@
                 </c:pt>
                 <c:pt idx="233">
                   <c:v>844</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5369,6 +5387,9 @@
                 <c:pt idx="233">
                   <c:v>45452</c:v>
                 </c:pt>
+                <c:pt idx="234">
+                  <c:v>45459</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6079,6 +6100,9 @@
                 </c:pt>
                 <c:pt idx="233">
                   <c:v>634</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7307,13 +7331,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N236"/>
+  <dimension ref="A1:N237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I237" sqref="I237"/>
+      <selection pane="bottomRight" activeCell="I238" sqref="I238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16314,6 +16338,52 @@
         <v>86</v>
       </c>
       <c r="N236">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>45459</v>
+      </c>
+      <c r="B237" s="2">
+        <v>9</v>
+      </c>
+      <c r="C237">
+        <f t="shared" ref="C237" si="382">SUM(D237:F237)</f>
+        <v>1673</v>
+      </c>
+      <c r="D237">
+        <v>1105</v>
+      </c>
+      <c r="E237">
+        <v>371</v>
+      </c>
+      <c r="F237" s="3">
+        <v>197</v>
+      </c>
+      <c r="G237" s="4">
+        <v>70</v>
+      </c>
+      <c r="H237" s="16">
+        <f t="shared" ref="H237" si="383">SUM(I237:K237)-SUM(L237:N237)</f>
+        <v>6497</v>
+      </c>
+      <c r="I237" s="5">
+        <v>6389</v>
+      </c>
+      <c r="J237" s="6">
+        <v>892</v>
+      </c>
+      <c r="K237" s="7">
+        <v>627</v>
+      </c>
+      <c r="L237">
+        <v>1305</v>
+      </c>
+      <c r="M237">
+        <v>86</v>
+      </c>
+      <c r="N237">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Typo (organizationTypeEum > organizationTypeEnum)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A38EAD1-120E-354C-A7FB-3E821615FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC6546A-A092-8240-A7D1-9D4F1980470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -985,6 +985,9 @@
                   <c:v>45479</c:v>
                 </c:pt>
                 <c:pt idx="239">
+                  <c:v>45485</c:v>
+                </c:pt>
+                <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
               </c:numCache>
@@ -1715,6 +1718,9 @@
                 </c:pt>
                 <c:pt idx="239" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6667</c:v>
+                </c:pt>
+                <c:pt idx="240" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2480,6 +2486,9 @@
                   <c:v>45479</c:v>
                 </c:pt>
                 <c:pt idx="239">
+                  <c:v>45485</c:v>
+                </c:pt>
+                <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
               </c:numCache>
@@ -3210,6 +3219,9 @@
                 </c:pt>
                 <c:pt idx="239">
                   <c:v>6541</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>6670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3977,6 +3989,9 @@
                   <c:v>45479</c:v>
                 </c:pt>
                 <c:pt idx="239">
+                  <c:v>45485</c:v>
+                </c:pt>
+                <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
               </c:numCache>
@@ -4707,6 +4722,9 @@
                 </c:pt>
                 <c:pt idx="239">
                   <c:v>849</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>919</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5493,6 +5511,9 @@
                   <c:v>45479</c:v>
                 </c:pt>
                 <c:pt idx="239">
+                  <c:v>45485</c:v>
+                </c:pt>
+                <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
               </c:numCache>
@@ -6223,6 +6244,9 @@
                 </c:pt>
                 <c:pt idx="239">
                   <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7451,13 +7475,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N242"/>
+  <dimension ref="A1:N243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I243" sqref="I243"/>
+      <selection pane="bottomRight" activeCell="I244" sqref="I244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16693,7 +16717,7 @@
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>45486</v>
+        <v>45485</v>
       </c>
       <c r="B242" s="2">
         <v>9</v>
@@ -16734,6 +16758,52 @@
         <v>86</v>
       </c>
       <c r="N242">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>45486</v>
+      </c>
+      <c r="B243" s="2">
+        <v>9</v>
+      </c>
+      <c r="C243">
+        <f t="shared" ref="C243" si="394">SUM(D243:F243)</f>
+        <v>1673</v>
+      </c>
+      <c r="D243">
+        <v>1105</v>
+      </c>
+      <c r="E243">
+        <v>371</v>
+      </c>
+      <c r="F243" s="3">
+        <v>197</v>
+      </c>
+      <c r="G243" s="4">
+        <v>73</v>
+      </c>
+      <c r="H243" s="16">
+        <f t="shared" ref="H243" si="395">SUM(I243:K243)-SUM(L243:N243)</f>
+        <v>6894</v>
+      </c>
+      <c r="I243" s="5">
+        <v>6670</v>
+      </c>
+      <c r="J243" s="6">
+        <v>919</v>
+      </c>
+      <c r="K243" s="7">
+        <v>716</v>
+      </c>
+      <c r="L243">
+        <v>1305</v>
+      </c>
+      <c r="M243">
+        <v>86</v>
+      </c>
+      <c r="N243">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correctly loads `club` section of Level2.json file.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC6546A-A092-8240-A7D1-9D4F1980470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D039A8-12E6-9C46-9919-DE4A208C8162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -990,6 +990,9 @@
                 <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
+                <c:pt idx="241">
+                  <c:v>45487</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1721,6 +1724,9 @@
                 </c:pt>
                 <c:pt idx="240" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6894</c:v>
+                </c:pt>
+                <c:pt idx="241" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2491,6 +2497,9 @@
                 <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
+                <c:pt idx="241">
+                  <c:v>45487</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3222,6 +3231,9 @@
                 </c:pt>
                 <c:pt idx="240">
                   <c:v>6670</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>6649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3994,6 +4006,9 @@
                 <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
+                <c:pt idx="241">
+                  <c:v>45487</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4725,6 +4740,9 @@
                 </c:pt>
                 <c:pt idx="240">
                   <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5516,6 +5534,9 @@
                 <c:pt idx="240">
                   <c:v>45486</c:v>
                 </c:pt>
+                <c:pt idx="241">
+                  <c:v>45487</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6247,6 +6268,9 @@
                 </c:pt>
                 <c:pt idx="240">
                   <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7475,13 +7499,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N243"/>
+  <dimension ref="A1:N244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I244" sqref="I244"/>
+      <selection pane="bottomRight" activeCell="I245" sqref="I245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16804,6 +16828,52 @@
         <v>86</v>
       </c>
       <c r="N243">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>45487</v>
+      </c>
+      <c r="B244" s="2">
+        <v>9</v>
+      </c>
+      <c r="C244">
+        <f t="shared" ref="C244" si="396">SUM(D244:F244)</f>
+        <v>1673</v>
+      </c>
+      <c r="D244">
+        <v>1105</v>
+      </c>
+      <c r="E244">
+        <v>371</v>
+      </c>
+      <c r="F244" s="3">
+        <v>197</v>
+      </c>
+      <c r="G244" s="4">
+        <v>75</v>
+      </c>
+      <c r="H244" s="16">
+        <f t="shared" ref="H244" si="397">SUM(I244:K244)-SUM(L244:N244)</f>
+        <v>6901</v>
+      </c>
+      <c r="I244" s="5">
+        <v>6649</v>
+      </c>
+      <c r="J244" s="6">
+        <v>948</v>
+      </c>
+      <c r="K244" s="7">
+        <v>715</v>
+      </c>
+      <c r="L244">
+        <v>1305</v>
+      </c>
+      <c r="M244">
+        <v>86</v>
+      </c>
+      <c r="N244">
         <v>20</v>
       </c>
     </row>
@@ -16825,7 +16895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Date conversion and code to read birthdays in level2.json files
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3583B907-B649-6B4D-9F2A-C3F0E124DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F4AAA5-B721-7C43-A271-EE378E70BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -7549,11 +7549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:N246"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K246" sqref="K246"/>
+      <selection pane="bottomRight" activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16976,7 +16976,7 @@
         <v>45493</v>
       </c>
       <c r="B246" s="2">
-        <v>677</v>
+        <v>9</v>
       </c>
       <c r="C246">
         <f t="shared" ref="C246" si="400">SUM(D246:F246)</f>
@@ -16992,7 +16992,7 @@
         <v>197</v>
       </c>
       <c r="G246" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H246" s="16">
         <f t="shared" ref="H246" si="401">SUM(I246:K246)-SUM(L246:N246)</f>
@@ -17035,7 +17035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #416 Photographer.findCreateUpdate now only accepts a parameter isDeceased: Bool? instead of complete Role and Status dictionaries.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4F3A92-90B5-C44A-9E8B-2A37B65CD634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E68C2-E8DD-C54A-BD4A-76507E5F3F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1738,7 +1738,7 @@
                   <c:v>6970</c:v>
                 </c:pt>
                 <c:pt idx="243" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7079</c:v>
+                  <c:v>7076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3257,7 +3257,7 @@
                   <c:v>6750</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>6834</c:v>
+                  <c:v>6830</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6318,7 +6318,7 @@
                   <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>716</c:v>
+                  <c:v>717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7549,7 +7549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:N246"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -16996,16 +16996,16 @@
       </c>
       <c r="H246" s="16">
         <f t="shared" ref="H246" si="401">SUM(I246:K246)-SUM(L246:N246)</f>
-        <v>7079</v>
+        <v>7076</v>
       </c>
       <c r="I246" s="5">
-        <v>6834</v>
+        <v>6830</v>
       </c>
       <c r="J246" s="6">
         <v>940</v>
       </c>
       <c r="K246" s="7">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="L246">
         <v>1305</v>
@@ -17035,7 +17035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #418 Support for roles and status of members in Level2.json files
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E68C2-E8DD-C54A-BD4A-76507E5F3F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA54FD-3141-CF42-B165-363AC7290241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -999,6 +999,9 @@
                 <c:pt idx="243">
                   <c:v>45493</c:v>
                 </c:pt>
+                <c:pt idx="244">
+                  <c:v>45494</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1739,6 +1742,9 @@
                 </c:pt>
                 <c:pt idx="243" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7076</c:v>
+                </c:pt>
+                <c:pt idx="244" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2518,6 +2524,9 @@
                 <c:pt idx="243">
                   <c:v>45493</c:v>
                 </c:pt>
+                <c:pt idx="244">
+                  <c:v>45494</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3258,6 +3267,9 @@
                 </c:pt>
                 <c:pt idx="243">
                   <c:v>6830</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>6866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4039,6 +4051,9 @@
                 <c:pt idx="243">
                   <c:v>45493</c:v>
                 </c:pt>
+                <c:pt idx="244">
+                  <c:v>45494</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4779,6 +4794,9 @@
                 </c:pt>
                 <c:pt idx="243">
                   <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5579,6 +5597,9 @@
                 <c:pt idx="243">
                   <c:v>45493</c:v>
                 </c:pt>
+                <c:pt idx="244">
+                  <c:v>45494</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6319,6 +6340,9 @@
                 </c:pt>
                 <c:pt idx="243">
                   <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7547,19 +7571,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N246"/>
+  <dimension ref="A1:N247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I247" sqref="I247"/>
+      <selection pane="bottomRight" activeCell="E238" sqref="E238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="3"/>
     <col min="7" max="7" width="10.83203125" style="4"/>
     <col min="9" max="9" width="10.83203125" style="5"/>
@@ -17014,6 +17039,52 @@
         <v>86</v>
       </c>
       <c r="N246">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>45494</v>
+      </c>
+      <c r="B247" s="2">
+        <v>9</v>
+      </c>
+      <c r="C247">
+        <f t="shared" ref="C247" si="402">SUM(D247:F247)</f>
+        <v>1673</v>
+      </c>
+      <c r="D247">
+        <v>1105</v>
+      </c>
+      <c r="E247">
+        <v>371</v>
+      </c>
+      <c r="F247" s="3">
+        <v>197</v>
+      </c>
+      <c r="G247" s="4">
+        <v>76</v>
+      </c>
+      <c r="H247" s="16">
+        <f t="shared" ref="H247" si="403">SUM(I247:K247)-SUM(L247:N247)</f>
+        <v>7127</v>
+      </c>
+      <c r="I247" s="5">
+        <v>6866</v>
+      </c>
+      <c r="J247" s="6">
+        <v>947</v>
+      </c>
+      <c r="K247" s="7">
+        <v>725</v>
+      </c>
+      <c r="L247">
+        <v>1305</v>
+      </c>
+      <c r="M247">
+        <v>86</v>
+      </c>
+      <c r="N247">
         <v>20</v>
       </c>
     </row>
@@ -17035,8 +17106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA33" sqref="AA33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Missing comma in level2.json for fgAnders
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA54FD-3141-CF42-B165-363AC7290241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473CE463-7295-6749-8F93-8E5A1E03EC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1744,7 +1744,7 @@
                   <c:v>7076</c:v>
                 </c:pt>
                 <c:pt idx="244" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7127</c:v>
+                  <c:v>7177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3269,7 +3269,7 @@
                   <c:v>6830</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>6866</c:v>
+                  <c:v>6897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4796,7 +4796,7 @@
                   <c:v>940</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>947</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6342,7 +6342,7 @@
                   <c:v>717</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>725</c:v>
+                  <c:v>731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7577,7 +7577,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E238" sqref="E238"/>
+      <selection pane="bottomRight" activeCell="I248" sqref="I248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17067,16 +17067,16 @@
       </c>
       <c r="H247" s="16">
         <f t="shared" ref="H247" si="403">SUM(I247:K247)-SUM(L247:N247)</f>
-        <v>7127</v>
+        <v>7177</v>
       </c>
       <c r="I247" s="5">
-        <v>6866</v>
+        <v>6897</v>
       </c>
       <c r="J247" s="6">
-        <v>947</v>
+        <v>960</v>
       </c>
       <c r="K247" s="7">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="L247">
         <v>1305</v>

</xml_diff>

<commit_message>
Lot of changes related to creating structs to hold optional parameters for Members, Photographers and Organizations (Clubs). Created files to load Level2 code for clubs fcBellusImago and fgAnders. Renamed website fields in database to organizationWebsite, photographerWebsite, memberWebsite for clarity.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4403F2D-0240-3348-93C0-E63B756BF9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B00D42-090E-234A-89AF-7984C39455B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1762,7 +1762,7 @@
                   <c:v>7238</c:v>
                 </c:pt>
                 <c:pt idx="247" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7036</c:v>
+                  <c:v>6980</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3305,7 +3305,7 @@
                   <c:v>6934</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>6767</c:v>
+                  <c:v>6702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4850,7 +4850,7 @@
                   <c:v>978</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>964</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6414,7 +6414,7 @@
                   <c:v>737</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>716</c:v>
+                  <c:v>721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7649,7 +7649,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I251" sqref="I251"/>
+      <selection pane="bottomRight" activeCell="O250" sqref="O250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17277,16 +17277,16 @@
       </c>
       <c r="H250" s="16">
         <f t="shared" ref="H250" si="409">SUM(I250:K250)-SUM(L250:N250)</f>
-        <v>7036</v>
+        <v>6980</v>
       </c>
       <c r="I250" s="5">
-        <v>6767</v>
+        <v>6702</v>
       </c>
       <c r="J250" s="6">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="K250" s="7">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="L250">
         <v>1305</v>
@@ -17317,7 +17317,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA43" sqref="AA43"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed 3 featured images from fgDeGender.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA48E699-89CE-3640-B3E2-DFC6462CF86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACAA1E8-E903-BA42-82DC-FF7BE7810E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1017,6 +1017,9 @@
                 <c:pt idx="249">
                   <c:v>45506</c:v>
                 </c:pt>
+                <c:pt idx="250">
+                  <c:v>45508</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1775,6 +1778,9 @@
                 </c:pt>
                 <c:pt idx="249" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6970</c:v>
+                </c:pt>
+                <c:pt idx="250" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2572,6 +2578,9 @@
                 <c:pt idx="249">
                   <c:v>45506</c:v>
                 </c:pt>
+                <c:pt idx="250">
+                  <c:v>45508</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3330,6 +3339,9 @@
                 </c:pt>
                 <c:pt idx="249">
                   <c:v>6711</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>6761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4129,6 +4141,9 @@
                 <c:pt idx="249">
                   <c:v>45506</c:v>
                 </c:pt>
+                <c:pt idx="250">
+                  <c:v>45508</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4887,6 +4902,9 @@
                 </c:pt>
                 <c:pt idx="249">
                   <c:v>963</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>971</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5705,6 +5723,9 @@
                 <c:pt idx="249">
                   <c:v>45506</c:v>
                 </c:pt>
+                <c:pt idx="250">
+                  <c:v>45508</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6463,6 +6484,9 @@
                 </c:pt>
                 <c:pt idx="249">
                   <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7691,13 +7715,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N252"/>
+  <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R230" sqref="R230"/>
+      <selection pane="bottomRight" activeCell="G254" sqref="G254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17435,6 +17459,52 @@
         <v>86</v>
       </c>
       <c r="N252">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>45508</v>
+      </c>
+      <c r="B253" s="2">
+        <v>9</v>
+      </c>
+      <c r="C253">
+        <f t="shared" ref="C253" si="414">SUM(D253:F253)</f>
+        <v>1673</v>
+      </c>
+      <c r="D253">
+        <v>1105</v>
+      </c>
+      <c r="E253">
+        <v>371</v>
+      </c>
+      <c r="F253" s="3">
+        <v>197</v>
+      </c>
+      <c r="G253" s="4">
+        <v>79</v>
+      </c>
+      <c r="H253" s="16">
+        <f t="shared" ref="H253" si="415">SUM(I253:K253)-SUM(L253:N253)</f>
+        <v>7038</v>
+      </c>
+      <c r="I253" s="5">
+        <v>6761</v>
+      </c>
+      <c r="J253" s="6">
+        <v>971</v>
+      </c>
+      <c r="K253" s="7">
+        <v>717</v>
+      </c>
+      <c r="L253">
+        <v>1305</v>
+      </c>
+      <c r="M253">
+        <v>86</v>
+      </c>
+      <c r="N253">
         <v>20</v>
       </c>
     </row>
@@ -17456,7 +17526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preparations for releasing as 2.7.0 (4630)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACAA1E8-E903-BA42-82DC-FF7BE7810E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27DD33-5131-DD47-BBFB-80077025B106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1020,6 +1020,9 @@
                 <c:pt idx="250">
                   <c:v>45508</c:v>
                 </c:pt>
+                <c:pt idx="251">
+                  <c:v>45515</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1781,6 +1784,9 @@
                 </c:pt>
                 <c:pt idx="250" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7038</c:v>
+                </c:pt>
+                <c:pt idx="251" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2581,6 +2587,9 @@
                 <c:pt idx="250">
                   <c:v>45508</c:v>
                 </c:pt>
+                <c:pt idx="251">
+                  <c:v>45515</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3342,6 +3351,9 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>6761</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>6767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4144,6 +4156,9 @@
                 <c:pt idx="250">
                   <c:v>45508</c:v>
                 </c:pt>
+                <c:pt idx="251">
+                  <c:v>45515</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4904,6 +4919,9 @@
                   <c:v>963</c:v>
                 </c:pt>
                 <c:pt idx="250">
+                  <c:v>971</c:v>
+                </c:pt>
+                <c:pt idx="251">
                   <c:v>971</c:v>
                 </c:pt>
               </c:numCache>
@@ -5726,6 +5744,9 @@
                 <c:pt idx="250">
                   <c:v>45508</c:v>
                 </c:pt>
+                <c:pt idx="251">
+                  <c:v>45515</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6487,6 +6508,9 @@
                 </c:pt>
                 <c:pt idx="250">
                   <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7715,13 +7739,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N253"/>
+  <dimension ref="A1:N254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G254" sqref="G254"/>
+      <selection pane="bottomRight" activeCell="I255" sqref="I255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17505,6 +17529,52 @@
         <v>86</v>
       </c>
       <c r="N253">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>45515</v>
+      </c>
+      <c r="B254" s="2">
+        <v>9</v>
+      </c>
+      <c r="C254">
+        <f t="shared" ref="C254" si="416">SUM(D254:F254)</f>
+        <v>1673</v>
+      </c>
+      <c r="D254">
+        <v>1105</v>
+      </c>
+      <c r="E254">
+        <v>371</v>
+      </c>
+      <c r="F254" s="3">
+        <v>197</v>
+      </c>
+      <c r="G254" s="4">
+        <v>79</v>
+      </c>
+      <c r="H254" s="16">
+        <f t="shared" ref="H254" si="417">SUM(I254:K254)-SUM(L254:N254)</f>
+        <v>7046</v>
+      </c>
+      <c r="I254" s="5">
+        <v>6767</v>
+      </c>
+      <c r="J254" s="6">
+        <v>971</v>
+      </c>
+      <c r="K254" s="7">
+        <v>719</v>
+      </c>
+      <c r="L254">
+        <v>1305</v>
+      </c>
+      <c r="M254">
+        <v>86</v>
+      </c>
+      <c r="N254">
         <v>20</v>
       </c>
     </row>
@@ -17526,8 +17596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA52" sqref="AA52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Imported SwiftyJSON as a package. Was a file for a while because ofan Xxcode problem.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D15CA4-F842-834A-805C-4BBADC28E4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F688C1-243C-4B42-8C02-3844BBA7A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1026,6 +1026,9 @@
                 <c:pt idx="252">
                   <c:v>45521</c:v>
                 </c:pt>
+                <c:pt idx="253">
+                  <c:v>45522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1793,6 +1796,9 @@
                 </c:pt>
                 <c:pt idx="252" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7047</c:v>
+                </c:pt>
+                <c:pt idx="253" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2599,6 +2605,9 @@
                 <c:pt idx="252">
                   <c:v>45521</c:v>
                 </c:pt>
+                <c:pt idx="253">
+                  <c:v>45522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3366,6 +3375,9 @@
                 </c:pt>
                 <c:pt idx="252">
                   <c:v>6768</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>5467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4174,6 +4186,9 @@
                 <c:pt idx="252">
                   <c:v>45521</c:v>
                 </c:pt>
+                <c:pt idx="253">
+                  <c:v>45522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4941,6 +4956,9 @@
                 </c:pt>
                 <c:pt idx="252">
                   <c:v>971</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5768,6 +5786,9 @@
                 <c:pt idx="252">
                   <c:v>45521</c:v>
                 </c:pt>
+                <c:pt idx="253">
+                  <c:v>45522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6535,6 +6556,9 @@
                 </c:pt>
                 <c:pt idx="252">
                   <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7763,13 +7787,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N255"/>
+  <dimension ref="A1:N256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A256" sqref="A256"/>
+      <selection pane="bottomRight" activeCell="G257" sqref="G257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17646,6 +17670,52 @@
       </c>
       <c r="N255">
         <v>20</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>45522</v>
+      </c>
+      <c r="B256" s="2">
+        <v>9</v>
+      </c>
+      <c r="C256">
+        <f t="shared" ref="C256" si="420">SUM(D256:F256)</f>
+        <v>1673</v>
+      </c>
+      <c r="D256">
+        <v>1105</v>
+      </c>
+      <c r="E256">
+        <v>371</v>
+      </c>
+      <c r="F256" s="3">
+        <v>197</v>
+      </c>
+      <c r="G256" s="4">
+        <v>78</v>
+      </c>
+      <c r="H256" s="16">
+        <f t="shared" ref="H256" si="421">SUM(I256:K256)-SUM(L256:N256)</f>
+        <v>7052</v>
+      </c>
+      <c r="I256" s="5">
+        <v>5467</v>
+      </c>
+      <c r="J256" s="6">
+        <v>885</v>
+      </c>
+      <c r="K256" s="7">
+        <v>700</v>
+      </c>
+      <c r="L256">
+        <v>0</v>
+      </c>
+      <c r="M256">
+        <v>0</v>
+      </c>
+      <c r="N256">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Organization parameter when creating a new Photographer record. Photographer doesn't depend on Club, although the Club that triggered adding the Photographer was printed in the log file.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F688C1-243C-4B42-8C02-3844BBA7A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F955A48D-1EB0-BE45-9890-7CDE07356B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1029,6 +1029,9 @@
                 <c:pt idx="253">
                   <c:v>45522</c:v>
                 </c:pt>
+                <c:pt idx="254">
+                  <c:v>45571</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1799,6 +1802,9 @@
                 </c:pt>
                 <c:pt idx="253" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7052</c:v>
+                </c:pt>
+                <c:pt idx="254" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7060</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2608,6 +2614,9 @@
                 <c:pt idx="253">
                   <c:v>45522</c:v>
                 </c:pt>
+                <c:pt idx="254">
+                  <c:v>45571</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3378,6 +3387,9 @@
                 </c:pt>
                 <c:pt idx="253">
                   <c:v>5467</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>5475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4189,6 +4201,9 @@
                 <c:pt idx="253">
                   <c:v>45522</c:v>
                 </c:pt>
+                <c:pt idx="254">
+                  <c:v>45571</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4958,6 +4973,9 @@
                   <c:v>971</c:v>
                 </c:pt>
                 <c:pt idx="253">
+                  <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="254">
                   <c:v>885</c:v>
                 </c:pt>
               </c:numCache>
@@ -5789,6 +5807,9 @@
                 <c:pt idx="253">
                   <c:v>45522</c:v>
                 </c:pt>
+                <c:pt idx="254">
+                  <c:v>45571</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6558,6 +6579,9 @@
                   <c:v>719</c:v>
                 </c:pt>
                 <c:pt idx="253">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="254">
                   <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
@@ -6585,7 +6609,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45550"/>
+          <c:max val="45600"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7787,13 +7811,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N256"/>
+  <dimension ref="A1:N257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G257" sqref="G257"/>
+      <selection pane="bottomRight" activeCell="J258" sqref="J258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17715,6 +17739,52 @@
         <v>0</v>
       </c>
       <c r="N256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>45571</v>
+      </c>
+      <c r="B257" s="2">
+        <v>9</v>
+      </c>
+      <c r="C257">
+        <f t="shared" ref="C257" si="422">SUM(D257:F257)</f>
+        <v>1673</v>
+      </c>
+      <c r="D257">
+        <v>1105</v>
+      </c>
+      <c r="E257">
+        <v>371</v>
+      </c>
+      <c r="F257" s="3">
+        <v>197</v>
+      </c>
+      <c r="G257" s="4">
+        <v>78</v>
+      </c>
+      <c r="H257" s="16">
+        <f t="shared" ref="H257" si="423">SUM(I257:K257)-SUM(L257:N257)</f>
+        <v>7060</v>
+      </c>
+      <c r="I257" s="5">
+        <v>5475</v>
+      </c>
+      <c r="J257" s="6">
+        <v>885</v>
+      </c>
+      <c r="K257" s="7">
+        <v>700</v>
+      </c>
+      <c r="L257">
+        <v>0</v>
+      </c>
+      <c r="M257">
+        <v>0</v>
+      </c>
+      <c r="N257">
         <v>0</v>
       </c>
     </row>
@@ -17736,7 +17806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deleted FotogroepWaalreMembersProvider+insertSomeHardcodedMemberData.swift File was no longer in target, so removal mainly impacts Excel spreadsheet with lines of code.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F955A48D-1EB0-BE45-9890-7CDE07356B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A08AE6-5761-A042-AA14-BD36B62C2E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1032,6 +1032,9 @@
                 <c:pt idx="254">
                   <c:v>45571</c:v>
                 </c:pt>
+                <c:pt idx="255">
+                  <c:v>45586</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1805,6 +1808,9 @@
                 </c:pt>
                 <c:pt idx="254" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7060</c:v>
+                </c:pt>
+                <c:pt idx="255" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2617,6 +2623,9 @@
                 <c:pt idx="254">
                   <c:v>45571</c:v>
                 </c:pt>
+                <c:pt idx="255">
+                  <c:v>45586</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3390,6 +3399,9 @@
                 </c:pt>
                 <c:pt idx="254">
                   <c:v>5475</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>5376</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4204,6 +4216,9 @@
                 <c:pt idx="254">
                   <c:v>45571</c:v>
                 </c:pt>
+                <c:pt idx="255">
+                  <c:v>45586</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4977,6 +4992,9 @@
                 </c:pt>
                 <c:pt idx="254">
                   <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5810,6 +5828,9 @@
                 <c:pt idx="254">
                   <c:v>45571</c:v>
                 </c:pt>
+                <c:pt idx="255">
+                  <c:v>45586</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6583,6 +6604,9 @@
                 </c:pt>
                 <c:pt idx="254">
                   <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7811,13 +7835,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N257"/>
+  <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J258" sqref="J258"/>
+      <selection pane="bottomRight" activeCell="K259" sqref="K259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17785,6 +17809,52 @@
         <v>0</v>
       </c>
       <c r="N257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>45586</v>
+      </c>
+      <c r="B258" s="2">
+        <v>9</v>
+      </c>
+      <c r="C258">
+        <f t="shared" ref="C258" si="424">SUM(D258:F258)</f>
+        <v>1673</v>
+      </c>
+      <c r="D258">
+        <v>1105</v>
+      </c>
+      <c r="E258">
+        <v>371</v>
+      </c>
+      <c r="F258" s="3">
+        <v>197</v>
+      </c>
+      <c r="G258" s="4">
+        <v>77</v>
+      </c>
+      <c r="H258" s="16">
+        <f t="shared" ref="H258" si="425">SUM(I258:K258)-SUM(L258:N258)</f>
+        <v>6950</v>
+      </c>
+      <c r="I258" s="5">
+        <v>5376</v>
+      </c>
+      <c r="J258" s="6">
+        <v>878</v>
+      </c>
+      <c r="K258" s="7">
+        <v>696</v>
+      </c>
+      <c r="L258">
+        <v>0</v>
+      </c>
+      <c r="M258">
+        <v>0</v>
+      </c>
+      <c r="N258">
         <v>0</v>
       </c>
     </row>
@@ -17806,7 +17876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved club/museum coordinates out of `optionalFields` because it is not supposed to be optional in the input data. It can be missing technically, so when the file doesn't contain coordinates, we use (0,0) which in the Atlantic, west of Africa.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4971AE8C-526D-614C-88CF-5B90C7990BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2DC582-0AB1-E64B-9405-9E1B5E3669A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1828,7 +1828,7 @@
                   <c:v>6968</c:v>
                 </c:pt>
                 <c:pt idx="258" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6965</c:v>
+                  <c:v>6665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3437,7 +3437,7 @@
                   <c:v>5392</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>5388</c:v>
+                  <c:v>5169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5048,7 +5048,7 @@
                   <c:v>878</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>878</c:v>
+                  <c:v>817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6678,7 +6678,7 @@
                   <c:v>698</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>699</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18043,20 +18043,20 @@
         <v>197</v>
       </c>
       <c r="G261" s="4">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H261" s="16">
         <f t="shared" ref="H261" si="431">SUM(I261:K261)-SUM(L261:N261)</f>
-        <v>6965</v>
+        <v>6665</v>
       </c>
       <c r="I261" s="5">
-        <v>5388</v>
+        <v>5169</v>
       </c>
       <c r="J261" s="6">
-        <v>878</v>
+        <v>817</v>
       </c>
       <c r="K261" s="7">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="L261">
         <v>0</v>

</xml_diff>

<commit_message>
renamed isScrollLocked to isMapScrollLocked in data model
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45A064B-9D1F-924A-B643-18080DF776DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0389599-410A-4947-ACCC-C29735DCD8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1047,6 +1047,9 @@
                 <c:pt idx="259">
                   <c:v>45626</c:v>
                 </c:pt>
+                <c:pt idx="260">
+                  <c:v>45630</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1835,6 +1838,9 @@
                 </c:pt>
                 <c:pt idx="259" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6699</c:v>
+                </c:pt>
+                <c:pt idx="260" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2662,6 +2668,9 @@
                 <c:pt idx="259">
                   <c:v>45626</c:v>
                 </c:pt>
+                <c:pt idx="260">
+                  <c:v>45630</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3450,6 +3459,9 @@
                 </c:pt>
                 <c:pt idx="259">
                   <c:v>5188</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>5187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4279,6 +4291,9 @@
                 <c:pt idx="259">
                   <c:v>45626</c:v>
                 </c:pt>
+                <c:pt idx="260">
+                  <c:v>45630</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5067,6 +5082,9 @@
                 </c:pt>
                 <c:pt idx="259">
                   <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>822</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5915,6 +5933,9 @@
                 <c:pt idx="259">
                   <c:v>45626</c:v>
                 </c:pt>
+                <c:pt idx="260">
+                  <c:v>45630</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6703,6 +6724,9 @@
                 </c:pt>
                 <c:pt idx="259">
                   <c:v>683</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7931,13 +7955,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N262"/>
+  <dimension ref="A1:N263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P243" sqref="P243"/>
+      <selection pane="bottomRight" activeCell="I264" sqref="I264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18135,6 +18159,52 @@
         <v>0</v>
       </c>
       <c r="N262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B263" s="2">
+        <v>9</v>
+      </c>
+      <c r="C263">
+        <f t="shared" ref="C263" si="434">SUM(D263:F263)</f>
+        <v>1673</v>
+      </c>
+      <c r="D263">
+        <v>1105</v>
+      </c>
+      <c r="E263">
+        <v>371</v>
+      </c>
+      <c r="F263" s="3">
+        <v>197</v>
+      </c>
+      <c r="G263" s="4">
+        <v>75</v>
+      </c>
+      <c r="H263" s="16">
+        <f t="shared" ref="H263" si="435">SUM(I263:K263)-SUM(L263:N263)</f>
+        <v>6689</v>
+      </c>
+      <c r="I263" s="5">
+        <v>5187</v>
+      </c>
+      <c r="J263" s="6">
+        <v>822</v>
+      </c>
+      <c r="K263" s="7">
+        <v>680</v>
+      </c>
+      <c r="L263">
+        <v>0</v>
+      </c>
+      <c r="M263">
+        <v>0</v>
+      </c>
+      <c r="N263">
         <v>0</v>
       </c>
     </row>
@@ -18156,7 +18226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Removed last traces of support for loading/storing phone numbers and e-mail addresses (disabled in release 2.7.0)
Former-commit-id: 82488e87bedd92c017959db9fe7a87a1ffd41a54
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4A925A-D47D-2040-8229-9846B4773704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0EF7BA-752F-3343-BBCB-E04C3B71AFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1051,6 +1051,9 @@
                   <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="261">
+                  <c:v>45666</c:v>
+                </c:pt>
+                <c:pt idx="262">
                   <c:v>45667</c:v>
                 </c:pt>
               </c:numCache>
@@ -1847,6 +1850,9 @@
                 </c:pt>
                 <c:pt idx="261" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6390</c:v>
+                </c:pt>
+                <c:pt idx="262" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2678,6 +2684,9 @@
                   <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="261">
+                  <c:v>45666</c:v>
+                </c:pt>
+                <c:pt idx="262">
                   <c:v>45667</c:v>
                 </c:pt>
               </c:numCache>
@@ -3474,6 +3483,9 @@
                 </c:pt>
                 <c:pt idx="261">
                   <c:v>4980</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>4958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4307,6 +4319,9 @@
                   <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="261">
+                  <c:v>45666</c:v>
+                </c:pt>
+                <c:pt idx="262">
                   <c:v>45667</c:v>
                 </c:pt>
               </c:numCache>
@@ -5103,6 +5118,9 @@
                 </c:pt>
                 <c:pt idx="261">
                   <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5955,6 +5973,9 @@
                   <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="261">
+                  <c:v>45666</c:v>
+                </c:pt>
+                <c:pt idx="262">
                   <c:v>45667</c:v>
                 </c:pt>
               </c:numCache>
@@ -6751,6 +6772,9 @@
                 </c:pt>
                 <c:pt idx="261">
                   <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7979,13 +8003,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N264"/>
+  <dimension ref="A1:N265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I265" sqref="I265"/>
+      <selection pane="bottomRight" activeCell="I266" sqref="I266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18234,7 +18258,7 @@
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>45667</v>
+        <v>45666</v>
       </c>
       <c r="B264" s="2">
         <v>9</v>
@@ -18275,6 +18299,52 @@
         <v>0</v>
       </c>
       <c r="N264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B265" s="2">
+        <v>9</v>
+      </c>
+      <c r="C265">
+        <f t="shared" ref="C265" si="438">SUM(D265:F265)</f>
+        <v>1673</v>
+      </c>
+      <c r="D265">
+        <v>1105</v>
+      </c>
+      <c r="E265">
+        <v>371</v>
+      </c>
+      <c r="F265" s="3">
+        <v>197</v>
+      </c>
+      <c r="G265" s="4">
+        <v>70</v>
+      </c>
+      <c r="H265" s="16">
+        <f t="shared" ref="H265" si="439">SUM(I265:K265)-SUM(L265:N265)</f>
+        <v>6365</v>
+      </c>
+      <c r="I265" s="5">
+        <v>4958</v>
+      </c>
+      <c r="J265" s="6">
+        <v>765</v>
+      </c>
+      <c r="K265" s="7">
+        <v>642</v>
+      </c>
+      <c r="L265">
+        <v>0</v>
+      </c>
+      <c r="M265">
+        <v>0</v>
+      </c>
+      <c r="N265">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added xampleMin.level1.json, xampleMax.level1.json, xampleMin.level2.json, xampleMax.level2.json
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459163BE-1892-C34A-BB66-211FBAFE1B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB390267-B6A6-D145-87A5-B6019E9058FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1059,6 +1059,9 @@
                 <c:pt idx="263">
                   <c:v>45668</c:v>
                 </c:pt>
+                <c:pt idx="264">
+                  <c:v>45669</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1859,6 +1862,9 @@
                 </c:pt>
                 <c:pt idx="263" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6487</c:v>
+                </c:pt>
+                <c:pt idx="264" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2698,6 +2704,9 @@
                 <c:pt idx="263">
                   <c:v>45668</c:v>
                 </c:pt>
+                <c:pt idx="264">
+                  <c:v>45669</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3498,6 +3507,9 @@
                 </c:pt>
                 <c:pt idx="263">
                   <c:v>5024</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>4980</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4339,6 +4351,9 @@
                 <c:pt idx="263">
                   <c:v>45668</c:v>
                 </c:pt>
+                <c:pt idx="264">
+                  <c:v>45669</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5139,6 +5154,9 @@
                 </c:pt>
                 <c:pt idx="263">
                   <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5999,6 +6017,9 @@
                 <c:pt idx="263">
                   <c:v>45668</c:v>
                 </c:pt>
+                <c:pt idx="264">
+                  <c:v>45669</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6799,6 +6820,9 @@
                 </c:pt>
                 <c:pt idx="263">
                   <c:v>667</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8027,13 +8051,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N266"/>
+  <dimension ref="A1:N267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O238" sqref="O238"/>
+      <selection pane="bottomRight" activeCell="O267" sqref="O267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18415,6 +18439,52 @@
         <v>0</v>
       </c>
       <c r="N266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>45669</v>
+      </c>
+      <c r="B267" s="2">
+        <v>9</v>
+      </c>
+      <c r="C267">
+        <f t="shared" ref="C267" si="442">SUM(D267:F267)</f>
+        <v>1673</v>
+      </c>
+      <c r="D267">
+        <v>1105</v>
+      </c>
+      <c r="E267">
+        <v>371</v>
+      </c>
+      <c r="F267" s="3">
+        <v>197</v>
+      </c>
+      <c r="G267" s="4">
+        <v>70</v>
+      </c>
+      <c r="H267" s="16">
+        <f t="shared" ref="H267" si="443">SUM(I267:K267)-SUM(L267:N267)</f>
+        <v>6370</v>
+      </c>
+      <c r="I267" s="5">
+        <v>4980</v>
+      </c>
+      <c r="J267" s="6">
+        <v>726</v>
+      </c>
+      <c r="K267" s="7">
+        <v>664</v>
+      </c>
+      <c r="L267">
+        <v>0</v>
+      </c>
+      <c r="M267">
+        <v>0</v>
+      </c>
+      <c r="N267">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First version of Level2_aanmaken_NL.md
Former-commit-id: 68541cd6e3b09fe2aee39ff33a00075bbf7509eb
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB390267-B6A6-D145-87A5-B6019E9058FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD06014-6C17-DA4F-918D-C469C66976B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1062,6 +1062,9 @@
                 <c:pt idx="264">
                   <c:v>45669</c:v>
                 </c:pt>
+                <c:pt idx="265">
+                  <c:v>45674</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1864,6 +1867,9 @@
                   <c:v>6487</c:v>
                 </c:pt>
                 <c:pt idx="264" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6370</c:v>
+                </c:pt>
+                <c:pt idx="265" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6370</c:v>
                 </c:pt>
               </c:numCache>
@@ -2707,6 +2713,9 @@
                 <c:pt idx="264">
                   <c:v>45669</c:v>
                 </c:pt>
+                <c:pt idx="265">
+                  <c:v>45674</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3509,6 +3518,9 @@
                   <c:v>5024</c:v>
                 </c:pt>
                 <c:pt idx="264">
+                  <c:v>4980</c:v>
+                </c:pt>
+                <c:pt idx="265">
                   <c:v>4980</c:v>
                 </c:pt>
               </c:numCache>
@@ -4354,6 +4366,9 @@
                 <c:pt idx="264">
                   <c:v>45669</c:v>
                 </c:pt>
+                <c:pt idx="265">
+                  <c:v>45674</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5156,6 +5171,9 @@
                   <c:v>796</c:v>
                 </c:pt>
                 <c:pt idx="264">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="265">
                   <c:v>726</c:v>
                 </c:pt>
               </c:numCache>
@@ -6020,6 +6038,9 @@
                 <c:pt idx="264">
                   <c:v>45669</c:v>
                 </c:pt>
+                <c:pt idx="265">
+                  <c:v>45674</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6822,6 +6843,9 @@
                   <c:v>667</c:v>
                 </c:pt>
                 <c:pt idx="264">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="265">
                   <c:v>664</c:v>
                 </c:pt>
               </c:numCache>
@@ -8051,13 +8075,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N267"/>
+  <dimension ref="A1:N268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O267" sqref="O267"/>
+      <selection pane="bottomRight" activeCell="P268" sqref="P268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18485,6 +18509,52 @@
         <v>0</v>
       </c>
       <c r="N267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>45674</v>
+      </c>
+      <c r="B268" s="2">
+        <v>9</v>
+      </c>
+      <c r="C268">
+        <f t="shared" ref="C268" si="444">SUM(D268:F268)</f>
+        <v>1673</v>
+      </c>
+      <c r="D268">
+        <v>1105</v>
+      </c>
+      <c r="E268">
+        <v>371</v>
+      </c>
+      <c r="F268" s="3">
+        <v>197</v>
+      </c>
+      <c r="G268" s="4">
+        <v>70</v>
+      </c>
+      <c r="H268" s="16">
+        <f t="shared" ref="H268" si="445">SUM(I268:K268)-SUM(L268:N268)</f>
+        <v>6370</v>
+      </c>
+      <c r="I268" s="5">
+        <v>4980</v>
+      </c>
+      <c r="J268" s="6">
+        <v>726</v>
+      </c>
+      <c r="K268" s="7">
+        <v>664</v>
+      </c>
+      <c r="L268">
+        <v>0</v>
+      </c>
+      <c r="M268">
+        <v>0</v>
+      </c>
+      <c r="N268">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new file Model.swift To allow code to be reused by Photo Club Hub HTML
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC895FC0-275A-8148-9D49-BEDF63849AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D04B99-2513-444E-8B3C-15A61DAFF145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1074,6 +1074,9 @@
                 <c:pt idx="268">
                   <c:v>45697</c:v>
                 </c:pt>
+                <c:pt idx="269">
+                  <c:v>45702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1889,6 +1892,9 @@
                 </c:pt>
                 <c:pt idx="268" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6393</c:v>
+                </c:pt>
+                <c:pt idx="269" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2743,6 +2749,9 @@
                 <c:pt idx="268">
                   <c:v>45697</c:v>
                 </c:pt>
+                <c:pt idx="269">
+                  <c:v>45702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3558,6 +3567,9 @@
                 </c:pt>
                 <c:pt idx="268">
                   <c:v>5037</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>5069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4414,6 +4426,9 @@
                 <c:pt idx="268">
                   <c:v>45697</c:v>
                 </c:pt>
+                <c:pt idx="269">
+                  <c:v>45702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5229,6 +5244,9 @@
                 </c:pt>
                 <c:pt idx="268">
                   <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6104,6 +6122,9 @@
                 <c:pt idx="268">
                   <c:v>45697</c:v>
                 </c:pt>
+                <c:pt idx="269">
+                  <c:v>45702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6919,6 +6940,9 @@
                 </c:pt>
                 <c:pt idx="268">
                   <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8147,13 +8171,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N271"/>
+  <dimension ref="A1:N272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P272" sqref="P272"/>
+      <selection pane="bottomRight" activeCell="I273" sqref="I273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18765,6 +18789,52 @@
         <v>0</v>
       </c>
       <c r="N271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>45702</v>
+      </c>
+      <c r="B272" s="2">
+        <v>9</v>
+      </c>
+      <c r="C272">
+        <f t="shared" ref="C272" si="452">SUM(D272:F272)</f>
+        <v>1673</v>
+      </c>
+      <c r="D272">
+        <v>1105</v>
+      </c>
+      <c r="E272">
+        <v>371</v>
+      </c>
+      <c r="F272" s="3">
+        <v>197</v>
+      </c>
+      <c r="G272" s="4">
+        <v>70</v>
+      </c>
+      <c r="H272" s="16">
+        <f t="shared" ref="H272" si="453">SUM(I272:K272)-SUM(L272:N272)</f>
+        <v>6414</v>
+      </c>
+      <c r="I272" s="5">
+        <v>5069</v>
+      </c>
+      <c r="J272" s="6">
+        <v>696</v>
+      </c>
+      <c r="K272" s="7">
+        <v>649</v>
+      </c>
+      <c r="L272">
+        <v>0</v>
+      </c>
+      <c r="M272">
+        <v>0</v>
+      </c>
+      <c r="N272">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
better error handling when creating a new Language object
Former-commit-id: 3d85c9785349ff9651940cc738ab03faf353a2c9
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D550EB6-FC98-5648-8658-22BDC16FD969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790BFAF7-E754-0343-82C1-7DDA77466EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Code</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>SwiftyJSON file</t>
+  </si>
+  <si>
+    <t>UnitTests</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -174,6 +177,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1080,6 +1089,9 @@
                 <c:pt idx="270">
                   <c:v>45707</c:v>
                 </c:pt>
+                <c:pt idx="271">
+                  <c:v>45711</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1901,6 +1913,9 @@
                 </c:pt>
                 <c:pt idx="270" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6434</c:v>
+                </c:pt>
+                <c:pt idx="271" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2761,6 +2776,9 @@
                 <c:pt idx="270">
                   <c:v>45707</c:v>
                 </c:pt>
+                <c:pt idx="271">
+                  <c:v>45711</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3582,6 +3600,9 @@
                 </c:pt>
                 <c:pt idx="270">
                   <c:v>5073</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>5685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4444,6 +4465,9 @@
                 <c:pt idx="270">
                   <c:v>45707</c:v>
                 </c:pt>
+                <c:pt idx="271">
+                  <c:v>45711</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5265,6 +5289,9 @@
                 </c:pt>
                 <c:pt idx="270">
                   <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6146,6 +6173,9 @@
                 <c:pt idx="270">
                   <c:v>45707</c:v>
                 </c:pt>
+                <c:pt idx="271">
+                  <c:v>45711</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6967,6 +6997,9 @@
                 </c:pt>
                 <c:pt idx="270">
                   <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8195,13 +8228,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:N273"/>
+  <dimension ref="A1:Q274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B214" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P271" sqref="P271"/>
+      <selection pane="bottomRight" activeCell="O275" sqref="O275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8214,30 +8247,36 @@
     <col min="9" max="9" width="10.83203125" style="5"/>
     <col min="10" max="10" width="10.83203125" style="6"/>
     <col min="11" max="11" width="10.83203125" style="7"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:17" ht="26" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="17" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="17" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+    </row>
+    <row r="2" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -8281,7 +8320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44380</v>
       </c>
@@ -8318,7 +8357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>44381</v>
@@ -8356,7 +8395,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>44382</v>
@@ -8394,7 +8433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>44383</v>
@@ -8432,7 +8471,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A27" si="2">A6+1</f>
         <v>44384</v>
@@ -8470,7 +8509,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44387</v>
       </c>
@@ -8507,7 +8546,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44392</v>
       </c>
@@ -8544,7 +8583,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>44393</v>
@@ -8582,7 +8621,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>44394</v>
@@ -8620,7 +8659,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>44395</v>
@@ -8659,7 +8698,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>44396</v>
@@ -8698,7 +8737,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>44397</v>
@@ -8737,7 +8776,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>44398</v>
@@ -8776,7 +8815,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44400</v>
       </c>
@@ -18862,7 +18901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>45707</v>
       </c>
@@ -18906,6 +18945,55 @@
       </c>
       <c r="N273">
         <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>45711</v>
+      </c>
+      <c r="B274" s="2">
+        <v>9</v>
+      </c>
+      <c r="C274">
+        <f t="shared" ref="C274" si="456">SUM(D274:F274)</f>
+        <v>1673</v>
+      </c>
+      <c r="D274">
+        <v>1105</v>
+      </c>
+      <c r="E274">
+        <v>371</v>
+      </c>
+      <c r="F274" s="3">
+        <v>197</v>
+      </c>
+      <c r="G274" s="4">
+        <v>82</v>
+      </c>
+      <c r="H274" s="16">
+        <f t="shared" ref="H274" si="457">SUM(I274:K274)-SUM(L274:N274)</f>
+        <v>7196</v>
+      </c>
+      <c r="I274" s="5">
+        <v>5685</v>
+      </c>
+      <c r="J274" s="6">
+        <v>787</v>
+      </c>
+      <c r="K274" s="7">
+        <v>724</v>
+      </c>
+      <c r="L274">
+        <v>0</v>
+      </c>
+      <c r="M274">
+        <v>0</v>
+      </c>
+      <c r="N274">
+        <v>0</v>
+      </c>
+      <c r="O274">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created LocalizedKeyword.swift class extension
Former-commit-id: 135807086dd71ecc60f890b9f3241b55ff79327a
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6733D13-A598-1D40-8554-BDC32C02F3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9959C00D-14F7-0848-B5D7-D191163A5190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1092,6 +1092,9 @@
                 <c:pt idx="271">
                   <c:v>45711</c:v>
                 </c:pt>
+                <c:pt idx="272">
+                  <c:v>45712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1915,7 +1918,10 @@
                   <c:v>6434</c:v>
                 </c:pt>
                 <c:pt idx="271" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7303</c:v>
+                  <c:v>7377</c:v>
+                </c:pt>
+                <c:pt idx="272" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2779,6 +2785,9 @@
                 <c:pt idx="271">
                   <c:v>45711</c:v>
                 </c:pt>
+                <c:pt idx="272">
+                  <c:v>45712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3602,7 +3611,10 @@
                   <c:v>5073</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>5761</c:v>
+                  <c:v>5831</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>5862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4468,6 +4480,9 @@
                 <c:pt idx="271">
                   <c:v>45711</c:v>
                 </c:pt>
+                <c:pt idx="272">
+                  <c:v>45712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5291,7 +5306,10 @@
                   <c:v>708</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>802</c:v>
+                  <c:v>803</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6176,6 +6194,9 @@
                 <c:pt idx="271">
                   <c:v>45711</c:v>
                 </c:pt>
+                <c:pt idx="272">
+                  <c:v>45712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6999,7 +7020,10 @@
                   <c:v>653</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>740</c:v>
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>739</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8228,13 +8252,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q274"/>
+  <dimension ref="A1:Q275"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I275" sqref="I275"/>
+      <selection pane="bottomRight" activeCell="M287" sqref="M287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18972,16 +18996,16 @@
       </c>
       <c r="H274" s="16">
         <f t="shared" ref="H274" si="457">SUM(I274:K274)-SUM(L274:N274)</f>
-        <v>7303</v>
+        <v>7377</v>
       </c>
       <c r="I274" s="5">
-        <v>5761</v>
+        <v>5831</v>
       </c>
       <c r="J274" s="6">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="K274" s="7">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="L274">
         <v>0</v>
@@ -18993,7 +19017,56 @@
         <v>0</v>
       </c>
       <c r="O274">
-        <v>14</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>45712</v>
+      </c>
+      <c r="B275" s="2">
+        <v>9</v>
+      </c>
+      <c r="C275">
+        <f t="shared" ref="C275" si="458">SUM(D275:F275)</f>
+        <v>1673</v>
+      </c>
+      <c r="D275">
+        <v>1105</v>
+      </c>
+      <c r="E275">
+        <v>371</v>
+      </c>
+      <c r="F275" s="3">
+        <v>197</v>
+      </c>
+      <c r="G275" s="4">
+        <v>82</v>
+      </c>
+      <c r="H275" s="16">
+        <f t="shared" ref="H275" si="459">SUM(I275:K275)-SUM(L275:N275)</f>
+        <v>7405</v>
+      </c>
+      <c r="I275" s="5">
+        <v>5862</v>
+      </c>
+      <c r="J275" s="6">
+        <v>804</v>
+      </c>
+      <c r="K275" s="7">
+        <v>739</v>
+      </c>
+      <c r="L275">
+        <v>0</v>
+      </c>
+      <c r="M275">
+        <v>0</v>
+      </c>
+      <c r="N275">
+        <v>0</v>
+      </c>
+      <c r="O275">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for LocalizedKeyword.swift
Former-commit-id: d1301b3518b1d775654b2af54aac25dba97e4f2a
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9959C00D-14F7-0848-B5D7-D191163A5190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9E6B22-5692-0647-BDB1-B61F41AA34FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -8254,11 +8254,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q275"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M287" sqref="M287"/>
+      <selection pane="bottomRight" activeCell="R279" sqref="R279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19066,7 +19066,7 @@
         <v>0</v>
       </c>
       <c r="O275">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -19087,7 +19087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #500 Nothing to fix, just fixed a typo in a comment
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9E6B22-5692-0647-BDB1-B61F41AA34FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4FDE85-0B32-6540-AED0-546019AD1E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1095,6 +1095,9 @@
                 <c:pt idx="272">
                   <c:v>45712</c:v>
                 </c:pt>
+                <c:pt idx="273">
+                  <c:v>45714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1921,7 +1924,10 @@
                   <c:v>7377</c:v>
                 </c:pt>
                 <c:pt idx="272" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7405</c:v>
+                  <c:v>7467</c:v>
+                </c:pt>
+                <c:pt idx="273" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2788,6 +2794,9 @@
                 <c:pt idx="272">
                   <c:v>45712</c:v>
                 </c:pt>
+                <c:pt idx="273">
+                  <c:v>45714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3614,7 +3623,10 @@
                   <c:v>5831</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>5862</c:v>
+                  <c:v>5928</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>5928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4483,6 +4495,9 @@
                 <c:pt idx="272">
                   <c:v>45712</c:v>
                 </c:pt>
+                <c:pt idx="273">
+                  <c:v>45714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5309,7 +5324,10 @@
                   <c:v>803</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>804</c:v>
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6197,6 +6215,9 @@
                 <c:pt idx="272">
                   <c:v>45712</c:v>
                 </c:pt>
+                <c:pt idx="273">
+                  <c:v>45714</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7023,7 +7044,10 @@
                   <c:v>743</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>739</c:v>
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>737</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8252,13 +8276,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q275"/>
+  <dimension ref="A1:Q276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R279" sqref="R279"/>
+      <selection pane="bottomRight" activeCell="B276" sqref="A276:O276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19041,20 +19065,20 @@
         <v>197</v>
       </c>
       <c r="G275" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H275" s="16">
         <f t="shared" ref="H275" si="459">SUM(I275:K275)-SUM(L275:N275)</f>
-        <v>7405</v>
+        <v>7467</v>
       </c>
       <c r="I275" s="5">
-        <v>5862</v>
+        <v>5928</v>
       </c>
       <c r="J275" s="6">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="K275" s="7">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="L275">
         <v>0</v>
@@ -19066,6 +19090,55 @@
         <v>0</v>
       </c>
       <c r="O275">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>45714</v>
+      </c>
+      <c r="B276" s="2">
+        <v>9</v>
+      </c>
+      <c r="C276">
+        <f t="shared" ref="C276" si="460">SUM(D276:F276)</f>
+        <v>1673</v>
+      </c>
+      <c r="D276">
+        <v>1105</v>
+      </c>
+      <c r="E276">
+        <v>371</v>
+      </c>
+      <c r="F276" s="3">
+        <v>197</v>
+      </c>
+      <c r="G276" s="4">
+        <v>83</v>
+      </c>
+      <c r="H276" s="16">
+        <f t="shared" ref="H276" si="461">SUM(I276:K276)-SUM(L276:N276)</f>
+        <v>7467</v>
+      </c>
+      <c r="I276" s="5">
+        <v>5928</v>
+      </c>
+      <c r="J276" s="6">
+        <v>802</v>
+      </c>
+      <c r="K276" s="7">
+        <v>737</v>
+      </c>
+      <c r="L276">
+        <v>0</v>
+      </c>
+      <c r="M276">
+        <v>0</v>
+      </c>
+      <c r="N276">
+        <v>0</v>
+      </c>
+      <c r="O276">
         <v>12</v>
       </c>
     </row>
@@ -19087,7 +19160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed Keyword.findCreateUpdate(context: id: isStandard) isStandard is not allowed to be nil to indicate that the value shouldn't change.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DFB4FD-8371-B045-9B42-BD7B0622E4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77630A94-FEE6-3540-97CD-42003B591F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1110,6 +1110,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1943,6 +1946,9 @@
                 </c:pt>
                 <c:pt idx="274" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7773</c:v>
+                </c:pt>
+                <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2815,6 +2821,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3648,6 +3657,9 @@
                 </c:pt>
                 <c:pt idx="274">
                   <c:v>6195</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>6200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4522,6 +4534,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5354,6 +5369,9 @@
                   <c:v>814</c:v>
                 </c:pt>
                 <c:pt idx="274">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="275">
                   <c:v>814</c:v>
                 </c:pt>
               </c:numCache>
@@ -6248,6 +6266,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7081,6 +7102,9 @@
                 </c:pt>
                 <c:pt idx="274">
                   <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8304,6 +8328,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9136,6 +9163,9 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="274">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="275">
                   <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
@@ -10009,6 +10039,9 @@
                 <c:pt idx="274">
                   <c:v>45717</c:v>
                 </c:pt>
+                <c:pt idx="275">
+                  <c:v>45718</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10841,6 +10874,9 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="274">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="275">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -12669,13 +12705,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q277"/>
+  <dimension ref="A1:Q278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I274" sqref="I274"/>
+      <selection pane="bottomRight" activeCell="I279" sqref="I279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24400,6 +24436,55 @@
         <v>14</v>
       </c>
     </row>
+    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>45718</v>
+      </c>
+      <c r="B278" s="2">
+        <v>9</v>
+      </c>
+      <c r="C278">
+        <f t="shared" ref="C278" si="464">SUM(D278:F278)</f>
+        <v>1673</v>
+      </c>
+      <c r="D278">
+        <v>1105</v>
+      </c>
+      <c r="E278">
+        <v>371</v>
+      </c>
+      <c r="F278" s="3">
+        <v>197</v>
+      </c>
+      <c r="G278" s="4">
+        <v>84</v>
+      </c>
+      <c r="H278" s="16">
+        <f t="shared" ref="H278" si="465">SUM(I278:K278)-SUM(L278:N278)</f>
+        <v>7777</v>
+      </c>
+      <c r="I278" s="5">
+        <v>6200</v>
+      </c>
+      <c r="J278" s="6">
+        <v>814</v>
+      </c>
+      <c r="K278" s="7">
+        <v>763</v>
+      </c>
+      <c r="L278">
+        <v>0</v>
+      </c>
+      <c r="M278">
+        <v>0</v>
+      </c>
+      <c r="N278">
+        <v>0</v>
+      </c>
+      <c r="O278">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -24418,7 +24503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First attempt to include keywords in PhotographerOptionalFields and store it via PhotographerKeyword.findCreateUpdate
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77630A94-FEE6-3540-97CD-42003B591F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9A0C02-D4E2-BB4E-9C7B-4497FBDF37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1948,7 +1948,7 @@
                   <c:v>7773</c:v>
                 </c:pt>
                 <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7777</c:v>
+                  <c:v>7781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3659,7 +3659,7 @@
                   <c:v>6195</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>6200</c:v>
+                  <c:v>6204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24461,10 +24461,10 @@
       </c>
       <c r="H278" s="16">
         <f t="shared" ref="H278" si="465">SUM(I278:K278)-SUM(L278:N278)</f>
-        <v>7777</v>
+        <v>7781</v>
       </c>
       <c r="I278" s="5">
-        <v>6200</v>
+        <v>6204</v>
       </c>
       <c r="J278" s="6">
         <v>814</v>
@@ -24504,7 +24504,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added temporary statistics about keywords near footer of Who's Who screen (for software testing) Fix: #504
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9A0C02-D4E2-BB4E-9C7B-4497FBDF37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7506A60C-6D4C-4E46-8817-43107D9E7086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1113,6 +1113,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1949,6 +1952,9 @@
                 </c:pt>
                 <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7781</c:v>
+                </c:pt>
+                <c:pt idx="276" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2824,6 +2830,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3660,6 +3669,9 @@
                 </c:pt>
                 <c:pt idx="275">
                   <c:v>6204</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>6320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4537,6 +4549,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5373,6 +5388,9 @@
                 </c:pt>
                 <c:pt idx="275">
                   <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6269,6 +6287,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7105,6 +7126,9 @@
                 </c:pt>
                 <c:pt idx="275">
                   <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8331,6 +8355,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9166,6 +9193,9 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="275">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="276">
                   <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
@@ -10042,6 +10072,9 @@
                 <c:pt idx="275">
                   <c:v>45718</c:v>
                 </c:pt>
+                <c:pt idx="276">
+                  <c:v>45721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10877,6 +10910,9 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="275">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="276">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -12705,13 +12741,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q278"/>
+  <dimension ref="A1:Q279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I279" sqref="I279"/>
+      <selection pane="bottomRight" activeCell="I280" sqref="I280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24482,6 +24518,55 @@
         <v>0</v>
       </c>
       <c r="O278">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>45721</v>
+      </c>
+      <c r="B279" s="2">
+        <v>9</v>
+      </c>
+      <c r="C279">
+        <f t="shared" ref="C279" si="466">SUM(D279:F279)</f>
+        <v>1673</v>
+      </c>
+      <c r="D279">
+        <v>1105</v>
+      </c>
+      <c r="E279">
+        <v>371</v>
+      </c>
+      <c r="F279" s="3">
+        <v>197</v>
+      </c>
+      <c r="G279" s="4">
+        <v>84</v>
+      </c>
+      <c r="H279" s="16">
+        <f t="shared" ref="H279" si="467">SUM(I279:K279)-SUM(L279:N279)</f>
+        <v>7904</v>
+      </c>
+      <c r="I279" s="5">
+        <v>6320</v>
+      </c>
+      <c r="J279" s="6">
+        <v>817</v>
+      </c>
+      <c r="K279" s="7">
+        <v>767</v>
+      </c>
+      <c r="L279">
+        <v>0</v>
+      </c>
+      <c r="M279">
+        <v>0</v>
+      </c>
+      <c r="N279">
+        <v>0</v>
+      </c>
+      <c r="O279">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First real test, but not about keywords yet.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7506A60C-6D4C-4E46-8817-43107D9E7086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E8A3EA-4889-894B-A6B8-CF6929050F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="2" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1954,7 +1954,7 @@
                   <c:v>7781</c:v>
                 </c:pt>
                 <c:pt idx="276" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7904</c:v>
+                  <c:v>7956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3671,7 +3671,7 @@
                   <c:v>6204</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>6320</c:v>
+                  <c:v>6351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5390,7 +5390,7 @@
                   <c:v>814</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>817</c:v>
+                  <c:v>828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7128,7 +7128,7 @@
                   <c:v>763</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>767</c:v>
+                  <c:v>777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9196,7 +9196,7 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>84</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10913,7 +10913,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12747,7 +12747,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I280" sqref="I280"/>
+      <selection pane="bottomRight" activeCell="G280" sqref="G280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24542,20 +24542,20 @@
         <v>197</v>
       </c>
       <c r="G279" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H279" s="16">
         <f t="shared" ref="H279" si="467">SUM(I279:K279)-SUM(L279:N279)</f>
-        <v>7904</v>
+        <v>7956</v>
       </c>
       <c r="I279" s="5">
-        <v>6320</v>
+        <v>6351</v>
       </c>
       <c r="J279" s="6">
-        <v>817</v>
+        <v>828</v>
       </c>
       <c r="K279" s="7">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="L279">
         <v>0</v>
@@ -24567,7 +24567,7 @@
         <v>0</v>
       </c>
       <c r="O279">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -24588,7 +24588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -24603,7 +24603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01361E9F-285B-9946-B1BF-3886CBEE5CAD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AF65" sqref="AF65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Directory struct cleanup Removed directories containing just one file (for loading a photo club) and moved files to parent directory..
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7A068-6266-FC45-B20A-B02D7B4C29BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEED66E8-43EA-AA4B-BA4B-42AA43CDCC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="2" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1119,6 +1119,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1961,6 +1964,9 @@
                 </c:pt>
                 <c:pt idx="277" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>7934</c:v>
+                </c:pt>
+                <c:pt idx="278" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>7990</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,6 +2848,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3684,6 +3693,9 @@
                 </c:pt>
                 <c:pt idx="277">
                   <c:v>6336</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>6375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4567,6 +4579,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5409,6 +5424,9 @@
                 </c:pt>
                 <c:pt idx="277">
                   <c:v>816</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6311,6 +6329,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7153,6 +7174,9 @@
                 </c:pt>
                 <c:pt idx="277">
                   <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7245,7 +7269,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8000"/>
+          <c:max val="8500"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8385,6 +8409,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9226,6 +9253,9 @@
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="277">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="278">
                   <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
@@ -10108,6 +10138,9 @@
                 <c:pt idx="277">
                   <c:v>45724</c:v>
                 </c:pt>
+                <c:pt idx="278">
+                  <c:v>45725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10950,6 +10983,9 @@
                 </c:pt>
                 <c:pt idx="277">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12777,13 +12813,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q280"/>
+  <dimension ref="A1:Q281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A280" sqref="A280"/>
+      <selection pane="bottomRight" activeCell="O282" sqref="O282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24653,6 +24689,55 @@
       </c>
       <c r="O280">
         <v>15</v>
+      </c>
+    </row>
+    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>45725</v>
+      </c>
+      <c r="B281" s="2">
+        <v>9</v>
+      </c>
+      <c r="C281">
+        <f t="shared" ref="C281" si="470">SUM(D281:F281)</f>
+        <v>1673</v>
+      </c>
+      <c r="D281">
+        <v>1105</v>
+      </c>
+      <c r="E281">
+        <v>371</v>
+      </c>
+      <c r="F281" s="3">
+        <v>197</v>
+      </c>
+      <c r="G281" s="4">
+        <v>83</v>
+      </c>
+      <c r="H281" s="16">
+        <f t="shared" ref="H281" si="471">SUM(I281:K281)-SUM(L281:N281)</f>
+        <v>7990</v>
+      </c>
+      <c r="I281" s="5">
+        <v>6375</v>
+      </c>
+      <c r="J281" s="6">
+        <v>823</v>
+      </c>
+      <c r="K281" s="7">
+        <v>792</v>
+      </c>
+      <c r="L281">
+        <v>0</v>
+      </c>
+      <c r="M281">
+        <v>0</v>
+      </c>
+      <c r="N281">
+        <v>0</v>
+      </c>
+      <c r="O281">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -24674,7 +24759,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24688,7 +24773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01361E9F-285B-9946-B1BF-3886CBEE5CAD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AF65" sqref="AF65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
3 working tests and TODO items fixed
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F518988-BE80-A845-9E7C-0831C617627E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBE71CC-E769-2D4F-8DA4-64DF89A77B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1122,6 +1122,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1967,6 +1970,9 @@
                 </c:pt>
                 <c:pt idx="278" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8037</c:v>
+                </c:pt>
+                <c:pt idx="279" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2851,6 +2857,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3696,6 +3705,9 @@
                 </c:pt>
                 <c:pt idx="278">
                   <c:v>6406</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>6455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4582,6 +4594,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5427,6 +5442,9 @@
                 </c:pt>
                 <c:pt idx="278">
                   <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6332,6 +6350,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7177,6 +7198,9 @@
                 </c:pt>
                 <c:pt idx="278">
                   <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>805</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8412,6 +8436,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9256,6 +9283,9 @@
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="278">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="279">
                   <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
@@ -10141,6 +10171,9 @@
                 <c:pt idx="278">
                   <c:v>45725</c:v>
                 </c:pt>
+                <c:pt idx="279">
+                  <c:v>45728</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10985,6 +11018,9 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="278">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="279">
                   <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
@@ -12813,13 +12849,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q281"/>
+  <dimension ref="A1:Q282"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I282" sqref="I282"/>
+      <selection pane="bottomRight" activeCell="M292" sqref="M292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24740,6 +24776,55 @@
         <v>17</v>
       </c>
     </row>
+    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>45728</v>
+      </c>
+      <c r="B282" s="2">
+        <v>9</v>
+      </c>
+      <c r="C282">
+        <f t="shared" ref="C282" si="472">SUM(D282:F282)</f>
+        <v>1673</v>
+      </c>
+      <c r="D282">
+        <v>1105</v>
+      </c>
+      <c r="E282">
+        <v>371</v>
+      </c>
+      <c r="F282" s="3">
+        <v>197</v>
+      </c>
+      <c r="G282" s="4">
+        <v>83</v>
+      </c>
+      <c r="H282" s="16">
+        <f t="shared" ref="H282" si="473">SUM(I282:K282)-SUM(L282:N282)</f>
+        <v>8084</v>
+      </c>
+      <c r="I282" s="5">
+        <v>6455</v>
+      </c>
+      <c r="J282" s="6">
+        <v>824</v>
+      </c>
+      <c r="K282" s="7">
+        <v>805</v>
+      </c>
+      <c r="L282">
+        <v>0</v>
+      </c>
+      <c r="M282">
+        <v>0</v>
+      </c>
+      <c r="N282">
+        <v>0</v>
+      </c>
+      <c r="O282">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -24758,7 +24843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 4th test to Level2JsonReaderTest It reads keywords for member PvdH from one club and independent keywords for same member from another club. The database should end up containing the union of both sets.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBE71CC-E769-2D4F-8DA4-64DF89A77B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC408C-801E-3C4C-911B-217EA59B5ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1972,7 +1972,7 @@
                   <c:v>8037</c:v>
                 </c:pt>
                 <c:pt idx="279" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8084</c:v>
+                  <c:v>8106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3707,7 +3707,7 @@
                   <c:v>6406</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>6455</c:v>
+                  <c:v>6467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5444,7 +5444,7 @@
                   <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>824</c:v>
+                  <c:v>834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12851,11 +12851,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M292" sqref="M292"/>
+      <selection pane="bottomRight" activeCell="I283" sqref="I283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24801,13 +24801,13 @@
       </c>
       <c r="H282" s="16">
         <f t="shared" ref="H282" si="473">SUM(I282:K282)-SUM(L282:N282)</f>
-        <v>8084</v>
+        <v>8106</v>
       </c>
       <c r="I282" s="5">
-        <v>6455</v>
+        <v>6467</v>
       </c>
       <c r="J282" s="6">
-        <v>824</v>
+        <v>834</v>
       </c>
       <c r="K282" s="7">
         <v>805</v>
@@ -24843,7 +24843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor refactoring of club loaders.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC408C-801E-3C4C-911B-217EA59B5ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC6A32F-4BAC-2749-A58F-A4A7B965C45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="2" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1972,7 +1972,7 @@
                   <c:v>8037</c:v>
                 </c:pt>
                 <c:pt idx="279" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8106</c:v>
+                  <c:v>8107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3707,7 +3707,7 @@
                   <c:v>6406</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>6467</c:v>
+                  <c:v>6472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5444,7 +5444,7 @@
                   <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>834</c:v>
+                  <c:v>826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7200,7 +7200,7 @@
                   <c:v>801</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>805</c:v>
+                  <c:v>809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9318,11 +9318,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFDCDD"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -11021,7 +11024,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12855,7 +12858,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I283" sqref="I283"/>
+      <selection pane="bottomRight" activeCell="O283" sqref="O283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24801,16 +24804,16 @@
       </c>
       <c r="H282" s="16">
         <f t="shared" ref="H282" si="473">SUM(I282:K282)-SUM(L282:N282)</f>
-        <v>8106</v>
+        <v>8107</v>
       </c>
       <c r="I282" s="5">
-        <v>6467</v>
+        <v>6472</v>
       </c>
       <c r="J282" s="6">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="K282" s="7">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="L282">
         <v>0</v>
@@ -24822,7 +24825,7 @@
         <v>0</v>
       </c>
       <c r="O282">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -24843,7 +24846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -24858,7 +24861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01361E9F-285B-9946-B1BF-3886CBEE5CAD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AF65" sqref="AF65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Line count Lost and recovered a few data points.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE62D86-B1BC-D942-B60D-41404F7C7FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193CC459-5508-C44F-9A3A-ACFFCD9B9EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1131,6 +1131,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1985,6 +1994,15 @@
                 </c:pt>
                 <c:pt idx="281" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8345</c:v>
+                </c:pt>
+                <c:pt idx="282" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8453</c:v>
+                </c:pt>
+                <c:pt idx="283" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8499</c:v>
+                </c:pt>
+                <c:pt idx="284" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8569</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2878,6 +2896,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3732,6 +3759,15 @@
                 </c:pt>
                 <c:pt idx="281">
                   <c:v>6677</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>6755</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>6809</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>6865</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4627,6 +4663,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5481,6 +5526,15 @@
                 </c:pt>
                 <c:pt idx="281">
                   <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>849</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6395,6 +6449,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7249,6 +7312,15 @@
                 </c:pt>
                 <c:pt idx="281">
                   <c:v>826</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>849</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7341,7 +7413,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8500"/>
+          <c:max val="9000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8493,6 +8565,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9346,6 +9427,15 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="281">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="284">
                   <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
@@ -10243,6 +10333,15 @@
                 <c:pt idx="281">
                   <c:v>45730</c:v>
                 </c:pt>
+                <c:pt idx="282">
+                  <c:v>45738</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45739</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11097,6 +11196,15 @@
                 </c:pt>
                 <c:pt idx="281">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12924,13 +13032,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q284"/>
+  <dimension ref="A1:Q287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I284" sqref="I284"/>
+      <selection pane="bottomRight" activeCell="A288" sqref="A288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24996,6 +25104,153 @@
       </c>
       <c r="O284">
         <v>20</v>
+      </c>
+    </row>
+    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>45738</v>
+      </c>
+      <c r="B285" s="2">
+        <v>9</v>
+      </c>
+      <c r="C285">
+        <f t="shared" ref="C285:C286" si="478">SUM(D285:F285)</f>
+        <v>1673</v>
+      </c>
+      <c r="D285">
+        <v>1105</v>
+      </c>
+      <c r="E285">
+        <v>371</v>
+      </c>
+      <c r="F285" s="3">
+        <v>197</v>
+      </c>
+      <c r="G285" s="4">
+        <v>84</v>
+      </c>
+      <c r="H285" s="16">
+        <f t="shared" ref="H285:H286" si="479">SUM(I285:K285)-SUM(L285:N285)</f>
+        <v>8453</v>
+      </c>
+      <c r="I285" s="5">
+        <v>6755</v>
+      </c>
+      <c r="J285" s="6">
+        <v>849</v>
+      </c>
+      <c r="K285" s="7">
+        <v>849</v>
+      </c>
+      <c r="L285">
+        <v>0</v>
+      </c>
+      <c r="M285">
+        <v>0</v>
+      </c>
+      <c r="N285">
+        <v>0</v>
+      </c>
+      <c r="O285">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>45739</v>
+      </c>
+      <c r="B286" s="2">
+        <v>9</v>
+      </c>
+      <c r="C286">
+        <f t="shared" si="478"/>
+        <v>1673</v>
+      </c>
+      <c r="D286">
+        <v>1105</v>
+      </c>
+      <c r="E286">
+        <v>371</v>
+      </c>
+      <c r="F286" s="3">
+        <v>197</v>
+      </c>
+      <c r="G286" s="4">
+        <v>84</v>
+      </c>
+      <c r="H286" s="16">
+        <f t="shared" si="479"/>
+        <v>8499</v>
+      </c>
+      <c r="I286" s="5">
+        <v>6809</v>
+      </c>
+      <c r="J286" s="6">
+        <v>845</v>
+      </c>
+      <c r="K286" s="7">
+        <v>845</v>
+      </c>
+      <c r="L286">
+        <v>0</v>
+      </c>
+      <c r="M286">
+        <v>0</v>
+      </c>
+      <c r="N286">
+        <v>0</v>
+      </c>
+      <c r="O286">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>45740</v>
+      </c>
+      <c r="B287" s="2">
+        <v>9</v>
+      </c>
+      <c r="C287">
+        <f t="shared" ref="C287" si="480">SUM(D287:F287)</f>
+        <v>1673</v>
+      </c>
+      <c r="D287">
+        <v>1105</v>
+      </c>
+      <c r="E287">
+        <v>371</v>
+      </c>
+      <c r="F287" s="3">
+        <v>197</v>
+      </c>
+      <c r="G287" s="4">
+        <v>84</v>
+      </c>
+      <c r="H287" s="16">
+        <f t="shared" ref="H287" si="481">SUM(I287:K287)-SUM(L287:N287)</f>
+        <v>8569</v>
+      </c>
+      <c r="I287" s="5">
+        <v>6865</v>
+      </c>
+      <c r="J287" s="6">
+        <v>853</v>
+      </c>
+      <c r="K287" s="7">
+        <v>851</v>
+      </c>
+      <c r="L287">
+        <v>0</v>
+      </c>
+      <c r="M287">
+        <v>0</v>
+      </c>
+      <c r="N287">
+        <v>0</v>
+      </c>
+      <c r="O287">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated keyword stats at bottom of Photographers screen
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193CC459-5508-C44F-9A3A-ACFFCD9B9EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A963580-2D8E-8946-BB5A-55511843D186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1140,6 +1140,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2003,6 +2006,9 @@
                 </c:pt>
                 <c:pt idx="284" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8569</c:v>
+                </c:pt>
+                <c:pt idx="285" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2905,6 +2911,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3768,6 +3777,9 @@
                 </c:pt>
                 <c:pt idx="284">
                   <c:v>6865</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>6848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4672,6 +4684,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5535,6 +5550,9 @@
                 </c:pt>
                 <c:pt idx="284">
                   <c:v>853</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6458,6 +6476,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7321,6 +7342,9 @@
                 </c:pt>
                 <c:pt idx="284">
                   <c:v>851</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8574,6 +8598,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9437,6 +9464,9 @@
                 </c:pt>
                 <c:pt idx="284">
                   <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10342,6 +10372,9 @@
                 <c:pt idx="284">
                   <c:v>45740</c:v>
                 </c:pt>
+                <c:pt idx="285">
+                  <c:v>45746</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11204,6 +11237,9 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="284">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="285">
                   <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
@@ -13032,13 +13068,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q287"/>
+  <dimension ref="A1:Q288"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A288" sqref="A288"/>
+      <selection pane="bottomRight" activeCell="G289" sqref="G289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25253,6 +25289,55 @@
         <v>22</v>
       </c>
     </row>
+    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>45746</v>
+      </c>
+      <c r="B288" s="2">
+        <v>9</v>
+      </c>
+      <c r="C288">
+        <f t="shared" ref="C288" si="482">SUM(D288:F288)</f>
+        <v>1673</v>
+      </c>
+      <c r="D288">
+        <v>1105</v>
+      </c>
+      <c r="E288">
+        <v>371</v>
+      </c>
+      <c r="F288" s="3">
+        <v>197</v>
+      </c>
+      <c r="G288" s="4">
+        <v>85</v>
+      </c>
+      <c r="H288" s="16">
+        <f t="shared" ref="H288" si="483">SUM(I288:K288)-SUM(L288:N288)</f>
+        <v>8559</v>
+      </c>
+      <c r="I288" s="5">
+        <v>6848</v>
+      </c>
+      <c r="J288" s="6">
+        <v>855</v>
+      </c>
+      <c r="K288" s="7">
+        <v>856</v>
+      </c>
+      <c r="L288">
+        <v>0</v>
+      </c>
+      <c r="M288">
+        <v>0</v>
+      </c>
+      <c r="N288">
+        <v>0</v>
+      </c>
+      <c r="O288">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -25271,7 +25356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test using languages.level0.json
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420556F2-E2CF-E347-8B54-27FFABC8E48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0BDDF5-30CF-6648-9720-1CB9170B8486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1146,6 +1146,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2015,6 +2018,9 @@
                 </c:pt>
                 <c:pt idx="286" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8561</c:v>
+                </c:pt>
+                <c:pt idx="287" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8080</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2923,6 +2929,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3792,6 +3801,9 @@
                 </c:pt>
                 <c:pt idx="286">
                   <c:v>6850</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>6442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4702,6 +4714,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5571,6 +5586,9 @@
                 </c:pt>
                 <c:pt idx="286">
                   <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6500,6 +6518,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7369,6 +7390,9 @@
                 </c:pt>
                 <c:pt idx="286">
                   <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8628,6 +8652,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9497,6 +9524,9 @@
                 </c:pt>
                 <c:pt idx="286">
                   <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10408,6 +10438,9 @@
                 <c:pt idx="286">
                   <c:v>45748</c:v>
                 </c:pt>
+                <c:pt idx="287">
+                  <c:v>45754</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11277,6 +11310,9 @@
                 </c:pt>
                 <c:pt idx="286">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13104,13 +13140,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q289"/>
+  <dimension ref="A1:Q290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K289" sqref="K289"/>
+      <selection pane="bottomRight" activeCell="I291" sqref="I291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25421,6 +25457,55 @@
       </c>
       <c r="O289">
         <v>22</v>
+      </c>
+    </row>
+    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>45754</v>
+      </c>
+      <c r="B290" s="2">
+        <v>9</v>
+      </c>
+      <c r="C290">
+        <f t="shared" ref="C290" si="486">SUM(D290:F290)</f>
+        <v>1673</v>
+      </c>
+      <c r="D290">
+        <v>1105</v>
+      </c>
+      <c r="E290">
+        <v>371</v>
+      </c>
+      <c r="F290" s="3">
+        <v>197</v>
+      </c>
+      <c r="G290" s="4">
+        <v>80</v>
+      </c>
+      <c r="H290" s="16">
+        <f t="shared" ref="H290" si="487">SUM(I290:K290)-SUM(L290:N290)</f>
+        <v>8080</v>
+      </c>
+      <c r="I290" s="5">
+        <v>6442</v>
+      </c>
+      <c r="J290" s="6">
+        <v>809</v>
+      </c>
+      <c r="K290" s="7">
+        <v>829</v>
+      </c>
+      <c r="L290">
+        <v>0</v>
+      </c>
+      <c r="M290">
+        <v>0</v>
+      </c>
+      <c r="N290">
+        <v>0</v>
+      </c>
+      <c r="O290">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added keywords related fetch function
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0BDDF5-30CF-6648-9720-1CB9170B8486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38BED2-45B1-FA42-8BCA-A2A0C7BE492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1149,6 +1149,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2021,6 +2024,9 @@
                 </c:pt>
                 <c:pt idx="287" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8080</c:v>
+                </c:pt>
+                <c:pt idx="288" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2932,6 +2938,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3804,6 +3813,9 @@
                 </c:pt>
                 <c:pt idx="287">
                   <c:v>6442</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>6491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4717,6 +4729,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5588,6 +5603,9 @@
                   <c:v>855</c:v>
                 </c:pt>
                 <c:pt idx="287">
+                  <c:v>809</c:v>
+                </c:pt>
+                <c:pt idx="288">
                   <c:v>809</c:v>
                 </c:pt>
               </c:numCache>
@@ -6521,6 +6539,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7392,6 +7413,9 @@
                   <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="287">
+                  <c:v>829</c:v>
+                </c:pt>
+                <c:pt idx="288">
                   <c:v>829</c:v>
                 </c:pt>
               </c:numCache>
@@ -8655,6 +8679,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9526,6 +9553,9 @@
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="287">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="288">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -10441,6 +10471,9 @@
                 <c:pt idx="287">
                   <c:v>45754</c:v>
                 </c:pt>
+                <c:pt idx="288">
+                  <c:v>45766</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11312,6 +11345,9 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="287">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="288">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13140,13 +13176,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q290"/>
+  <dimension ref="A1:Q291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I291" sqref="I291"/>
+      <selection pane="bottomRight" activeCell="A292" sqref="A292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25505,6 +25541,55 @@
         <v>0</v>
       </c>
       <c r="O290">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>45766</v>
+      </c>
+      <c r="B291" s="2">
+        <v>9</v>
+      </c>
+      <c r="C291">
+        <f t="shared" ref="C291" si="488">SUM(D291:F291)</f>
+        <v>1673</v>
+      </c>
+      <c r="D291">
+        <v>1105</v>
+      </c>
+      <c r="E291">
+        <v>371</v>
+      </c>
+      <c r="F291" s="3">
+        <v>197</v>
+      </c>
+      <c r="G291" s="4">
+        <v>80</v>
+      </c>
+      <c r="H291" s="16">
+        <f t="shared" ref="H291" si="489">SUM(I291:K291)-SUM(L291:N291)</f>
+        <v>8129</v>
+      </c>
+      <c r="I291" s="5">
+        <v>6491</v>
+      </c>
+      <c r="J291" s="6">
+        <v>809</v>
+      </c>
+      <c r="K291" s="7">
+        <v>829</v>
+      </c>
+      <c r="L291">
+        <v>0</v>
+      </c>
+      <c r="M291">
+        <v>0</v>
+      </c>
+      <c r="N291">
+        <v>0</v>
+      </c>
+      <c r="O291">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated footnotes of Who's Who screen. Keyword -> Expertise related.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFE277A-2630-2C40-8A49-A5CEC7FB9446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D1BC20-B81F-9D46-8572-1FA2CAAC6EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1158,6 +1158,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2039,6 +2042,9 @@
                 </c:pt>
                 <c:pt idx="290" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8269</c:v>
+                </c:pt>
+                <c:pt idx="291" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2959,6 +2965,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3840,6 +3849,9 @@
                 </c:pt>
                 <c:pt idx="290">
                   <c:v>6564</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>6894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4762,6 +4774,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5643,6 +5658,9 @@
                 </c:pt>
                 <c:pt idx="290">
                   <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6584,6 +6602,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7465,6 +7486,9 @@
                 </c:pt>
                 <c:pt idx="290">
                   <c:v>863</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8736,6 +8760,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9617,6 +9644,9 @@
                 </c:pt>
                 <c:pt idx="290">
                   <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10540,6 +10570,9 @@
                 <c:pt idx="290">
                   <c:v>45810</c:v>
                 </c:pt>
+                <c:pt idx="291">
+                  <c:v>45811</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11420,6 +11453,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="290">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="291">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13248,13 +13284,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q293"/>
+  <dimension ref="A1:Q294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O293" sqref="O293"/>
+      <selection pane="bottomRight" activeCell="G294" sqref="G294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25763,6 +25799,55 @@
         <v>23</v>
       </c>
     </row>
+    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B294" s="2">
+        <v>9</v>
+      </c>
+      <c r="C294">
+        <f t="shared" ref="C294" si="494">SUM(D294:F294)</f>
+        <v>1673</v>
+      </c>
+      <c r="D294">
+        <v>1105</v>
+      </c>
+      <c r="E294">
+        <v>371</v>
+      </c>
+      <c r="F294" s="3">
+        <v>197</v>
+      </c>
+      <c r="G294" s="4">
+        <v>86</v>
+      </c>
+      <c r="H294" s="16">
+        <f t="shared" ref="H294" si="495">SUM(I294:K294)-SUM(L294:N294)</f>
+        <v>8646</v>
+      </c>
+      <c r="I294" s="5">
+        <v>6894</v>
+      </c>
+      <c r="J294" s="6">
+        <v>862</v>
+      </c>
+      <c r="K294" s="7">
+        <v>890</v>
+      </c>
+      <c r="L294">
+        <v>0</v>
+      </c>
+      <c r="M294">
+        <v>0</v>
+      </c>
+      <c r="N294">
+        <v>0</v>
+      </c>
+      <c r="O294">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -25781,7 +25866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #544 Sorting of Expertise list Sorting should be on local language.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D1BC20-B81F-9D46-8572-1FA2CAAC6EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6FFEC-6E2E-AA48-8888-3220EAA5176F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1161,6 +1161,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2045,6 +2048,9 @@
                 </c:pt>
                 <c:pt idx="291" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8646</c:v>
+                </c:pt>
+                <c:pt idx="292" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2968,6 +2974,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3852,6 +3861,9 @@
                 </c:pt>
                 <c:pt idx="291">
                   <c:v>6894</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>6904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4777,6 +4789,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5660,6 +5675,9 @@
                   <c:v>842</c:v>
                 </c:pt>
                 <c:pt idx="291">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="292">
                   <c:v>862</c:v>
                 </c:pt>
               </c:numCache>
@@ -6605,6 +6623,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7489,6 +7510,9 @@
                 </c:pt>
                 <c:pt idx="291">
                   <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8763,6 +8787,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9646,6 +9673,9 @@
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="291">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="292">
                   <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
@@ -10573,6 +10603,9 @@
                 <c:pt idx="291">
                   <c:v>45811</c:v>
                 </c:pt>
+                <c:pt idx="292">
+                  <c:v>45812</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11456,6 +11489,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="291">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="292">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13284,13 +13320,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q294"/>
+  <dimension ref="A1:Q295"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G294" sqref="G294"/>
+      <selection pane="bottomRight" activeCell="R291" sqref="R291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25848,6 +25884,55 @@
         <v>23</v>
       </c>
     </row>
+    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>45812</v>
+      </c>
+      <c r="B295" s="2">
+        <v>9</v>
+      </c>
+      <c r="C295">
+        <f t="shared" ref="C295" si="496">SUM(D295:F295)</f>
+        <v>1673</v>
+      </c>
+      <c r="D295">
+        <v>1105</v>
+      </c>
+      <c r="E295">
+        <v>371</v>
+      </c>
+      <c r="F295" s="3">
+        <v>197</v>
+      </c>
+      <c r="G295" s="4">
+        <v>86</v>
+      </c>
+      <c r="H295" s="16">
+        <f t="shared" ref="H295" si="497">SUM(I295:K295)-SUM(L295:N295)</f>
+        <v>8658</v>
+      </c>
+      <c r="I295" s="5">
+        <v>6904</v>
+      </c>
+      <c r="J295" s="6">
+        <v>862</v>
+      </c>
+      <c r="K295" s="7">
+        <v>892</v>
+      </c>
+      <c r="L295">
+        <v>0</v>
+      </c>
+      <c r="M295">
+        <v>0</v>
+      </c>
+      <c r="N295">
+        <v>0</v>
+      </c>
+      <c r="O295">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -25866,7 +25951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Synchronized changes from Photo Club Hub HTML Many but not all.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6FFEC-6E2E-AA48-8888-3220EAA5176F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3891FF14-59E0-2046-B988-C1537AE18468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -2050,7 +2050,7 @@
                   <c:v>8646</c:v>
                 </c:pt>
                 <c:pt idx="292" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8658</c:v>
+                  <c:v>8310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3863,7 +3863,7 @@
                   <c:v>6894</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>6904</c:v>
+                  <c:v>6541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5678,7 +5678,7 @@
                   <c:v>862</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>862</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7512,7 +7512,7 @@
                   <c:v>890</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>892</c:v>
+                  <c:v>913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13322,11 +13322,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R291" sqref="R291"/>
+      <selection pane="bottomRight" activeCell="I296" sqref="I296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25909,16 +25909,16 @@
       </c>
       <c r="H295" s="16">
         <f t="shared" ref="H295" si="497">SUM(I295:K295)-SUM(L295:N295)</f>
-        <v>8658</v>
+        <v>8310</v>
       </c>
       <c r="I295" s="5">
-        <v>6904</v>
+        <v>6541</v>
       </c>
       <c r="J295" s="6">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="K295" s="7">
-        <v>892</v>
+        <v>913</v>
       </c>
       <c r="L295">
         <v>0</v>
@@ -25951,7 +25951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #554 (put expertises on one line in UI)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1565D2C4-C9B7-2F46-A8C8-10A9072A949D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E3AE9C-32A6-0F46-87FE-A37BF45D6DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -2056,7 +2056,7 @@
                   <c:v>8324</c:v>
                 </c:pt>
                 <c:pt idx="293" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8415</c:v>
+                  <c:v>8437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3875,7 +3875,7 @@
                   <c:v>6555</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>6623</c:v>
+                  <c:v>6645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5696,7 +5696,7 @@
                   <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>867</c:v>
+                  <c:v>868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7536,7 +7536,7 @@
                   <c:v>913</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>925</c:v>
+                  <c:v>924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13362,7 +13362,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G296" sqref="G296"/>
+      <selection pane="bottomRight" activeCell="I297" sqref="I297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25994,16 +25994,16 @@
       </c>
       <c r="H296" s="16">
         <f t="shared" ref="H296" si="499">SUM(I296:K296)-SUM(L296:N296)</f>
-        <v>8415</v>
+        <v>8437</v>
       </c>
       <c r="I296" s="5">
-        <v>6623</v>
+        <v>6645</v>
       </c>
       <c r="J296" s="6">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="K296" s="7">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L296">
         <v>0</v>

</xml_diff>

<commit_message>
Added support for fgDenDungen
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F1F46A-1EB5-3B48-8240-982BE8C25724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627FE831-2010-0942-B282-EBDA22BE64D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1170,6 +1170,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2063,6 +2066,9 @@
                 </c:pt>
                 <c:pt idx="294" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8462</c:v>
+                </c:pt>
+                <c:pt idx="295" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2995,6 +3001,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3888,6 +3897,9 @@
                 </c:pt>
                 <c:pt idx="294">
                   <c:v>6664</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>6711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4822,6 +4834,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5715,6 +5730,9 @@
                 </c:pt>
                 <c:pt idx="294">
                   <c:v>869</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6668,6 +6686,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7561,6 +7582,9 @@
                 </c:pt>
                 <c:pt idx="294">
                   <c:v>929</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8844,6 +8868,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9737,6 +9764,9 @@
                 </c:pt>
                 <c:pt idx="294">
                   <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10672,6 +10702,9 @@
                 <c:pt idx="294">
                   <c:v>45818</c:v>
                 </c:pt>
+                <c:pt idx="295">
+                  <c:v>45822</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11564,6 +11597,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="294">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="295">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13392,13 +13428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q297"/>
+  <dimension ref="A1:Q298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I298" sqref="I298"/>
+      <selection pane="bottomRight" activeCell="G299" sqref="G299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26100,6 +26136,55 @@
         <v>0</v>
       </c>
       <c r="O297">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>45822</v>
+      </c>
+      <c r="B298" s="2">
+        <v>9</v>
+      </c>
+      <c r="C298">
+        <f t="shared" ref="C298" si="502">SUM(D298:F298)</f>
+        <v>1673</v>
+      </c>
+      <c r="D298">
+        <v>1105</v>
+      </c>
+      <c r="E298">
+        <v>371</v>
+      </c>
+      <c r="F298" s="3">
+        <v>197</v>
+      </c>
+      <c r="G298" s="4">
+        <v>87</v>
+      </c>
+      <c r="H298" s="16">
+        <f t="shared" ref="H298" si="503">SUM(I298:K298)-SUM(L298:N298)</f>
+        <v>8531</v>
+      </c>
+      <c r="I298" s="5">
+        <v>6711</v>
+      </c>
+      <c r="J298" s="6">
+        <v>879</v>
+      </c>
+      <c r="K298" s="7">
+        <v>941</v>
+      </c>
+      <c r="L298">
+        <v>0</v>
+      </c>
+      <c r="M298">
+        <v>0</v>
+      </c>
+      <c r="N298">
+        <v>0</v>
+      </c>
+      <c r="O298">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed Keyword>Expertise in json files and in some remaining places in the code
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ED3FED-A87A-B243-AE56-9BCE05F0946C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74256B-9B63-7A4F-AD07-D9D51E7A3CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1176,6 +1176,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2075,6 +2078,9 @@
                 </c:pt>
                 <c:pt idx="296" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8537</c:v>
+                </c:pt>
+                <c:pt idx="297" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3013,6 +3019,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3912,6 +3921,9 @@
                 </c:pt>
                 <c:pt idx="296">
                   <c:v>6708</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>6718</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4852,6 +4864,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5751,6 +5766,9 @@
                 </c:pt>
                 <c:pt idx="296">
                   <c:v>883</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6710,6 +6728,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7609,6 +7630,9 @@
                 </c:pt>
                 <c:pt idx="296">
                   <c:v>946</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8898,6 +8922,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9796,6 +9823,9 @@
                   <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="296">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="297">
                   <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
@@ -10738,6 +10768,9 @@
                 <c:pt idx="296">
                   <c:v>45823</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>45832</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11636,6 +11669,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="296">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="297">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13464,13 +13500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q299"/>
+  <dimension ref="A1:Q300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G300" sqref="G300"/>
+      <selection pane="bottomRight" activeCell="I301" sqref="I301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26273,6 +26309,55 @@
         <v>23</v>
       </c>
     </row>
+    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>45832</v>
+      </c>
+      <c r="B300" s="2">
+        <v>9</v>
+      </c>
+      <c r="C300">
+        <f t="shared" ref="C300" si="506">SUM(D300:F300)</f>
+        <v>1673</v>
+      </c>
+      <c r="D300">
+        <v>1105</v>
+      </c>
+      <c r="E300">
+        <v>371</v>
+      </c>
+      <c r="F300" s="3">
+        <v>197</v>
+      </c>
+      <c r="G300" s="4">
+        <v>88</v>
+      </c>
+      <c r="H300" s="16">
+        <f t="shared" ref="H300" si="507">SUM(I300:K300)-SUM(L300:N300)</f>
+        <v>8550</v>
+      </c>
+      <c r="I300" s="5">
+        <v>6718</v>
+      </c>
+      <c r="J300" s="6">
+        <v>884</v>
+      </c>
+      <c r="K300" s="7">
+        <v>948</v>
+      </c>
+      <c r="L300">
+        <v>0</v>
+      </c>
+      <c r="M300">
+        <v>0</v>
+      </c>
+      <c r="N300">
+        <v>0</v>
+      </c>
+      <c r="O300">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -26291,7 +26376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #560 wrong image if FeaturedImage missing from Level2 record
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74256B-9B63-7A4F-AD07-D9D51E7A3CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB68583-EC81-0B4C-A4FE-AC2C6846EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1177,6 +1177,9 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
+                  <c:v>45831</c:v>
+                </c:pt>
+                <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
               </c:numCache>
@@ -2081,6 +2084,9 @@
                 </c:pt>
                 <c:pt idx="297" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8550</c:v>
+                </c:pt>
+                <c:pt idx="298" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3020,7 +3026,7 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>45832</c:v>
+                  <c:v>45831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4865,7 +4871,7 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>45832</c:v>
+                  <c:v>45831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6729,7 +6735,7 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>45832</c:v>
+                  <c:v>45831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8923,6 +8929,9 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
+                  <c:v>45831</c:v>
+                </c:pt>
+                <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
               </c:numCache>
@@ -9826,6 +9835,9 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="297">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="298">
                   <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
@@ -10769,6 +10781,9 @@
                   <c:v>45823</c:v>
                 </c:pt>
                 <c:pt idx="297">
+                  <c:v>45831</c:v>
+                </c:pt>
+                <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
               </c:numCache>
@@ -11672,6 +11687,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="297">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="298">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13500,13 +13518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q300"/>
+  <dimension ref="A1:Q301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I301" sqref="I301"/>
+      <selection pane="bottomRight" activeCell="I302" sqref="I302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26311,7 +26329,7 @@
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
-        <v>45832</v>
+        <v>45831</v>
       </c>
       <c r="B300" s="2">
         <v>9</v>
@@ -26355,6 +26373,55 @@
         <v>0</v>
       </c>
       <c r="O300">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>45832</v>
+      </c>
+      <c r="B301" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C301">
+        <f t="shared" ref="C301" si="508">SUM(D301:F301)</f>
+        <v>1673</v>
+      </c>
+      <c r="D301">
+        <v>1105</v>
+      </c>
+      <c r="E301">
+        <v>371</v>
+      </c>
+      <c r="F301" s="3">
+        <v>197</v>
+      </c>
+      <c r="G301" s="4">
+        <v>88</v>
+      </c>
+      <c r="H301" s="16">
+        <f t="shared" ref="H301" si="509">SUM(I301:K301)-SUM(L301:N301)</f>
+        <v>8562</v>
+      </c>
+      <c r="I301" s="5">
+        <v>6707</v>
+      </c>
+      <c r="J301" s="6">
+        <v>907</v>
+      </c>
+      <c r="K301" s="7">
+        <v>948</v>
+      </c>
+      <c r="L301">
+        <v>0</v>
+      </c>
+      <c r="M301">
+        <v>0</v>
+      </c>
+      <c r="N301">
+        <v>0</v>
+      </c>
+      <c r="O301">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: #559 (forced database refresh on release 2.8.0)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB68583-EC81-0B4C-A4FE-AC2C6846EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D664525-D0BC-8544-B9EA-3FDF81D84194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1182,6 +1182,9 @@
                 <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
+                <c:pt idx="299">
+                  <c:v>45833</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2086,6 +2089,9 @@
                   <c:v>8550</c:v>
                 </c:pt>
                 <c:pt idx="298" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8562</c:v>
+                </c:pt>
+                <c:pt idx="299" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8562</c:v>
                 </c:pt>
               </c:numCache>
@@ -8934,6 +8940,9 @@
                 <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
+                <c:pt idx="299">
+                  <c:v>45833</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9838,6 +9847,9 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="298">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="299">
                   <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
@@ -10786,6 +10798,9 @@
                 <c:pt idx="298">
                   <c:v>45832</c:v>
                 </c:pt>
+                <c:pt idx="299">
+                  <c:v>45833</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11690,6 +11705,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="298">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="299">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13518,13 +13536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q301"/>
+  <dimension ref="A1:Q302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I302" sqref="I302"/>
+      <selection pane="bottomRight" activeCell="I303" sqref="I303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26422,6 +26440,55 @@
         <v>0</v>
       </c>
       <c r="O301">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B302" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C302">
+        <f t="shared" ref="C302" si="510">SUM(D302:F302)</f>
+        <v>1673</v>
+      </c>
+      <c r="D302">
+        <v>1105</v>
+      </c>
+      <c r="E302">
+        <v>371</v>
+      </c>
+      <c r="F302" s="3">
+        <v>197</v>
+      </c>
+      <c r="G302" s="4">
+        <v>88</v>
+      </c>
+      <c r="H302" s="16">
+        <f t="shared" ref="H302" si="511">SUM(I302:K302)-SUM(L302:N302)</f>
+        <v>8562</v>
+      </c>
+      <c r="I302" s="5">
+        <v>6727</v>
+      </c>
+      <c r="J302" s="6">
+        <v>884</v>
+      </c>
+      <c r="K302" s="7">
+        <v>951</v>
+      </c>
+      <c r="L302">
+        <v>0</v>
+      </c>
+      <c r="M302">
+        <v>0</v>
+      </c>
+      <c r="N302">
+        <v>0</v>
+      </c>
+      <c r="O302">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: #565 New settings toggle to load extra clubs
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D664525-D0BC-8544-B9EA-3FDF81D84194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771D51DA-A67A-3B49-8DB2-4E2E037C5EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1185,6 +1185,9 @@
                 <c:pt idx="299">
                   <c:v>45833</c:v>
                 </c:pt>
+                <c:pt idx="300">
+                  <c:v>45844</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2093,6 +2096,9 @@
                 </c:pt>
                 <c:pt idx="299" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8562</c:v>
+                </c:pt>
+                <c:pt idx="300" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8943,6 +8949,9 @@
                 <c:pt idx="299">
                   <c:v>45833</c:v>
                 </c:pt>
+                <c:pt idx="300">
+                  <c:v>45844</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9850,6 +9859,9 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="299">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="300">
                   <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
@@ -10801,6 +10813,9 @@
                 <c:pt idx="299">
                   <c:v>45833</c:v>
                 </c:pt>
+                <c:pt idx="300">
+                  <c:v>45844</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11708,6 +11723,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="299">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="300">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13536,13 +13554,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q302"/>
+  <dimension ref="A1:Q303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I303" sqref="I303"/>
+      <selection pane="bottomRight" activeCell="I304" sqref="I304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26489,6 +26507,55 @@
         <v>0</v>
       </c>
       <c r="O302">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>45844</v>
+      </c>
+      <c r="B303" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C303">
+        <f t="shared" ref="C303" si="512">SUM(D303:F303)</f>
+        <v>1673</v>
+      </c>
+      <c r="D303">
+        <v>1105</v>
+      </c>
+      <c r="E303">
+        <v>371</v>
+      </c>
+      <c r="F303" s="3">
+        <v>197</v>
+      </c>
+      <c r="G303" s="4">
+        <v>88</v>
+      </c>
+      <c r="H303" s="16">
+        <f t="shared" ref="H303" si="513">SUM(I303:K303)-SUM(L303:N303)</f>
+        <v>8578</v>
+      </c>
+      <c r="I303" s="5">
+        <v>6741</v>
+      </c>
+      <c r="J303" s="6">
+        <v>886</v>
+      </c>
+      <c r="K303" s="7">
+        <v>951</v>
+      </c>
+      <c r="L303">
+        <v>0</v>
+      </c>
+      <c r="M303">
+        <v>0</v>
+      </c>
+      <c r="N303">
+        <v>0</v>
+      </c>
+      <c r="O303">
         <v>23</v>
       </c>
     </row>
@@ -26511,7 +26578,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="AA66" sqref="AA66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix: #566 new club IndividueelBO Club is hidden behind switch in settings (for now)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771D51DA-A67A-3B49-8DB2-4E2E037C5EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4A28F0-0A24-6643-BB43-B2CA501FA679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -2098,7 +2098,7 @@
                   <c:v>8562</c:v>
                 </c:pt>
                 <c:pt idx="300" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8578</c:v>
+                  <c:v>8619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9862,7 +9862,7 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="300">
-                  <c:v>88</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13556,11 +13556,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q303"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I304" sqref="I304"/>
+      <selection pane="bottomRight" activeCell="V309" sqref="V309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26531,20 +26531,20 @@
         <v>197</v>
       </c>
       <c r="G303" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H303" s="16">
         <f t="shared" ref="H303" si="513">SUM(I303:K303)-SUM(L303:N303)</f>
-        <v>8578</v>
+        <v>8619</v>
       </c>
       <c r="I303" s="5">
-        <v>6741</v>
+        <v>6764</v>
       </c>
       <c r="J303" s="6">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="K303" s="7">
-        <v>951</v>
+        <v>962</v>
       </c>
       <c r="L303">
         <v>0</v>
@@ -26577,7 +26577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA66" sqref="AA66"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated data for 1 member of fgDeGender
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2685255-64CE-B74E-A011-D5AFD52ACE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAADD9-6F34-1844-9CC4-3D51A548EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1191,6 +1191,9 @@
                 <c:pt idx="301">
                   <c:v>45857</c:v>
                 </c:pt>
+                <c:pt idx="302">
+                  <c:v>45858</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2104,6 +2107,9 @@
                   <c:v>8619</c:v>
                 </c:pt>
                 <c:pt idx="301" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8639</c:v>
+                </c:pt>
+                <c:pt idx="302" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8639</c:v>
                 </c:pt>
               </c:numCache>
@@ -8961,6 +8967,9 @@
                 <c:pt idx="301">
                   <c:v>45857</c:v>
                 </c:pt>
+                <c:pt idx="302">
+                  <c:v>45858</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9874,6 +9883,9 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="301">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="302">
                   <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
@@ -10831,6 +10843,9 @@
                 <c:pt idx="301">
                   <c:v>45857</c:v>
                 </c:pt>
+                <c:pt idx="302">
+                  <c:v>45858</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11744,6 +11759,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="301">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="302">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13572,13 +13590,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q304"/>
+  <dimension ref="A1:Q305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I305" sqref="I305"/>
+      <selection pane="bottomRight" activeCell="N309" sqref="N309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26623,6 +26641,55 @@
         <v>0</v>
       </c>
       <c r="O304">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>45858</v>
+      </c>
+      <c r="B305" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C305">
+        <f t="shared" ref="C305" si="516">SUM(D305:F305)</f>
+        <v>1673</v>
+      </c>
+      <c r="D305">
+        <v>1105</v>
+      </c>
+      <c r="E305">
+        <v>371</v>
+      </c>
+      <c r="F305" s="3">
+        <v>197</v>
+      </c>
+      <c r="G305" s="4">
+        <v>89</v>
+      </c>
+      <c r="H305" s="16">
+        <f t="shared" ref="H305" si="517">SUM(I305:K305)-SUM(L305:N305)</f>
+        <v>8639</v>
+      </c>
+      <c r="I305" s="5">
+        <v>6781</v>
+      </c>
+      <c r="J305" s="6">
+        <v>894</v>
+      </c>
+      <c r="K305" s="7">
+        <v>964</v>
+      </c>
+      <c r="L305">
+        <v>0</v>
+      </c>
+      <c r="M305">
+        <v>0</v>
+      </c>
+      <c r="N305">
+        <v>0</v>
+      </c>
+      <c r="O305">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: #578 Cleanup of dataResetPending code
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAADD9-6F34-1844-9CC4-3D51A548EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D13596-1517-8842-A100-2D13EDC39030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1194,6 +1194,9 @@
                 <c:pt idx="302">
                   <c:v>45858</c:v>
                 </c:pt>
+                <c:pt idx="303">
+                  <c:v>45868</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2111,6 +2114,9 @@
                 </c:pt>
                 <c:pt idx="302" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8639</c:v>
+                </c:pt>
+                <c:pt idx="303" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8970,6 +8976,9 @@
                 <c:pt idx="302">
                   <c:v>45858</c:v>
                 </c:pt>
+                <c:pt idx="303">
+                  <c:v>45868</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -9886,6 +9895,9 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="302">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="303">
                   <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
@@ -10846,6 +10858,9 @@
                 <c:pt idx="302">
                   <c:v>45858</c:v>
                 </c:pt>
+                <c:pt idx="303">
+                  <c:v>45868</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11762,6 +11777,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="302">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="303">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13590,13 +13608,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q305"/>
+  <dimension ref="A1:Q306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N309" sqref="N309"/>
+      <selection pane="bottomRight" activeCell="I307" sqref="I307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26690,6 +26708,55 @@
         <v>0</v>
       </c>
       <c r="O305">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>45868</v>
+      </c>
+      <c r="B306" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C306">
+        <f t="shared" ref="C306" si="518">SUM(D306:F306)</f>
+        <v>1673</v>
+      </c>
+      <c r="D306">
+        <v>1105</v>
+      </c>
+      <c r="E306">
+        <v>371</v>
+      </c>
+      <c r="F306" s="3">
+        <v>197</v>
+      </c>
+      <c r="G306" s="4">
+        <v>89</v>
+      </c>
+      <c r="H306" s="16">
+        <f t="shared" ref="H306" si="519">SUM(I306:K306)-SUM(L306:N306)</f>
+        <v>8651</v>
+      </c>
+      <c r="I306" s="5">
+        <v>6791</v>
+      </c>
+      <c r="J306" s="6">
+        <v>893</v>
+      </c>
+      <c r="K306" s="7">
+        <v>967</v>
+      </c>
+      <c r="L306">
+        <v>0</v>
+      </c>
+      <c r="M306">
+        <v>0</v>
+      </c>
+      <c r="N306">
+        <v>0</v>
+      </c>
+      <c r="O306">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduced String.canonicalCase to get case-insensitive behavior.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CF281B-87C4-694A-B942-1E85A3A2370B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AC33F9-96B2-A442-9D99-05A8C8C28570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1200,6 +1200,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2123,6 +2126,9 @@
                 </c:pt>
                 <c:pt idx="304" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8728</c:v>
+                </c:pt>
+                <c:pt idx="305" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3085,6 +3091,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4008,6 +4017,9 @@
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>6859</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>6959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4972,6 +4984,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5895,6 +5910,9 @@
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6878,6 +6896,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7801,6 +7822,9 @@
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9114,6 +9138,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10037,6 +10064,9 @@
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11002,6 +11032,9 @@
                 <c:pt idx="304">
                   <c:v>45870</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>45892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11924,6 +11957,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="304">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="305">
                   <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
@@ -13752,13 +13788,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q307"/>
+  <dimension ref="A1:Q308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I308" sqref="I308"/>
+      <selection pane="bottomRight" activeCell="G309" sqref="G309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26950,6 +26986,55 @@
         <v>0</v>
       </c>
       <c r="O307">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>45892</v>
+      </c>
+      <c r="B308" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C308">
+        <f t="shared" ref="C308" si="522">SUM(D308:F308)</f>
+        <v>1673</v>
+      </c>
+      <c r="D308">
+        <v>1105</v>
+      </c>
+      <c r="E308">
+        <v>371</v>
+      </c>
+      <c r="F308" s="3">
+        <v>197</v>
+      </c>
+      <c r="G308" s="4">
+        <v>90</v>
+      </c>
+      <c r="H308" s="16">
+        <f t="shared" ref="H308" si="523">SUM(I308:K308)-SUM(L308:N308)</f>
+        <v>8904</v>
+      </c>
+      <c r="I308" s="5">
+        <v>6959</v>
+      </c>
+      <c r="J308" s="6">
+        <v>977</v>
+      </c>
+      <c r="K308" s="7">
+        <v>968</v>
+      </c>
+      <c r="L308">
+        <v>0</v>
+      </c>
+      <c r="M308">
+        <v>0</v>
+      </c>
+      <c r="N308">
+        <v>0</v>
+      </c>
+      <c r="O308">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated testing of Expertise class. Changes related to case-insensitivity changes.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AC33F9-96B2-A442-9D99-05A8C8C28570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAA7A53-D35F-514B-8C88-3F1CDA9CC0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1203,6 +1203,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2129,6 +2132,9 @@
                 </c:pt>
                 <c:pt idx="305" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8904</c:v>
+                </c:pt>
+                <c:pt idx="306" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>8971</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3094,6 +3100,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4020,6 +4029,9 @@
                 </c:pt>
                 <c:pt idx="305">
                   <c:v>6959</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>7046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4987,6 +4999,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5913,6 +5928,9 @@
                 </c:pt>
                 <c:pt idx="305">
                   <c:v>977</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6899,6 +6917,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7825,6 +7846,9 @@
                 </c:pt>
                 <c:pt idx="305">
                   <c:v>968</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7851,7 +7875,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45900"/>
+          <c:max val="45930"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -9141,6 +9165,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10066,6 +10093,9 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="305">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="306">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -11035,6 +11065,9 @@
                 <c:pt idx="305">
                   <c:v>45892</c:v>
                 </c:pt>
+                <c:pt idx="306">
+                  <c:v>45895</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11961,6 +11994,9 @@
                 </c:pt>
                 <c:pt idx="305">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13788,13 +13824,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q308"/>
+  <dimension ref="A1:Q309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G309" sqref="G309"/>
+      <selection pane="bottomRight" activeCell="I310" sqref="I310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27036,6 +27072,55 @@
       </c>
       <c r="O308">
         <v>23</v>
+      </c>
+    </row>
+    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>45895</v>
+      </c>
+      <c r="B309" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C309">
+        <f t="shared" ref="C309" si="524">SUM(D309:F309)</f>
+        <v>1673</v>
+      </c>
+      <c r="D309">
+        <v>1105</v>
+      </c>
+      <c r="E309">
+        <v>371</v>
+      </c>
+      <c r="F309" s="3">
+        <v>197</v>
+      </c>
+      <c r="G309" s="4">
+        <v>90</v>
+      </c>
+      <c r="H309" s="16">
+        <f t="shared" ref="H309" si="525">SUM(I309:K309)-SUM(L309:N309)</f>
+        <v>8971</v>
+      </c>
+      <c r="I309" s="5">
+        <v>7046</v>
+      </c>
+      <c r="J309" s="6">
+        <v>939</v>
+      </c>
+      <c r="K309" s="7">
+        <v>986</v>
+      </c>
+      <c r="L309">
+        <v>0</v>
+      </c>
+      <c r="M309">
+        <v>0</v>
+      </c>
+      <c r="N309">
+        <v>0</v>
+      </c>
+      <c r="O309">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed test problem: random Town value generated for testing triggered an assertion in code.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAA7A53-D35F-514B-8C88-3F1CDA9CC0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F96575F-A5ED-F041-8AAB-5241958D1B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1206,6 +1206,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2135,6 +2138,9 @@
                 </c:pt>
                 <c:pt idx="306" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>8971</c:v>
+                </c:pt>
+                <c:pt idx="307" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>9040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3103,6 +3109,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4032,6 +4041,9 @@
                 </c:pt>
                 <c:pt idx="306">
                   <c:v>7046</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>7177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5002,6 +5014,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5931,6 +5946,9 @@
                 </c:pt>
                 <c:pt idx="306">
                   <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6920,6 +6938,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7849,6 +7870,9 @@
                 </c:pt>
                 <c:pt idx="306">
                   <c:v>986</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9168,6 +9192,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10096,6 +10123,9 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="306">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="307">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -11068,6 +11098,9 @@
                 <c:pt idx="306">
                   <c:v>45895</c:v>
                 </c:pt>
+                <c:pt idx="307">
+                  <c:v>45898</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -11996,6 +12029,9 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="306">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="307">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -13824,13 +13860,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q309"/>
+  <dimension ref="A1:Q310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I310" sqref="I310"/>
+      <selection pane="bottomRight" activeCell="L310" sqref="L310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27120,6 +27156,55 @@
         <v>0</v>
       </c>
       <c r="O309">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>45898</v>
+      </c>
+      <c r="B310" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C310">
+        <f t="shared" ref="C310" si="526">SUM(D310:F310)</f>
+        <v>1673</v>
+      </c>
+      <c r="D310">
+        <v>1105</v>
+      </c>
+      <c r="E310">
+        <v>371</v>
+      </c>
+      <c r="F310" s="3">
+        <v>197</v>
+      </c>
+      <c r="G310" s="4">
+        <v>90</v>
+      </c>
+      <c r="H310" s="16">
+        <f t="shared" ref="H310" si="527">SUM(I310:K310)-SUM(L310:N310)</f>
+        <v>9040</v>
+      </c>
+      <c r="I310" s="5">
+        <v>7177</v>
+      </c>
+      <c r="J310" s="6">
+        <v>905</v>
+      </c>
+      <c r="K310" s="7">
+        <v>958</v>
+      </c>
+      <c r="L310">
+        <v>0</v>
+      </c>
+      <c r="M310">
+        <v>0</v>
+      </c>
+      <c r="N310">
+        <v>0</v>
+      </c>
+      <c r="O310">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split 7 more files into versions for iOS 17/18 versus iOS 26
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F96575F-A5ED-F041-8AAB-5241958D1B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE43BF-9376-7145-A536-05F71BC409EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1209,6 +1209,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2141,6 +2144,9 @@
                 </c:pt>
                 <c:pt idx="307" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>9040</c:v>
+                </c:pt>
+                <c:pt idx="308" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>10657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3112,6 +3118,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4044,6 +4053,9 @@
                 </c:pt>
                 <c:pt idx="307">
                   <c:v>7177</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>8635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5017,6 +5029,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5949,6 +5964,9 @@
                 </c:pt>
                 <c:pt idx="307">
                   <c:v>905</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6941,6 +6959,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7873,6 +7894,9 @@
                 </c:pt>
                 <c:pt idx="307">
                   <c:v>958</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>1043</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9195,6 +9219,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10127,6 +10154,9 @@
                 </c:pt>
                 <c:pt idx="307">
                   <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11101,6 +11131,9 @@
                 <c:pt idx="307">
                   <c:v>45898</c:v>
                 </c:pt>
+                <c:pt idx="308">
+                  <c:v>45908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12032,6 +12065,9 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="307">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="308">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -13860,13 +13896,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q310"/>
+  <dimension ref="A1:Q311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L310" sqref="L310"/>
+      <selection pane="bottomRight" activeCell="G312" sqref="G312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27205,6 +27241,55 @@
         <v>0</v>
       </c>
       <c r="O310">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>45908</v>
+      </c>
+      <c r="B311" s="2">
+        <v>6707</v>
+      </c>
+      <c r="C311">
+        <f t="shared" ref="C311" si="528">SUM(D311:F311)</f>
+        <v>1673</v>
+      </c>
+      <c r="D311">
+        <v>1105</v>
+      </c>
+      <c r="E311">
+        <v>371</v>
+      </c>
+      <c r="F311" s="3">
+        <v>197</v>
+      </c>
+      <c r="G311" s="4">
+        <v>99</v>
+      </c>
+      <c r="H311" s="16">
+        <f t="shared" ref="H311" si="529">SUM(I311:K311)-SUM(L311:N311)</f>
+        <v>10657</v>
+      </c>
+      <c r="I311" s="5">
+        <v>8635</v>
+      </c>
+      <c r="J311" s="6">
+        <v>979</v>
+      </c>
+      <c r="K311" s="7">
+        <v>1043</v>
+      </c>
+      <c r="L311">
+        <v>0</v>
+      </c>
+      <c r="M311">
+        <v>0</v>
+      </c>
+      <c r="N311">
+        <v>0</v>
+      </c>
+      <c r="O311">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Release notes and line count
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A12C90B-D960-A445-AE99-02F6FCB29DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BBAA61-A99E-194E-9733-A6AAFFEF50E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="740" yWindow="620" windowWidth="35220" windowHeight="26380" activeTab="2" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -8287,7 +8287,7 @@
           <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Unit Tests</c:v>
+            <c:v>Swift files</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -10186,7 +10186,7 @@
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="309">
-                  <c:v>100</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10202,7 +10202,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Swift files</c:v>
+            <c:v>Unit tests</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -12104,7 +12104,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="309">
-                  <c:v>24</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12131,7 +12131,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45800"/>
+          <c:max val="45930"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -12197,7 +12197,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="105"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -13938,7 +13938,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G313" sqref="G313"/>
+      <selection pane="bottomRight" activeCell="O313" sqref="O313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27350,7 +27350,7 @@
         <v>197</v>
       </c>
       <c r="G312" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H312" s="16">
         <f t="shared" ref="H312" si="531">SUM(I312:K312)-SUM(L312:N312)</f>
@@ -27375,7 +27375,7 @@
         <v>0</v>
       </c>
       <c r="O312">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -27396,7 +27396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
@@ -27411,7 +27411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01361E9F-285B-9946-B1BF-3886CBEE5CAD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AF65" sqref="AF65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preparations for next release
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FB0FF2-5236-D34A-9BEF-296E30B58635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED9AE2-2BA0-3748-9FF3-820F9938892A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16640" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1221,6 +1221,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2165,6 +2168,9 @@
                 </c:pt>
                 <c:pt idx="311" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11108</c:v>
+                </c:pt>
+                <c:pt idx="312" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3148,6 +3154,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4092,6 +4101,9 @@
                 </c:pt>
                 <c:pt idx="311">
                   <c:v>9039</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>9132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5077,6 +5089,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6021,6 +6036,9 @@
                 </c:pt>
                 <c:pt idx="311">
                   <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7025,6 +7043,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7969,6 +7990,9 @@
                 </c:pt>
                 <c:pt idx="311">
                   <c:v>1069</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>1033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9303,6 +9327,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10246,6 +10273,9 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="311">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="312">
                   <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
@@ -11233,6 +11263,9 @@
                 <c:pt idx="311">
                   <c:v>45949</c:v>
                 </c:pt>
+                <c:pt idx="312">
+                  <c:v>45954</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12176,6 +12209,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="311">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="312">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14004,13 +14040,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q314"/>
+  <dimension ref="A1:Q315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B314" sqref="A314:H314"/>
+      <selection pane="bottomRight" activeCell="T310" sqref="T310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26867,7 +26903,7 @@
         <v>45832</v>
       </c>
       <c r="B301" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C301">
         <f t="shared" ref="C301" si="508">SUM(D301:F301)</f>
@@ -26916,7 +26952,7 @@
         <v>45833</v>
       </c>
       <c r="B302" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C302">
         <f t="shared" ref="C302" si="510">SUM(D302:F302)</f>
@@ -26965,7 +27001,7 @@
         <v>45844</v>
       </c>
       <c r="B303" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C303">
         <f t="shared" ref="C303" si="512">SUM(D303:F303)</f>
@@ -27014,7 +27050,7 @@
         <v>45857</v>
       </c>
       <c r="B304" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C304">
         <f t="shared" ref="C304" si="514">SUM(D304:F304)</f>
@@ -27063,7 +27099,7 @@
         <v>45858</v>
       </c>
       <c r="B305" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C305">
         <f t="shared" ref="C305" si="516">SUM(D305:F305)</f>
@@ -27112,7 +27148,7 @@
         <v>45868</v>
       </c>
       <c r="B306" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C306">
         <f t="shared" ref="C306" si="518">SUM(D306:F306)</f>
@@ -27161,7 +27197,7 @@
         <v>45870</v>
       </c>
       <c r="B307" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C307">
         <f t="shared" ref="C307" si="520">SUM(D307:F307)</f>
@@ -27210,7 +27246,7 @@
         <v>45892</v>
       </c>
       <c r="B308" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C308">
         <f t="shared" ref="C308" si="522">SUM(D308:F308)</f>
@@ -27259,7 +27295,7 @@
         <v>45895</v>
       </c>
       <c r="B309" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C309">
         <f t="shared" ref="C309" si="524">SUM(D309:F309)</f>
@@ -27308,7 +27344,7 @@
         <v>45898</v>
       </c>
       <c r="B310" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C310">
         <f t="shared" ref="C310" si="526">SUM(D310:F310)</f>
@@ -27357,7 +27393,7 @@
         <v>45908</v>
       </c>
       <c r="B311" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C311">
         <f t="shared" ref="C311" si="528">SUM(D311:F311)</f>
@@ -27406,7 +27442,7 @@
         <v>45913</v>
       </c>
       <c r="B312" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C312">
         <f t="shared" ref="C312" si="530">SUM(D312:F312)</f>
@@ -27455,7 +27491,7 @@
         <v>45931</v>
       </c>
       <c r="B313" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C313">
         <f t="shared" ref="C313" si="532">SUM(D313:F313)</f>
@@ -27504,7 +27540,7 @@
         <v>45949</v>
       </c>
       <c r="B314" s="2">
-        <v>6707</v>
+        <v>9</v>
       </c>
       <c r="C314">
         <f t="shared" ref="C314" si="534">SUM(D314:F314)</f>
@@ -27545,6 +27581,55 @@
         <v>0</v>
       </c>
       <c r="O314">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A315" s="1">
+        <v>45954</v>
+      </c>
+      <c r="B315" s="2">
+        <v>9</v>
+      </c>
+      <c r="C315">
+        <f t="shared" ref="C315" si="536">SUM(D315:F315)</f>
+        <v>1673</v>
+      </c>
+      <c r="D315">
+        <v>1105</v>
+      </c>
+      <c r="E315">
+        <v>371</v>
+      </c>
+      <c r="F315" s="3">
+        <v>197</v>
+      </c>
+      <c r="G315" s="4">
+        <v>101</v>
+      </c>
+      <c r="H315" s="16">
+        <f t="shared" ref="H315" si="537">SUM(I315:K315)-SUM(L315:N315)</f>
+        <v>11162</v>
+      </c>
+      <c r="I315" s="5">
+        <v>9132</v>
+      </c>
+      <c r="J315" s="6">
+        <v>997</v>
+      </c>
+      <c r="K315" s="7">
+        <v>1033</v>
+      </c>
+      <c r="L315">
+        <v>0</v>
+      </c>
+      <c r="M315">
+        <v>0</v>
+      </c>
+      <c r="N315">
+        <v>0</v>
+      </c>
+      <c r="O315">
         <v>31</v>
       </c>
     </row>
@@ -27566,8 +27651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="G37" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Renamed PPT to FotoclubHubIntro_NL to prepare for a future FotoclubHubIntro_EN
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED9AE2-2BA0-3748-9FF3-820F9938892A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E5B52B-D991-DA48-8F30-8FFE18437749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1224,6 +1224,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2170,6 +2173,9 @@
                   <c:v>11108</c:v>
                 </c:pt>
                 <c:pt idx="312" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11162</c:v>
+                </c:pt>
+                <c:pt idx="313" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11162</c:v>
                 </c:pt>
               </c:numCache>
@@ -3157,6 +3163,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4103,6 +4112,9 @@
                   <c:v>9039</c:v>
                 </c:pt>
                 <c:pt idx="312">
+                  <c:v>9132</c:v>
+                </c:pt>
+                <c:pt idx="313">
                   <c:v>9132</c:v>
                 </c:pt>
               </c:numCache>
@@ -5092,6 +5104,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6038,6 +6053,9 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="312">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="313">
                   <c:v>997</c:v>
                 </c:pt>
               </c:numCache>
@@ -7046,6 +7064,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7992,6 +8013,9 @@
                   <c:v>1069</c:v>
                 </c:pt>
                 <c:pt idx="312">
+                  <c:v>1033</c:v>
+                </c:pt>
+                <c:pt idx="313">
                   <c:v>1033</c:v>
                 </c:pt>
               </c:numCache>
@@ -9330,6 +9354,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10276,6 +10303,9 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="312">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="313">
                   <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
@@ -11266,6 +11296,9 @@
                 <c:pt idx="312">
                   <c:v>45954</c:v>
                 </c:pt>
+                <c:pt idx="313">
+                  <c:v>45965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12212,6 +12245,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="312">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="313">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14040,13 +14076,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q315"/>
+  <dimension ref="A1:Q316"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T310" sqref="T310"/>
+      <selection pane="bottomRight" activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27633,6 +27669,55 @@
         <v>31</v>
       </c>
     </row>
+    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>45965</v>
+      </c>
+      <c r="B316" s="2">
+        <v>9</v>
+      </c>
+      <c r="C316">
+        <f t="shared" ref="C316" si="538">SUM(D316:F316)</f>
+        <v>1673</v>
+      </c>
+      <c r="D316">
+        <v>1105</v>
+      </c>
+      <c r="E316">
+        <v>371</v>
+      </c>
+      <c r="F316" s="3">
+        <v>197</v>
+      </c>
+      <c r="G316" s="4">
+        <v>101</v>
+      </c>
+      <c r="H316" s="16">
+        <f t="shared" ref="H316" si="539">SUM(I316:K316)-SUM(L316:N316)</f>
+        <v>11162</v>
+      </c>
+      <c r="I316" s="5">
+        <v>9132</v>
+      </c>
+      <c r="J316" s="6">
+        <v>997</v>
+      </c>
+      <c r="K316" s="7">
+        <v>1033</v>
+      </c>
+      <c r="L316">
+        <v>0</v>
+      </c>
+      <c r="M316">
+        <v>0</v>
+      </c>
+      <c r="N316">
+        <v>0</v>
+      </c>
+      <c r="O316">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -27651,7 +27736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added image assets for PreludeView
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E5B52B-D991-DA48-8F30-8FFE18437749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92661F2A-FC74-E94F-BA1D-962C4A31D125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1227,6 +1227,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2177,6 +2180,9 @@
                 </c:pt>
                 <c:pt idx="313" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11162</c:v>
+                </c:pt>
+                <c:pt idx="314" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3166,6 +3172,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4116,6 +4125,9 @@
                 </c:pt>
                 <c:pt idx="313">
                   <c:v>9132</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>9134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5107,6 +5119,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6057,6 +6072,9 @@
                 </c:pt>
                 <c:pt idx="313">
                   <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>1002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7067,6 +7085,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8016,6 +8037,9 @@
                   <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="313">
+                  <c:v>1033</c:v>
+                </c:pt>
+                <c:pt idx="314">
                   <c:v>1033</c:v>
                 </c:pt>
               </c:numCache>
@@ -9357,6 +9381,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10307,6 +10334,9 @@
                 </c:pt>
                 <c:pt idx="313">
                   <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11299,6 +11329,9 @@
                 <c:pt idx="313">
                   <c:v>45965</c:v>
                 </c:pt>
+                <c:pt idx="314">
+                  <c:v>45972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12248,6 +12281,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="313">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="314">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14076,13 +14112,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q316"/>
+  <dimension ref="A1:Q317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A316" sqref="A316"/>
+      <selection pane="bottomRight" activeCell="I318" sqref="I318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27715,6 +27751,55 @@
         <v>0</v>
       </c>
       <c r="O316">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>45972</v>
+      </c>
+      <c r="B317" s="2">
+        <v>9</v>
+      </c>
+      <c r="C317">
+        <f t="shared" ref="C317" si="540">SUM(D317:F317)</f>
+        <v>1673</v>
+      </c>
+      <c r="D317">
+        <v>1105</v>
+      </c>
+      <c r="E317">
+        <v>371</v>
+      </c>
+      <c r="F317" s="3">
+        <v>197</v>
+      </c>
+      <c r="G317" s="4">
+        <v>102</v>
+      </c>
+      <c r="H317" s="16">
+        <f t="shared" ref="H317" si="541">SUM(I317:K317)-SUM(L317:N317)</f>
+        <v>11169</v>
+      </c>
+      <c r="I317" s="5">
+        <v>9134</v>
+      </c>
+      <c r="J317" s="6">
+        <v>1002</v>
+      </c>
+      <c r="K317" s="7">
+        <v>1033</v>
+      </c>
+      <c r="L317">
+        <v>0</v>
+      </c>
+      <c r="M317">
+        <v>0</v>
+      </c>
+      <c r="N317">
+        <v>0</v>
+      </c>
+      <c r="O317">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: #630 Prelude View randomly selects 1 of 6 images.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92661F2A-FC74-E94F-BA1D-962C4A31D125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B06F4B-359E-8144-9306-D77DC1D3924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -2182,7 +2182,7 @@
                   <c:v>11162</c:v>
                 </c:pt>
                 <c:pt idx="314" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11169</c:v>
+                  <c:v>11246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4127,7 +4127,7 @@
                   <c:v>9132</c:v>
                 </c:pt>
                 <c:pt idx="314">
-                  <c:v>9134</c:v>
+                  <c:v>9197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8040,7 +8040,7 @@
                   <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="314">
-                  <c:v>1033</c:v>
+                  <c:v>1047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27779,16 +27779,16 @@
       </c>
       <c r="H317" s="16">
         <f t="shared" ref="H317" si="541">SUM(I317:K317)-SUM(L317:N317)</f>
-        <v>11169</v>
+        <v>11246</v>
       </c>
       <c r="I317" s="5">
-        <v>9134</v>
+        <v>9197</v>
       </c>
       <c r="J317" s="6">
         <v>1002</v>
       </c>
       <c r="K317" s="7">
-        <v>1033</v>
+        <v>1047</v>
       </c>
       <c r="L317">
         <v>0</v>

</xml_diff>

<commit_message>
Replaced fileprivate by private. This occurred in many source files.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B4B463-6617-E348-9F5C-4CFFB5C6A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE86467-F056-9145-B826-FECD745847FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1230,6 +1230,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2183,6 +2186,9 @@
                 </c:pt>
                 <c:pt idx="314" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11303</c:v>
+                </c:pt>
+                <c:pt idx="315" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3175,6 +3181,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4128,6 +4137,9 @@
                 </c:pt>
                 <c:pt idx="314">
                   <c:v>9236</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>9232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5122,6 +5134,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6075,6 +6090,9 @@
                 </c:pt>
                 <c:pt idx="314">
                   <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7088,6 +7106,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8041,6 +8062,9 @@
                 </c:pt>
                 <c:pt idx="314">
                   <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1060</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9384,6 +9408,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10336,6 +10363,9 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="314">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="315">
                   <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
@@ -11332,6 +11362,9 @@
                 <c:pt idx="314">
                   <c:v>45972</c:v>
                 </c:pt>
+                <c:pt idx="315">
+                  <c:v>45973</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12284,6 +12317,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="314">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="315">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14112,13 +14148,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q317"/>
+  <dimension ref="A1:Q318"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C298" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I318" sqref="I318"/>
+      <selection pane="bottomRight" activeCell="I319" sqref="I319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27803,6 +27839,55 @@
         <v>31</v>
       </c>
     </row>
+    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>45973</v>
+      </c>
+      <c r="B318" s="2">
+        <v>9</v>
+      </c>
+      <c r="C318">
+        <f t="shared" ref="C318" si="542">SUM(D318:F318)</f>
+        <v>1673</v>
+      </c>
+      <c r="D318">
+        <v>1105</v>
+      </c>
+      <c r="E318">
+        <v>371</v>
+      </c>
+      <c r="F318" s="3">
+        <v>197</v>
+      </c>
+      <c r="G318" s="4">
+        <v>103</v>
+      </c>
+      <c r="H318" s="16">
+        <f t="shared" ref="H318" si="543">SUM(I318:K318)-SUM(L318:N318)</f>
+        <v>11304</v>
+      </c>
+      <c r="I318" s="5">
+        <v>9232</v>
+      </c>
+      <c r="J318" s="6">
+        <v>1012</v>
+      </c>
+      <c r="K318" s="7">
+        <v>1060</v>
+      </c>
+      <c r="L318">
+        <v>0</v>
+      </c>
+      <c r="M318">
+        <v>0</v>
+      </c>
+      <c r="N318">
+        <v>0</v>
+      </c>
+      <c r="O318">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -27821,7 +27906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PreludeView - alignment of copyright
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BC2D0F-9B93-D64D-8D4A-CF7D31C2FD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9763D05-B72B-D844-8233-16B94B138276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16640" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1236,6 +1236,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2195,6 +2198,9 @@
                 </c:pt>
                 <c:pt idx="316" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11360</c:v>
+                </c:pt>
+                <c:pt idx="317" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3193,6 +3199,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4152,6 +4161,9 @@
                 </c:pt>
                 <c:pt idx="316">
                   <c:v>9263</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>9305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5152,6 +5164,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6111,6 +6126,9 @@
                 </c:pt>
                 <c:pt idx="316">
                   <c:v>1032</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>1038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7130,6 +7148,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8089,6 +8110,9 @@
                 </c:pt>
                 <c:pt idx="316">
                   <c:v>1065</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>1071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9438,6 +9462,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10397,6 +10424,9 @@
                 </c:pt>
                 <c:pt idx="316">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11398,6 +11428,9 @@
                 <c:pt idx="316">
                   <c:v>45975</c:v>
                 </c:pt>
+                <c:pt idx="317">
+                  <c:v>45976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12356,6 +12389,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="316">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="317">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14184,13 +14220,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q319"/>
+  <dimension ref="A1:Q320"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I320" sqref="I320"/>
+      <selection pane="bottomRight" activeCell="K321" sqref="K321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27973,6 +28009,55 @@
         <v>31</v>
       </c>
     </row>
+    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>45976</v>
+      </c>
+      <c r="B320" s="2">
+        <v>9</v>
+      </c>
+      <c r="C320">
+        <f t="shared" ref="C320" si="546">SUM(D320:F320)</f>
+        <v>1673</v>
+      </c>
+      <c r="D320">
+        <v>1105</v>
+      </c>
+      <c r="E320">
+        <v>371</v>
+      </c>
+      <c r="F320" s="3">
+        <v>197</v>
+      </c>
+      <c r="G320" s="4">
+        <v>104</v>
+      </c>
+      <c r="H320" s="16">
+        <f t="shared" ref="H320" si="547">SUM(I320:K320)-SUM(L320:N320)</f>
+        <v>11414</v>
+      </c>
+      <c r="I320" s="5">
+        <v>9305</v>
+      </c>
+      <c r="J320" s="6">
+        <v>1038</v>
+      </c>
+      <c r="K320" s="7">
+        <v>1071</v>
+      </c>
+      <c r="L320">
+        <v>0</v>
+      </c>
+      <c r="M320">
+        <v>0</v>
+      </c>
+      <c r="N320">
+        <v>0</v>
+      </c>
+      <c r="O320">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -27991,7 +28076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #633 Swiping on Preview screen.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9763D05-B72B-D844-8233-16B94B138276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED151A9-FD46-1A41-9B36-2F2F1F2D6F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16640" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -2200,7 +2200,7 @@
                   <c:v>11360</c:v>
                 </c:pt>
                 <c:pt idx="317" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11414</c:v>
+                  <c:v>11437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4163,7 +4163,7 @@
                   <c:v>9263</c:v>
                 </c:pt>
                 <c:pt idx="317">
-                  <c:v>9305</c:v>
+                  <c:v>9315</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6128,7 +6128,7 @@
                   <c:v>1032</c:v>
                 </c:pt>
                 <c:pt idx="317">
-                  <c:v>1038</c:v>
+                  <c:v>1051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8205,7 +8205,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="11500"/>
+          <c:max val="12000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8315,7 +8315,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8333,6 +8333,39 @@
         <c:crossAx val="1582352671"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -14222,11 +14255,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K321" sqref="K321"/>
+      <selection pane="bottomRight" activeCell="I321" sqref="I321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28034,13 +28067,13 @@
       </c>
       <c r="H320" s="16">
         <f t="shared" ref="H320" si="547">SUM(I320:K320)-SUM(L320:N320)</f>
-        <v>11414</v>
+        <v>11437</v>
       </c>
       <c r="I320" s="5">
-        <v>9305</v>
+        <v>9315</v>
       </c>
       <c r="J320" s="6">
-        <v>1038</v>
+        <v>1051</v>
       </c>
       <c r="K320" s="7">
         <v>1071</v>
@@ -28076,8 +28109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AA53" sqref="AA53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix: 643 Sync with Photo Club Hub HTML
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3E9CA3-F5BF-FA4D-9AEC-29695EEEE5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC1DD0-5283-AA40-84A4-D169CDC1CD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1242,6 +1242,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2207,6 +2210,9 @@
                 </c:pt>
                 <c:pt idx="318" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>11518</c:v>
+                </c:pt>
+                <c:pt idx="319" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>11618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3211,6 +3217,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4176,6 +4185,9 @@
                 </c:pt>
                 <c:pt idx="318">
                   <c:v>9340</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>9402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5182,6 +5194,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6147,6 +6162,9 @@
                 </c:pt>
                 <c:pt idx="318">
                   <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>1110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7172,6 +7190,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8137,6 +8158,9 @@
                 </c:pt>
                 <c:pt idx="318">
                   <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>1106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9525,6 +9549,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10490,6 +10517,9 @@
                 </c:pt>
                 <c:pt idx="318">
                   <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11497,6 +11527,9 @@
                 <c:pt idx="318">
                   <c:v>45989</c:v>
                 </c:pt>
+                <c:pt idx="319">
+                  <c:v>46004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12461,6 +12494,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="318">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="319">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14289,13 +14325,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q321"/>
+  <dimension ref="A1:Q322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I322" sqref="I322"/>
+      <selection pane="bottomRight" activeCell="G323" sqref="G323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28173,6 +28209,55 @@
         <v>0</v>
       </c>
       <c r="O321">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>46004</v>
+      </c>
+      <c r="B322" s="2">
+        <v>9</v>
+      </c>
+      <c r="C322">
+        <f t="shared" ref="C322" si="550">SUM(D322:F322)</f>
+        <v>1673</v>
+      </c>
+      <c r="D322">
+        <v>1105</v>
+      </c>
+      <c r="E322">
+        <v>371</v>
+      </c>
+      <c r="F322" s="3">
+        <v>197</v>
+      </c>
+      <c r="G322" s="4">
+        <v>108</v>
+      </c>
+      <c r="H322" s="16">
+        <f t="shared" ref="H322" si="551">SUM(I322:K322)-SUM(L322:N322)</f>
+        <v>11618</v>
+      </c>
+      <c r="I322" s="5">
+        <v>9402</v>
+      </c>
+      <c r="J322" s="6">
+        <v>1110</v>
+      </c>
+      <c r="K322" s="7">
+        <v>1106</v>
+      </c>
+      <c r="L322">
+        <v>0</v>
+      </c>
+      <c r="M322">
+        <v>0</v>
+      </c>
+      <c r="N322">
+        <v>0</v>
+      </c>
+      <c r="O322">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added loading of Persoonlijk03.level2.json
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC1DD0-5283-AA40-84A4-D169CDC1CD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A3C1D-575B-F045-9C61-F134E06A5212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="26380" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1245,6 +1245,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2014,205 +2017,208 @@
                   <c:v>7047</c:v>
                 </c:pt>
                 <c:pt idx="253" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7052</c:v>
+                  <c:v>5641</c:v>
                 </c:pt>
                 <c:pt idx="254" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7060</c:v>
+                  <c:v>5649</c:v>
                 </c:pt>
                 <c:pt idx="255" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6950</c:v>
+                  <c:v>5539</c:v>
                 </c:pt>
                 <c:pt idx="256" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6953</c:v>
+                  <c:v>5542</c:v>
                 </c:pt>
                 <c:pt idx="257" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6968</c:v>
+                  <c:v>5557</c:v>
                 </c:pt>
                 <c:pt idx="258" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6665</c:v>
+                  <c:v>5254</c:v>
                 </c:pt>
                 <c:pt idx="259" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6699</c:v>
+                  <c:v>5288</c:v>
                 </c:pt>
                 <c:pt idx="260" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6387</c:v>
+                  <c:v>4976</c:v>
                 </c:pt>
                 <c:pt idx="261" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6390</c:v>
+                  <c:v>4979</c:v>
                 </c:pt>
                 <c:pt idx="262" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>4951</c:v>
+                </c:pt>
+                <c:pt idx="263" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5076</c:v>
+                </c:pt>
+                <c:pt idx="264" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>4959</c:v>
+                </c:pt>
+                <c:pt idx="265" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>4959</c:v>
+                </c:pt>
+                <c:pt idx="266" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>4954</c:v>
+                </c:pt>
+                <c:pt idx="267" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5085</c:v>
+                </c:pt>
+                <c:pt idx="268" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>4982</c:v>
+                </c:pt>
+                <c:pt idx="269" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5003</c:v>
+                </c:pt>
+                <c:pt idx="270" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5023</c:v>
+                </c:pt>
+                <c:pt idx="271" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>5966</c:v>
+                </c:pt>
+                <c:pt idx="272" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6056</c:v>
+                </c:pt>
+                <c:pt idx="273" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>6273</c:v>
+                </c:pt>
+                <c:pt idx="274" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6362</c:v>
                 </c:pt>
-                <c:pt idx="263" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6487</c:v>
-                </c:pt>
-                <c:pt idx="264" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>6370</c:v>
                 </c:pt>
-                <c:pt idx="265" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6370</c:v>
-                </c:pt>
-                <c:pt idx="266" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6365</c:v>
-                </c:pt>
-                <c:pt idx="267" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6496</c:v>
-                </c:pt>
-                <c:pt idx="268" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6393</c:v>
-                </c:pt>
-                <c:pt idx="269" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6414</c:v>
-                </c:pt>
-                <c:pt idx="270" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6434</c:v>
-                </c:pt>
-                <c:pt idx="271" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7377</c:v>
-                </c:pt>
-                <c:pt idx="272" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7467</c:v>
-                </c:pt>
-                <c:pt idx="273" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7684</c:v>
-                </c:pt>
-                <c:pt idx="274" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7773</c:v>
-                </c:pt>
-                <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7781</c:v>
-                </c:pt>
                 <c:pt idx="276" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7956</c:v>
+                  <c:v>6545</c:v>
                 </c:pt>
                 <c:pt idx="277" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7934</c:v>
+                  <c:v>6523</c:v>
                 </c:pt>
                 <c:pt idx="278" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8037</c:v>
+                  <c:v>6626</c:v>
                 </c:pt>
                 <c:pt idx="279" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8280</c:v>
+                  <c:v>6869</c:v>
                 </c:pt>
                 <c:pt idx="280" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8306</c:v>
+                  <c:v>6895</c:v>
                 </c:pt>
                 <c:pt idx="281" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8345</c:v>
+                  <c:v>6934</c:v>
                 </c:pt>
                 <c:pt idx="282" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8453</c:v>
+                  <c:v>7042</c:v>
                 </c:pt>
                 <c:pt idx="283" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8499</c:v>
+                  <c:v>7088</c:v>
                 </c:pt>
                 <c:pt idx="284" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8569</c:v>
+                  <c:v>7158</c:v>
                 </c:pt>
                 <c:pt idx="285" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8559</c:v>
+                  <c:v>7148</c:v>
                 </c:pt>
                 <c:pt idx="286" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8561</c:v>
+                  <c:v>7150</c:v>
                 </c:pt>
                 <c:pt idx="287" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8080</c:v>
+                  <c:v>6669</c:v>
                 </c:pt>
                 <c:pt idx="288" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8129</c:v>
+                  <c:v>6718</c:v>
                 </c:pt>
                 <c:pt idx="289" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8159</c:v>
+                  <c:v>6748</c:v>
                 </c:pt>
                 <c:pt idx="290" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8269</c:v>
+                  <c:v>6858</c:v>
                 </c:pt>
                 <c:pt idx="291" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8646</c:v>
+                  <c:v>7235</c:v>
                 </c:pt>
                 <c:pt idx="292" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8324</c:v>
+                  <c:v>6913</c:v>
                 </c:pt>
                 <c:pt idx="293" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8437</c:v>
+                  <c:v>7026</c:v>
                 </c:pt>
                 <c:pt idx="294" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8462</c:v>
+                  <c:v>7051</c:v>
                 </c:pt>
                 <c:pt idx="295" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8531</c:v>
+                  <c:v>7120</c:v>
                 </c:pt>
                 <c:pt idx="296" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8537</c:v>
+                  <c:v>7126</c:v>
                 </c:pt>
                 <c:pt idx="297" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8550</c:v>
+                  <c:v>7139</c:v>
                 </c:pt>
                 <c:pt idx="298" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8562</c:v>
+                  <c:v>7151</c:v>
                 </c:pt>
                 <c:pt idx="299" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8562</c:v>
+                  <c:v>7151</c:v>
                 </c:pt>
                 <c:pt idx="300" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8619</c:v>
+                  <c:v>7208</c:v>
                 </c:pt>
                 <c:pt idx="301" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8639</c:v>
+                  <c:v>7228</c:v>
                 </c:pt>
                 <c:pt idx="302" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8639</c:v>
+                  <c:v>7228</c:v>
                 </c:pt>
                 <c:pt idx="303" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8651</c:v>
+                  <c:v>7240</c:v>
                 </c:pt>
                 <c:pt idx="304" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8728</c:v>
+                  <c:v>7317</c:v>
                 </c:pt>
                 <c:pt idx="305" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8904</c:v>
+                  <c:v>7493</c:v>
                 </c:pt>
                 <c:pt idx="306" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>8971</c:v>
+                  <c:v>7560</c:v>
                 </c:pt>
                 <c:pt idx="307" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9040</c:v>
+                  <c:v>7629</c:v>
                 </c:pt>
                 <c:pt idx="308" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10652</c:v>
+                  <c:v>9241</c:v>
                 </c:pt>
                 <c:pt idx="309" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10876</c:v>
+                  <c:v>9465</c:v>
                 </c:pt>
                 <c:pt idx="310" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11103</c:v>
+                  <c:v>9692</c:v>
                 </c:pt>
                 <c:pt idx="311" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11108</c:v>
+                  <c:v>9697</c:v>
                 </c:pt>
                 <c:pt idx="312" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11162</c:v>
+                  <c:v>9751</c:v>
                 </c:pt>
                 <c:pt idx="313" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11162</c:v>
+                  <c:v>9751</c:v>
                 </c:pt>
                 <c:pt idx="314" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11303</c:v>
+                  <c:v>9892</c:v>
                 </c:pt>
                 <c:pt idx="315" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11304</c:v>
+                  <c:v>9893</c:v>
                 </c:pt>
                 <c:pt idx="316" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11360</c:v>
+                  <c:v>9949</c:v>
                 </c:pt>
                 <c:pt idx="317" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11437</c:v>
+                  <c:v>10026</c:v>
                 </c:pt>
                 <c:pt idx="318" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11518</c:v>
+                  <c:v>10107</c:v>
                 </c:pt>
                 <c:pt idx="319" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11618</c:v>
+                  <c:v>10207</c:v>
+                </c:pt>
+                <c:pt idx="320" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>10284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3220,6 +3226,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4188,6 +4197,9 @@
                 </c:pt>
                 <c:pt idx="319">
                   <c:v>9402</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>9460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5197,6 +5209,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6165,6 +6180,9 @@
                 </c:pt>
                 <c:pt idx="319">
                   <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>1117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7193,6 +7211,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8161,6 +8182,9 @@
                 </c:pt>
                 <c:pt idx="319">
                   <c:v>1106</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>1118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9552,6 +9576,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10520,6 +10547,9 @@
                 </c:pt>
                 <c:pt idx="319">
                   <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11530,6 +11560,9 @@
                 <c:pt idx="319">
                   <c:v>46004</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>46012</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12497,6 +12530,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="319">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="320">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14325,13 +14361,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q322"/>
+  <dimension ref="A1:Q323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B273" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G323" sqref="G323"/>
+      <selection pane="bottomRight" activeCell="I324" sqref="I324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25003,7 +25039,7 @@
       </c>
       <c r="H256" s="16">
         <f t="shared" ref="H256" si="421">SUM(I256:K256)-SUM(L256:N256)</f>
-        <v>7052</v>
+        <v>5641</v>
       </c>
       <c r="I256" s="5">
         <v>5467</v>
@@ -25015,13 +25051,13 @@
         <v>700</v>
       </c>
       <c r="L256">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M256">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N256">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O256">
         <v>0</v>
@@ -25052,7 +25088,7 @@
       </c>
       <c r="H257" s="16">
         <f t="shared" ref="H257" si="423">SUM(I257:K257)-SUM(L257:N257)</f>
-        <v>7060</v>
+        <v>5649</v>
       </c>
       <c r="I257" s="5">
         <v>5475</v>
@@ -25064,13 +25100,13 @@
         <v>700</v>
       </c>
       <c r="L257">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M257">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N257">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O257">
         <v>0</v>
@@ -25101,7 +25137,7 @@
       </c>
       <c r="H258" s="16">
         <f t="shared" ref="H258" si="425">SUM(I258:K258)-SUM(L258:N258)</f>
-        <v>6950</v>
+        <v>5539</v>
       </c>
       <c r="I258" s="5">
         <v>5376</v>
@@ -25113,13 +25149,13 @@
         <v>696</v>
       </c>
       <c r="L258">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M258">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N258">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O258">
         <v>0</v>
@@ -25150,7 +25186,7 @@
       </c>
       <c r="H259" s="16">
         <f t="shared" ref="H259" si="427">SUM(I259:K259)-SUM(L259:N259)</f>
-        <v>6953</v>
+        <v>5542</v>
       </c>
       <c r="I259" s="5">
         <v>5379</v>
@@ -25162,13 +25198,13 @@
         <v>696</v>
       </c>
       <c r="L259">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M259">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N259">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O259">
         <v>0</v>
@@ -25199,7 +25235,7 @@
       </c>
       <c r="H260" s="16">
         <f t="shared" ref="H260" si="429">SUM(I260:K260)-SUM(L260:N260)</f>
-        <v>6968</v>
+        <v>5557</v>
       </c>
       <c r="I260" s="5">
         <v>5392</v>
@@ -25211,13 +25247,13 @@
         <v>698</v>
       </c>
       <c r="L260">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M260">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N260">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O260">
         <v>0</v>
@@ -25248,7 +25284,7 @@
       </c>
       <c r="H261" s="16">
         <f t="shared" ref="H261" si="431">SUM(I261:K261)-SUM(L261:N261)</f>
-        <v>6665</v>
+        <v>5254</v>
       </c>
       <c r="I261" s="5">
         <v>5169</v>
@@ -25260,13 +25296,13 @@
         <v>679</v>
       </c>
       <c r="L261">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M261">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N261">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O261">
         <v>0</v>
@@ -25297,7 +25333,7 @@
       </c>
       <c r="H262" s="16">
         <f t="shared" ref="H262" si="433">SUM(I262:K262)-SUM(L262:N262)</f>
-        <v>6699</v>
+        <v>5288</v>
       </c>
       <c r="I262" s="5">
         <v>5188</v>
@@ -25309,13 +25345,13 @@
         <v>683</v>
       </c>
       <c r="L262">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M262">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N262">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O262">
         <v>0</v>
@@ -25346,7 +25382,7 @@
       </c>
       <c r="H263" s="16">
         <f t="shared" ref="H263" si="435">SUM(I263:K263)-SUM(L263:N263)</f>
-        <v>6387</v>
+        <v>4976</v>
       </c>
       <c r="I263" s="5">
         <v>4970</v>
@@ -25358,13 +25394,13 @@
         <v>648</v>
       </c>
       <c r="L263">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M263">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N263">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O263">
         <v>0</v>
@@ -25395,7 +25431,7 @@
       </c>
       <c r="H264" s="16">
         <f t="shared" ref="H264" si="437">SUM(I264:K264)-SUM(L264:N264)</f>
-        <v>6390</v>
+        <v>4979</v>
       </c>
       <c r="I264" s="5">
         <v>4980</v>
@@ -25407,13 +25443,13 @@
         <v>644</v>
       </c>
       <c r="L264">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M264">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N264">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O264">
         <v>0</v>
@@ -25444,7 +25480,7 @@
       </c>
       <c r="H265" s="16">
         <f t="shared" ref="H265" si="439">SUM(I265:K265)-SUM(L265:N265)</f>
-        <v>6362</v>
+        <v>4951</v>
       </c>
       <c r="I265" s="5">
         <v>4955</v>
@@ -25456,13 +25492,13 @@
         <v>642</v>
       </c>
       <c r="L265">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M265">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N265">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O265">
         <v>0</v>
@@ -25493,7 +25529,7 @@
       </c>
       <c r="H266" s="16">
         <f t="shared" ref="H266" si="441">SUM(I266:K266)-SUM(L266:N266)</f>
-        <v>6487</v>
+        <v>5076</v>
       </c>
       <c r="I266" s="5">
         <v>5024</v>
@@ -25505,13 +25541,13 @@
         <v>667</v>
       </c>
       <c r="L266">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M266">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N266">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O266">
         <v>0</v>
@@ -25542,7 +25578,7 @@
       </c>
       <c r="H267" s="16">
         <f t="shared" ref="H267" si="443">SUM(I267:K267)-SUM(L267:N267)</f>
-        <v>6370</v>
+        <v>4959</v>
       </c>
       <c r="I267" s="5">
         <v>4980</v>
@@ -25554,13 +25590,13 @@
         <v>664</v>
       </c>
       <c r="L267">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M267">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N267">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O267">
         <v>0</v>
@@ -25591,7 +25627,7 @@
       </c>
       <c r="H268" s="16">
         <f t="shared" ref="H268" si="445">SUM(I268:K268)-SUM(L268:N268)</f>
-        <v>6370</v>
+        <v>4959</v>
       </c>
       <c r="I268" s="5">
         <v>4980</v>
@@ -25603,13 +25639,13 @@
         <v>664</v>
       </c>
       <c r="L268">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M268">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N268">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O268">
         <v>0</v>
@@ -25640,7 +25676,7 @@
       </c>
       <c r="H269" s="16">
         <f t="shared" ref="H269" si="447">SUM(I269:K269)-SUM(L269:N269)</f>
-        <v>6365</v>
+        <v>4954</v>
       </c>
       <c r="I269" s="5">
         <v>4958</v>
@@ -25652,13 +25688,13 @@
         <v>642</v>
       </c>
       <c r="L269">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M269">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N269">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O269">
         <v>0</v>
@@ -25689,7 +25725,7 @@
       </c>
       <c r="H270" s="16">
         <f t="shared" ref="H270" si="449">SUM(I270:K270)-SUM(L270:N270)</f>
-        <v>6496</v>
+        <v>5085</v>
       </c>
       <c r="I270" s="5">
         <v>5082</v>
@@ -25701,13 +25737,13 @@
         <v>673</v>
       </c>
       <c r="L270">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M270">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N270">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O270">
         <v>0</v>
@@ -25738,7 +25774,7 @@
       </c>
       <c r="H271" s="16">
         <f t="shared" ref="H271" si="451">SUM(I271:K271)-SUM(L271:N271)</f>
-        <v>6393</v>
+        <v>4982</v>
       </c>
       <c r="I271" s="5">
         <v>5037</v>
@@ -25750,13 +25786,13 @@
         <v>652</v>
       </c>
       <c r="L271">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M271">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N271">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O271">
         <v>0</v>
@@ -25787,7 +25823,7 @@
       </c>
       <c r="H272" s="16">
         <f t="shared" ref="H272" si="453">SUM(I272:K272)-SUM(L272:N272)</f>
-        <v>6414</v>
+        <v>5003</v>
       </c>
       <c r="I272" s="5">
         <v>5069</v>
@@ -25799,13 +25835,13 @@
         <v>649</v>
       </c>
       <c r="L272">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M272">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N272">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O272">
         <v>0</v>
@@ -25836,7 +25872,7 @@
       </c>
       <c r="H273" s="16">
         <f t="shared" ref="H273" si="455">SUM(I273:K273)-SUM(L273:N273)</f>
-        <v>6434</v>
+        <v>5023</v>
       </c>
       <c r="I273" s="5">
         <v>5073</v>
@@ -25848,13 +25884,13 @@
         <v>653</v>
       </c>
       <c r="L273">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M273">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N273">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O273">
         <v>0</v>
@@ -25885,7 +25921,7 @@
       </c>
       <c r="H274" s="16">
         <f t="shared" ref="H274" si="457">SUM(I274:K274)-SUM(L274:N274)</f>
-        <v>7377</v>
+        <v>5966</v>
       </c>
       <c r="I274" s="5">
         <v>5831</v>
@@ -25897,13 +25933,13 @@
         <v>743</v>
       </c>
       <c r="L274">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M274">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N274">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O274">
         <v>9</v>
@@ -25934,7 +25970,7 @@
       </c>
       <c r="H275" s="16">
         <f t="shared" ref="H275" si="459">SUM(I275:K275)-SUM(L275:N275)</f>
-        <v>7467</v>
+        <v>6056</v>
       </c>
       <c r="I275" s="5">
         <v>5928</v>
@@ -25946,13 +25982,13 @@
         <v>737</v>
       </c>
       <c r="L275">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M275">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N275">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O275">
         <v>12</v>
@@ -25983,7 +26019,7 @@
       </c>
       <c r="H276" s="16">
         <f t="shared" ref="H276" si="461">SUM(I276:K276)-SUM(L276:N276)</f>
-        <v>7684</v>
+        <v>6273</v>
       </c>
       <c r="I276" s="5">
         <v>6120</v>
@@ -25995,13 +26031,13 @@
         <v>750</v>
       </c>
       <c r="L276">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M276">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N276">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O276">
         <v>14</v>
@@ -26032,7 +26068,7 @@
       </c>
       <c r="H277" s="16">
         <f t="shared" ref="H277" si="463">SUM(I277:K277)-SUM(L277:N277)</f>
-        <v>7773</v>
+        <v>6362</v>
       </c>
       <c r="I277" s="5">
         <v>6195</v>
@@ -26044,13 +26080,13 @@
         <v>764</v>
       </c>
       <c r="L277">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M277">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N277">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O277">
         <v>14</v>
@@ -26081,7 +26117,7 @@
       </c>
       <c r="H278" s="16">
         <f t="shared" ref="H278" si="465">SUM(I278:K278)-SUM(L278:N278)</f>
-        <v>7781</v>
+        <v>6370</v>
       </c>
       <c r="I278" s="5">
         <v>6204</v>
@@ -26093,13 +26129,13 @@
         <v>763</v>
       </c>
       <c r="L278">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M278">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N278">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O278">
         <v>14</v>
@@ -26130,7 +26166,7 @@
       </c>
       <c r="H279" s="16">
         <f t="shared" ref="H279" si="467">SUM(I279:K279)-SUM(L279:N279)</f>
-        <v>7956</v>
+        <v>6545</v>
       </c>
       <c r="I279" s="5">
         <v>6351</v>
@@ -26142,13 +26178,13 @@
         <v>777</v>
       </c>
       <c r="L279">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M279">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N279">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O279">
         <v>15</v>
@@ -26179,7 +26215,7 @@
       </c>
       <c r="H280" s="16">
         <f t="shared" ref="H280" si="469">SUM(I280:K280)-SUM(L280:N280)</f>
-        <v>7934</v>
+        <v>6523</v>
       </c>
       <c r="I280" s="5">
         <v>6336</v>
@@ -26191,13 +26227,13 @@
         <v>782</v>
       </c>
       <c r="L280">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M280">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N280">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O280">
         <v>15</v>
@@ -26228,7 +26264,7 @@
       </c>
       <c r="H281" s="16">
         <f t="shared" ref="H281" si="471">SUM(I281:K281)-SUM(L281:N281)</f>
-        <v>8037</v>
+        <v>6626</v>
       </c>
       <c r="I281" s="5">
         <v>6406</v>
@@ -26240,13 +26276,13 @@
         <v>801</v>
       </c>
       <c r="L281">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M281">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N281">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O281">
         <v>17</v>
@@ -26277,7 +26313,7 @@
       </c>
       <c r="H282" s="16">
         <f t="shared" ref="H282" si="473">SUM(I282:K282)-SUM(L282:N282)</f>
-        <v>8280</v>
+        <v>6869</v>
       </c>
       <c r="I282" s="5">
         <v>6617</v>
@@ -26289,13 +26325,13 @@
         <v>823</v>
       </c>
       <c r="L282">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M282">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N282">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O282">
         <v>19</v>
@@ -26326,7 +26362,7 @@
       </c>
       <c r="H283" s="16">
         <f t="shared" ref="H283" si="475">SUM(I283:K283)-SUM(L283:N283)</f>
-        <v>8306</v>
+        <v>6895</v>
       </c>
       <c r="I283" s="5">
         <v>6643</v>
@@ -26338,13 +26374,13 @@
         <v>823</v>
       </c>
       <c r="L283">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M283">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N283">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O283">
         <v>19</v>
@@ -26375,7 +26411,7 @@
       </c>
       <c r="H284" s="16">
         <f t="shared" ref="H284" si="477">SUM(I284:K284)-SUM(L284:N284)</f>
-        <v>8345</v>
+        <v>6934</v>
       </c>
       <c r="I284" s="5">
         <v>6677</v>
@@ -26387,13 +26423,13 @@
         <v>826</v>
       </c>
       <c r="L284">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M284">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N284">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O284">
         <v>20</v>
@@ -26424,7 +26460,7 @@
       </c>
       <c r="H285" s="16">
         <f t="shared" ref="H285:H286" si="479">SUM(I285:K285)-SUM(L285:N285)</f>
-        <v>8453</v>
+        <v>7042</v>
       </c>
       <c r="I285" s="5">
         <v>6755</v>
@@ -26436,13 +26472,13 @@
         <v>849</v>
       </c>
       <c r="L285">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M285">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N285">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O285">
         <v>22</v>
@@ -26473,7 +26509,7 @@
       </c>
       <c r="H286" s="16">
         <f t="shared" si="479"/>
-        <v>8499</v>
+        <v>7088</v>
       </c>
       <c r="I286" s="5">
         <v>6809</v>
@@ -26485,13 +26521,13 @@
         <v>845</v>
       </c>
       <c r="L286">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M286">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N286">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O286">
         <v>22</v>
@@ -26522,7 +26558,7 @@
       </c>
       <c r="H287" s="16">
         <f t="shared" ref="H287" si="481">SUM(I287:K287)-SUM(L287:N287)</f>
-        <v>8569</v>
+        <v>7158</v>
       </c>
       <c r="I287" s="5">
         <v>6865</v>
@@ -26534,13 +26570,13 @@
         <v>851</v>
       </c>
       <c r="L287">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M287">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N287">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O287">
         <v>22</v>
@@ -26571,7 +26607,7 @@
       </c>
       <c r="H288" s="16">
         <f t="shared" ref="H288" si="483">SUM(I288:K288)-SUM(L288:N288)</f>
-        <v>8559</v>
+        <v>7148</v>
       </c>
       <c r="I288" s="5">
         <v>6848</v>
@@ -26583,13 +26619,13 @@
         <v>856</v>
       </c>
       <c r="L288">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M288">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N288">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O288">
         <v>22</v>
@@ -26620,7 +26656,7 @@
       </c>
       <c r="H289" s="16">
         <f t="shared" ref="H289" si="485">SUM(I289:K289)-SUM(L289:N289)</f>
-        <v>8561</v>
+        <v>7150</v>
       </c>
       <c r="I289" s="5">
         <v>6850</v>
@@ -26632,13 +26668,13 @@
         <v>856</v>
       </c>
       <c r="L289">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M289">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N289">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O289">
         <v>22</v>
@@ -26669,7 +26705,7 @@
       </c>
       <c r="H290" s="16">
         <f t="shared" ref="H290" si="487">SUM(I290:K290)-SUM(L290:N290)</f>
-        <v>8080</v>
+        <v>6669</v>
       </c>
       <c r="I290" s="5">
         <v>6442</v>
@@ -26681,13 +26717,13 @@
         <v>829</v>
       </c>
       <c r="L290">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M290">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N290">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O290">
         <v>23</v>
@@ -26718,7 +26754,7 @@
       </c>
       <c r="H291" s="16">
         <f t="shared" ref="H291" si="489">SUM(I291:K291)-SUM(L291:N291)</f>
-        <v>8129</v>
+        <v>6718</v>
       </c>
       <c r="I291" s="5">
         <v>6491</v>
@@ -26730,13 +26766,13 @@
         <v>829</v>
       </c>
       <c r="L291">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M291">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N291">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O291">
         <v>23</v>
@@ -26767,7 +26803,7 @@
       </c>
       <c r="H292" s="16">
         <f t="shared" ref="H292" si="491">SUM(I292:K292)-SUM(L292:N292)</f>
-        <v>8159</v>
+        <v>6748</v>
       </c>
       <c r="I292" s="5">
         <v>6486</v>
@@ -26779,13 +26815,13 @@
         <v>844</v>
       </c>
       <c r="L292">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M292">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N292">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O292">
         <v>23</v>
@@ -26816,7 +26852,7 @@
       </c>
       <c r="H293" s="16">
         <f t="shared" ref="H293" si="493">SUM(I293:K293)-SUM(L293:N293)</f>
-        <v>8269</v>
+        <v>6858</v>
       </c>
       <c r="I293" s="5">
         <v>6564</v>
@@ -26828,13 +26864,13 @@
         <v>863</v>
       </c>
       <c r="L293">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M293">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N293">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O293">
         <v>23</v>
@@ -26865,7 +26901,7 @@
       </c>
       <c r="H294" s="16">
         <f t="shared" ref="H294" si="495">SUM(I294:K294)-SUM(L294:N294)</f>
-        <v>8646</v>
+        <v>7235</v>
       </c>
       <c r="I294" s="5">
         <v>6894</v>
@@ -26877,13 +26913,13 @@
         <v>890</v>
       </c>
       <c r="L294">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M294">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N294">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O294">
         <v>23</v>
@@ -26914,7 +26950,7 @@
       </c>
       <c r="H295" s="16">
         <f t="shared" ref="H295" si="497">SUM(I295:K295)-SUM(L295:N295)</f>
-        <v>8324</v>
+        <v>6913</v>
       </c>
       <c r="I295" s="5">
         <v>6555</v>
@@ -26926,13 +26962,13 @@
         <v>913</v>
       </c>
       <c r="L295">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M295">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N295">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O295">
         <v>23</v>
@@ -26963,7 +26999,7 @@
       </c>
       <c r="H296" s="16">
         <f t="shared" ref="H296" si="499">SUM(I296:K296)-SUM(L296:N296)</f>
-        <v>8437</v>
+        <v>7026</v>
       </c>
       <c r="I296" s="5">
         <v>6645</v>
@@ -26975,13 +27011,13 @@
         <v>924</v>
       </c>
       <c r="L296">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M296">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N296">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O296">
         <v>23</v>
@@ -27012,7 +27048,7 @@
       </c>
       <c r="H297" s="16">
         <f t="shared" ref="H297" si="501">SUM(I297:K297)-SUM(L297:N297)</f>
-        <v>8462</v>
+        <v>7051</v>
       </c>
       <c r="I297" s="5">
         <v>6664</v>
@@ -27024,13 +27060,13 @@
         <v>929</v>
       </c>
       <c r="L297">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M297">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N297">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O297">
         <v>23</v>
@@ -27061,7 +27097,7 @@
       </c>
       <c r="H298" s="16">
         <f t="shared" ref="H298" si="503">SUM(I298:K298)-SUM(L298:N298)</f>
-        <v>8531</v>
+        <v>7120</v>
       </c>
       <c r="I298" s="5">
         <v>6711</v>
@@ -27073,13 +27109,13 @@
         <v>941</v>
       </c>
       <c r="L298">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M298">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N298">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O298">
         <v>23</v>
@@ -27110,7 +27146,7 @@
       </c>
       <c r="H299" s="16">
         <f t="shared" ref="H299" si="505">SUM(I299:K299)-SUM(L299:N299)</f>
-        <v>8537</v>
+        <v>7126</v>
       </c>
       <c r="I299" s="5">
         <v>6708</v>
@@ -27122,13 +27158,13 @@
         <v>946</v>
       </c>
       <c r="L299">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M299">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N299">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O299">
         <v>23</v>
@@ -27159,7 +27195,7 @@
       </c>
       <c r="H300" s="16">
         <f t="shared" ref="H300" si="507">SUM(I300:K300)-SUM(L300:N300)</f>
-        <v>8550</v>
+        <v>7139</v>
       </c>
       <c r="I300" s="5">
         <v>6718</v>
@@ -27171,13 +27207,13 @@
         <v>948</v>
       </c>
       <c r="L300">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M300">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N300">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O300">
         <v>23</v>
@@ -27208,7 +27244,7 @@
       </c>
       <c r="H301" s="16">
         <f t="shared" ref="H301" si="509">SUM(I301:K301)-SUM(L301:N301)</f>
-        <v>8562</v>
+        <v>7151</v>
       </c>
       <c r="I301" s="5">
         <v>6707</v>
@@ -27220,13 +27256,13 @@
         <v>948</v>
       </c>
       <c r="L301">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M301">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N301">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O301">
         <v>23</v>
@@ -27257,7 +27293,7 @@
       </c>
       <c r="H302" s="16">
         <f t="shared" ref="H302" si="511">SUM(I302:K302)-SUM(L302:N302)</f>
-        <v>8562</v>
+        <v>7151</v>
       </c>
       <c r="I302" s="5">
         <v>6727</v>
@@ -27269,13 +27305,13 @@
         <v>951</v>
       </c>
       <c r="L302">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M302">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N302">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O302">
         <v>23</v>
@@ -27306,7 +27342,7 @@
       </c>
       <c r="H303" s="16">
         <f t="shared" ref="H303" si="513">SUM(I303:K303)-SUM(L303:N303)</f>
-        <v>8619</v>
+        <v>7208</v>
       </c>
       <c r="I303" s="5">
         <v>6764</v>
@@ -27318,13 +27354,13 @@
         <v>962</v>
       </c>
       <c r="L303">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M303">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N303">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O303">
         <v>23</v>
@@ -27355,7 +27391,7 @@
       </c>
       <c r="H304" s="16">
         <f t="shared" ref="H304" si="515">SUM(I304:K304)-SUM(L304:N304)</f>
-        <v>8639</v>
+        <v>7228</v>
       </c>
       <c r="I304" s="5">
         <v>6781</v>
@@ -27367,13 +27403,13 @@
         <v>964</v>
       </c>
       <c r="L304">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M304">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N304">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O304">
         <v>23</v>
@@ -27404,7 +27440,7 @@
       </c>
       <c r="H305" s="16">
         <f t="shared" ref="H305" si="517">SUM(I305:K305)-SUM(L305:N305)</f>
-        <v>8639</v>
+        <v>7228</v>
       </c>
       <c r="I305" s="5">
         <v>6781</v>
@@ -27416,13 +27452,13 @@
         <v>964</v>
       </c>
       <c r="L305">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M305">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N305">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O305">
         <v>23</v>
@@ -27453,7 +27489,7 @@
       </c>
       <c r="H306" s="16">
         <f t="shared" ref="H306" si="519">SUM(I306:K306)-SUM(L306:N306)</f>
-        <v>8651</v>
+        <v>7240</v>
       </c>
       <c r="I306" s="5">
         <v>6791</v>
@@ -27465,13 +27501,13 @@
         <v>967</v>
       </c>
       <c r="L306">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M306">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N306">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O306">
         <v>23</v>
@@ -27502,7 +27538,7 @@
       </c>
       <c r="H307" s="16">
         <f t="shared" ref="H307" si="521">SUM(I307:K307)-SUM(L307:N307)</f>
-        <v>8728</v>
+        <v>7317</v>
       </c>
       <c r="I307" s="5">
         <v>6859</v>
@@ -27514,13 +27550,13 @@
         <v>973</v>
       </c>
       <c r="L307">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M307">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N307">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O307">
         <v>23</v>
@@ -27551,7 +27587,7 @@
       </c>
       <c r="H308" s="16">
         <f t="shared" ref="H308" si="523">SUM(I308:K308)-SUM(L308:N308)</f>
-        <v>8904</v>
+        <v>7493</v>
       </c>
       <c r="I308" s="5">
         <v>6959</v>
@@ -27563,13 +27599,13 @@
         <v>968</v>
       </c>
       <c r="L308">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M308">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N308">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O308">
         <v>23</v>
@@ -27600,7 +27636,7 @@
       </c>
       <c r="H309" s="16">
         <f t="shared" ref="H309" si="525">SUM(I309:K309)-SUM(L309:N309)</f>
-        <v>8971</v>
+        <v>7560</v>
       </c>
       <c r="I309" s="5">
         <v>7046</v>
@@ -27612,13 +27648,13 @@
         <v>986</v>
       </c>
       <c r="L309">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M309">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N309">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O309">
         <v>24</v>
@@ -27649,7 +27685,7 @@
       </c>
       <c r="H310" s="16">
         <f t="shared" ref="H310" si="527">SUM(I310:K310)-SUM(L310:N310)</f>
-        <v>9040</v>
+        <v>7629</v>
       </c>
       <c r="I310" s="5">
         <v>7177</v>
@@ -27661,13 +27697,13 @@
         <v>958</v>
       </c>
       <c r="L310">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M310">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N310">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O310">
         <v>24</v>
@@ -27698,7 +27734,7 @@
       </c>
       <c r="H311" s="16">
         <f t="shared" ref="H311" si="529">SUM(I311:K311)-SUM(L311:N311)</f>
-        <v>10652</v>
+        <v>9241</v>
       </c>
       <c r="I311" s="5">
         <v>8630</v>
@@ -27710,13 +27746,13 @@
         <v>1043</v>
       </c>
       <c r="L311">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M311">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N311">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O311">
         <v>24</v>
@@ -27747,7 +27783,7 @@
       </c>
       <c r="H312" s="16">
         <f t="shared" ref="H312" si="531">SUM(I312:K312)-SUM(L312:N312)</f>
-        <v>10876</v>
+        <v>9465</v>
       </c>
       <c r="I312" s="5">
         <v>8833</v>
@@ -27759,13 +27795,13 @@
         <v>1056</v>
       </c>
       <c r="L312">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M312">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N312">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O312">
         <v>31</v>
@@ -27796,7 +27832,7 @@
       </c>
       <c r="H313" s="16">
         <f t="shared" ref="H313" si="533">SUM(I313:K313)-SUM(L313:N313)</f>
-        <v>11103</v>
+        <v>9692</v>
       </c>
       <c r="I313" s="5">
         <v>9036</v>
@@ -27808,13 +27844,13 @@
         <v>1068</v>
       </c>
       <c r="L313">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M313">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N313">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O313">
         <v>31</v>
@@ -27845,7 +27881,7 @@
       </c>
       <c r="H314" s="16">
         <f t="shared" ref="H314" si="535">SUM(I314:K314)-SUM(L314:N314)</f>
-        <v>11108</v>
+        <v>9697</v>
       </c>
       <c r="I314" s="5">
         <v>9039</v>
@@ -27857,13 +27893,13 @@
         <v>1069</v>
       </c>
       <c r="L314">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M314">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N314">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O314">
         <v>31</v>
@@ -27894,7 +27930,7 @@
       </c>
       <c r="H315" s="16">
         <f t="shared" ref="H315" si="537">SUM(I315:K315)-SUM(L315:N315)</f>
-        <v>11162</v>
+        <v>9751</v>
       </c>
       <c r="I315" s="5">
         <v>9132</v>
@@ -27906,13 +27942,13 @@
         <v>1033</v>
       </c>
       <c r="L315">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M315">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N315">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O315">
         <v>31</v>
@@ -27943,7 +27979,7 @@
       </c>
       <c r="H316" s="16">
         <f t="shared" ref="H316" si="539">SUM(I316:K316)-SUM(L316:N316)</f>
-        <v>11162</v>
+        <v>9751</v>
       </c>
       <c r="I316" s="5">
         <v>9132</v>
@@ -27955,13 +27991,13 @@
         <v>1033</v>
       </c>
       <c r="L316">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M316">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N316">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O316">
         <v>31</v>
@@ -27992,7 +28028,7 @@
       </c>
       <c r="H317" s="16">
         <f t="shared" ref="H317" si="541">SUM(I317:K317)-SUM(L317:N317)</f>
-        <v>11303</v>
+        <v>9892</v>
       </c>
       <c r="I317" s="5">
         <v>9236</v>
@@ -28004,13 +28040,13 @@
         <v>1056</v>
       </c>
       <c r="L317">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M317">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N317">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O317">
         <v>31</v>
@@ -28041,7 +28077,7 @@
       </c>
       <c r="H318" s="16">
         <f t="shared" ref="H318" si="543">SUM(I318:K318)-SUM(L318:N318)</f>
-        <v>11304</v>
+        <v>9893</v>
       </c>
       <c r="I318" s="5">
         <v>9232</v>
@@ -28053,13 +28089,13 @@
         <v>1060</v>
       </c>
       <c r="L318">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M318">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N318">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O318">
         <v>31</v>
@@ -28090,7 +28126,7 @@
       </c>
       <c r="H319" s="16">
         <f t="shared" ref="H319" si="545">SUM(I319:K319)-SUM(L319:N319)</f>
-        <v>11360</v>
+        <v>9949</v>
       </c>
       <c r="I319" s="5">
         <v>9263</v>
@@ -28102,13 +28138,13 @@
         <v>1065</v>
       </c>
       <c r="L319">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M319">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N319">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O319">
         <v>31</v>
@@ -28139,7 +28175,7 @@
       </c>
       <c r="H320" s="16">
         <f t="shared" ref="H320" si="547">SUM(I320:K320)-SUM(L320:N320)</f>
-        <v>11437</v>
+        <v>10026</v>
       </c>
       <c r="I320" s="5">
         <v>9315</v>
@@ -28151,13 +28187,13 @@
         <v>1071</v>
       </c>
       <c r="L320">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M320">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N320">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O320">
         <v>31</v>
@@ -28188,7 +28224,7 @@
       </c>
       <c r="H321" s="16">
         <f t="shared" ref="H321" si="549">SUM(I321:K321)-SUM(L321:N321)</f>
-        <v>11518</v>
+        <v>10107</v>
       </c>
       <c r="I321" s="5">
         <v>9340</v>
@@ -28200,13 +28236,13 @@
         <v>1096</v>
       </c>
       <c r="L321">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M321">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N321">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O321">
         <v>31</v>
@@ -28237,7 +28273,7 @@
       </c>
       <c r="H322" s="16">
         <f t="shared" ref="H322" si="551">SUM(I322:K322)-SUM(L322:N322)</f>
-        <v>11618</v>
+        <v>10207</v>
       </c>
       <c r="I322" s="5">
         <v>9402</v>
@@ -28249,15 +28285,64 @@
         <v>1106</v>
       </c>
       <c r="L322">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="M322">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N322">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O322">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>46012</v>
+      </c>
+      <c r="B323" s="2">
+        <v>9</v>
+      </c>
+      <c r="C323">
+        <f t="shared" ref="C323" si="552">SUM(D323:F323)</f>
+        <v>1673</v>
+      </c>
+      <c r="D323">
+        <v>1105</v>
+      </c>
+      <c r="E323">
+        <v>371</v>
+      </c>
+      <c r="F323" s="3">
+        <v>197</v>
+      </c>
+      <c r="G323" s="4">
+        <v>109</v>
+      </c>
+      <c r="H323" s="16">
+        <f t="shared" ref="H323" si="553">SUM(I323:K323)-SUM(L323:N323)</f>
+        <v>10284</v>
+      </c>
+      <c r="I323" s="5">
+        <v>9460</v>
+      </c>
+      <c r="J323" s="6">
+        <v>1117</v>
+      </c>
+      <c r="K323" s="7">
+        <v>1118</v>
+      </c>
+      <c r="L323">
+        <v>1305</v>
+      </c>
+      <c r="M323">
+        <v>86</v>
+      </c>
+      <c r="N323">
+        <v>20</v>
+      </c>
+      <c r="O323">
         <v>31</v>
       </c>
     </row>
@@ -28280,7 +28365,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Minimized search bar in Who's Who screen.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A3C1D-575B-F045-9C61-F134E06A5212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8BA193-5E4E-594F-8B33-F4B3717321D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1248,6 +1248,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2219,6 +2225,12 @@
                 </c:pt>
                 <c:pt idx="320" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>10284</c:v>
+                </c:pt>
+                <c:pt idx="321" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>10590</c:v>
+                </c:pt>
+                <c:pt idx="322" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>-1411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3229,6 +3241,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4200,6 +4218,9 @@
                 </c:pt>
                 <c:pt idx="320">
                   <c:v>9460</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>9701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5212,6 +5233,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6183,6 +6210,9 @@
                 </c:pt>
                 <c:pt idx="320">
                   <c:v>1117</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>1150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7214,6 +7244,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8185,6 +8221,9 @@
                 </c:pt>
                 <c:pt idx="320">
                   <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>1150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9579,6 +9618,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10550,6 +10595,12 @@
                 </c:pt>
                 <c:pt idx="320">
                   <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11563,6 +11614,12 @@
                 <c:pt idx="320">
                   <c:v>46012</c:v>
                 </c:pt>
+                <c:pt idx="321">
+                  <c:v>46015</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>46016</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12533,6 +12590,12 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="320">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="322">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14361,13 +14424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q323"/>
+  <dimension ref="A1:Q325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B273" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B316" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I324" sqref="I324"/>
+      <selection pane="bottomRight" activeCell="K329" sqref="K329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28346,6 +28409,95 @@
         <v>31</v>
       </c>
     </row>
+    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>46015</v>
+      </c>
+      <c r="B324" s="2">
+        <v>9</v>
+      </c>
+      <c r="C324">
+        <f t="shared" ref="C324" si="554">SUM(D324:F324)</f>
+        <v>1673</v>
+      </c>
+      <c r="D324">
+        <v>1105</v>
+      </c>
+      <c r="E324">
+        <v>371</v>
+      </c>
+      <c r="F324" s="3">
+        <v>197</v>
+      </c>
+      <c r="G324" s="4">
+        <v>111</v>
+      </c>
+      <c r="H324" s="16">
+        <f t="shared" ref="H324" si="555">SUM(I324:K324)-SUM(L324:N324)</f>
+        <v>10590</v>
+      </c>
+      <c r="I324" s="5">
+        <v>9701</v>
+      </c>
+      <c r="J324" s="6">
+        <v>1150</v>
+      </c>
+      <c r="K324" s="7">
+        <v>1150</v>
+      </c>
+      <c r="L324">
+        <v>1305</v>
+      </c>
+      <c r="M324">
+        <v>86</v>
+      </c>
+      <c r="N324">
+        <v>20</v>
+      </c>
+      <c r="O324">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>46016</v>
+      </c>
+      <c r="B325" s="2">
+        <v>9</v>
+      </c>
+      <c r="C325">
+        <f t="shared" ref="C325" si="556">SUM(D325:F325)</f>
+        <v>1673</v>
+      </c>
+      <c r="D325">
+        <v>1105</v>
+      </c>
+      <c r="E325">
+        <v>371</v>
+      </c>
+      <c r="F325" s="3">
+        <v>197</v>
+      </c>
+      <c r="G325" s="4">
+        <v>112</v>
+      </c>
+      <c r="H325" s="16">
+        <f t="shared" ref="H325" si="557">SUM(I325:K325)-SUM(L325:N325)</f>
+        <v>-1411</v>
+      </c>
+      <c r="L325">
+        <v>1305</v>
+      </c>
+      <c r="M325">
+        <v>86</v>
+      </c>
+      <c r="N325">
+        <v>20</v>
+      </c>
+      <c r="O325">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -28364,7 +28516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minimized search bar on Portfolios screen
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8BA193-5E4E-594F-8B33-F4B3717321D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCD92F7-7778-3B4E-9BD0-5402F3D57B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -2230,7 +2230,7 @@
                   <c:v>10590</c:v>
                 </c:pt>
                 <c:pt idx="322" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>-1411</c:v>
+                  <c:v>10849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4221,6 +4221,9 @@
                 </c:pt>
                 <c:pt idx="321">
                   <c:v>9701</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>9942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6213,6 +6216,9 @@
                 </c:pt>
                 <c:pt idx="321">
                   <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>1160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8224,6 +8230,9 @@
                 </c:pt>
                 <c:pt idx="321">
                   <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>1158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14430,7 +14439,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B316" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K329" sqref="K329"/>
+      <selection pane="bottomRight" activeCell="I326" sqref="I326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28483,7 +28492,16 @@
       </c>
       <c r="H325" s="16">
         <f t="shared" ref="H325" si="557">SUM(I325:K325)-SUM(L325:N325)</f>
-        <v>-1411</v>
+        <v>10849</v>
+      </c>
+      <c r="I325" s="5">
+        <v>9942</v>
+      </c>
+      <c r="J325" s="6">
+        <v>1160</v>
+      </c>
+      <c r="K325" s="7">
+        <v>1158</v>
       </c>
       <c r="L325">
         <v>1305</v>
@@ -28516,7 +28534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
       <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Line count fix. Size of SwiftJson.swift shouldn't be subtracted from line count anymore.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864C83F1-02B3-5146-B3FB-535BB2FD9362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F63E3CB-8A18-E54D-853C-0F92329A926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +113,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,11 +149,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -196,8 +203,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1260,6 +1269,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2029,220 +2041,223 @@
                   <c:v>7047</c:v>
                 </c:pt>
                 <c:pt idx="253" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5641</c:v>
+                  <c:v>7052</c:v>
                 </c:pt>
                 <c:pt idx="254" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5649</c:v>
+                  <c:v>7060</c:v>
                 </c:pt>
                 <c:pt idx="255" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5539</c:v>
+                  <c:v>6950</c:v>
                 </c:pt>
                 <c:pt idx="256" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5542</c:v>
+                  <c:v>6953</c:v>
                 </c:pt>
                 <c:pt idx="257" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5557</c:v>
+                  <c:v>6968</c:v>
                 </c:pt>
                 <c:pt idx="258" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5254</c:v>
+                  <c:v>6665</c:v>
                 </c:pt>
                 <c:pt idx="259" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5288</c:v>
+                  <c:v>6699</c:v>
                 </c:pt>
                 <c:pt idx="260" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4976</c:v>
+                  <c:v>6387</c:v>
                 </c:pt>
                 <c:pt idx="261" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4979</c:v>
+                  <c:v>6390</c:v>
                 </c:pt>
                 <c:pt idx="262" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4951</c:v>
+                  <c:v>6362</c:v>
                 </c:pt>
                 <c:pt idx="263" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5076</c:v>
+                  <c:v>6487</c:v>
                 </c:pt>
                 <c:pt idx="264" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4959</c:v>
+                  <c:v>6370</c:v>
                 </c:pt>
                 <c:pt idx="265" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4959</c:v>
+                  <c:v>6370</c:v>
                 </c:pt>
                 <c:pt idx="266" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4954</c:v>
+                  <c:v>6365</c:v>
                 </c:pt>
                 <c:pt idx="267" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5085</c:v>
+                  <c:v>6496</c:v>
                 </c:pt>
                 <c:pt idx="268" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>4982</c:v>
+                  <c:v>6393</c:v>
                 </c:pt>
                 <c:pt idx="269" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5003</c:v>
+                  <c:v>6414</c:v>
                 </c:pt>
                 <c:pt idx="270" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5023</c:v>
+                  <c:v>6434</c:v>
                 </c:pt>
                 <c:pt idx="271" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>5966</c:v>
+                  <c:v>7377</c:v>
                 </c:pt>
                 <c:pt idx="272" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6056</c:v>
+                  <c:v>7467</c:v>
                 </c:pt>
                 <c:pt idx="273" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6273</c:v>
+                  <c:v>7684</c:v>
                 </c:pt>
                 <c:pt idx="274" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6362</c:v>
+                  <c:v>7773</c:v>
                 </c:pt>
                 <c:pt idx="275" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6370</c:v>
+                  <c:v>7781</c:v>
                 </c:pt>
                 <c:pt idx="276" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6545</c:v>
+                  <c:v>7956</c:v>
                 </c:pt>
                 <c:pt idx="277" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6523</c:v>
+                  <c:v>7934</c:v>
                 </c:pt>
                 <c:pt idx="278" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6626</c:v>
+                  <c:v>8037</c:v>
                 </c:pt>
                 <c:pt idx="279" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6869</c:v>
+                  <c:v>8280</c:v>
                 </c:pt>
                 <c:pt idx="280" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6895</c:v>
+                  <c:v>8306</c:v>
                 </c:pt>
                 <c:pt idx="281" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6934</c:v>
+                  <c:v>8345</c:v>
                 </c:pt>
                 <c:pt idx="282" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7042</c:v>
+                  <c:v>8453</c:v>
                 </c:pt>
                 <c:pt idx="283" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7088</c:v>
+                  <c:v>8499</c:v>
                 </c:pt>
                 <c:pt idx="284" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7158</c:v>
+                  <c:v>8569</c:v>
                 </c:pt>
                 <c:pt idx="285" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7148</c:v>
+                  <c:v>8559</c:v>
                 </c:pt>
                 <c:pt idx="286" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7150</c:v>
+                  <c:v>8561</c:v>
                 </c:pt>
                 <c:pt idx="287" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6669</c:v>
+                  <c:v>8080</c:v>
                 </c:pt>
                 <c:pt idx="288" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6718</c:v>
+                  <c:v>8129</c:v>
                 </c:pt>
                 <c:pt idx="289" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6748</c:v>
+                  <c:v>8159</c:v>
                 </c:pt>
                 <c:pt idx="290" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6858</c:v>
+                  <c:v>8269</c:v>
                 </c:pt>
                 <c:pt idx="291" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7235</c:v>
+                  <c:v>8646</c:v>
                 </c:pt>
                 <c:pt idx="292" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>6913</c:v>
+                  <c:v>8324</c:v>
                 </c:pt>
                 <c:pt idx="293" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7026</c:v>
+                  <c:v>8437</c:v>
                 </c:pt>
                 <c:pt idx="294" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7051</c:v>
+                  <c:v>8462</c:v>
                 </c:pt>
                 <c:pt idx="295" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7120</c:v>
+                  <c:v>8531</c:v>
                 </c:pt>
                 <c:pt idx="296" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7126</c:v>
+                  <c:v>8537</c:v>
                 </c:pt>
                 <c:pt idx="297" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7139</c:v>
+                  <c:v>8550</c:v>
                 </c:pt>
                 <c:pt idx="298" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7151</c:v>
+                  <c:v>8562</c:v>
                 </c:pt>
                 <c:pt idx="299" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7151</c:v>
+                  <c:v>8562</c:v>
                 </c:pt>
                 <c:pt idx="300" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7208</c:v>
+                  <c:v>8619</c:v>
                 </c:pt>
                 <c:pt idx="301" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7228</c:v>
+                  <c:v>8639</c:v>
                 </c:pt>
                 <c:pt idx="302" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7228</c:v>
+                  <c:v>8639</c:v>
                 </c:pt>
                 <c:pt idx="303" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7240</c:v>
+                  <c:v>8651</c:v>
                 </c:pt>
                 <c:pt idx="304" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7317</c:v>
+                  <c:v>8728</c:v>
                 </c:pt>
                 <c:pt idx="305" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7493</c:v>
+                  <c:v>8904</c:v>
                 </c:pt>
                 <c:pt idx="306" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7560</c:v>
+                  <c:v>8971</c:v>
                 </c:pt>
                 <c:pt idx="307" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>7629</c:v>
+                  <c:v>9040</c:v>
                 </c:pt>
                 <c:pt idx="308" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9241</c:v>
+                  <c:v>10652</c:v>
                 </c:pt>
                 <c:pt idx="309" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9465</c:v>
+                  <c:v>10876</c:v>
                 </c:pt>
                 <c:pt idx="310" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9692</c:v>
+                  <c:v>11103</c:v>
                 </c:pt>
                 <c:pt idx="311" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9697</c:v>
+                  <c:v>11108</c:v>
                 </c:pt>
                 <c:pt idx="312" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9751</c:v>
+                  <c:v>11162</c:v>
                 </c:pt>
                 <c:pt idx="313" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9751</c:v>
+                  <c:v>11162</c:v>
                 </c:pt>
                 <c:pt idx="314" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9892</c:v>
+                  <c:v>11303</c:v>
                 </c:pt>
                 <c:pt idx="315" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9893</c:v>
+                  <c:v>11304</c:v>
                 </c:pt>
                 <c:pt idx="316" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>9949</c:v>
+                  <c:v>11360</c:v>
                 </c:pt>
                 <c:pt idx="317" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10026</c:v>
+                  <c:v>11437</c:v>
                 </c:pt>
                 <c:pt idx="318" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10107</c:v>
+                  <c:v>11518</c:v>
                 </c:pt>
                 <c:pt idx="319" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10207</c:v>
+                  <c:v>11618</c:v>
                 </c:pt>
                 <c:pt idx="320" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10284</c:v>
+                  <c:v>11695</c:v>
                 </c:pt>
                 <c:pt idx="321" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10590</c:v>
+                  <c:v>12001</c:v>
                 </c:pt>
                 <c:pt idx="322" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10849</c:v>
+                  <c:v>12260</c:v>
                 </c:pt>
                 <c:pt idx="323" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>10923</c:v>
+                  <c:v>12334</c:v>
                 </c:pt>
                 <c:pt idx="324" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>11041</c:v>
+                  <c:v>12452</c:v>
+                </c:pt>
+                <c:pt idx="325" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3265,6 +3280,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4248,6 +4266,9 @@
                 </c:pt>
                 <c:pt idx="324">
                   <c:v>10069</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>10054</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5272,6 +5293,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6255,6 +6279,9 @@
                 </c:pt>
                 <c:pt idx="324">
                   <c:v>1209</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>1214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7298,6 +7325,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8281,6 +8311,9 @@
                 </c:pt>
                 <c:pt idx="324">
                   <c:v>1174</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>1177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8373,7 +8406,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12000"/>
+          <c:max val="13000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -9687,6 +9720,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10670,6 +10706,9 @@
                 </c:pt>
                 <c:pt idx="324">
                   <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11695,6 +11734,9 @@
                 <c:pt idx="324">
                   <c:v>46025</c:v>
                 </c:pt>
+                <c:pt idx="325">
+                  <c:v>46025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12677,6 +12719,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="324">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="325">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14505,13 +14550,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q327"/>
+  <dimension ref="A1:Q328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B296" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q324" sqref="Q324"/>
+      <selection pane="bottomRight" activeCell="J332" sqref="J332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25182,8 +25227,8 @@
         <v>78</v>
       </c>
       <c r="H256" s="16">
-        <f t="shared" ref="H256" si="421">SUM(I256:K256)-SUM(L256:N256)</f>
-        <v>5641</v>
+        <f>SUM(I256:K256)</f>
+        <v>7052</v>
       </c>
       <c r="I256" s="5">
         <v>5467</v>
@@ -25194,15 +25239,9 @@
       <c r="K256" s="7">
         <v>700</v>
       </c>
-      <c r="L256">
-        <v>1305</v>
-      </c>
-      <c r="M256">
-        <v>86</v>
-      </c>
-      <c r="N256">
-        <v>20</v>
-      </c>
+      <c r="L256" s="22"/>
+      <c r="M256" s="22"/>
+      <c r="N256" s="22"/>
       <c r="O256">
         <v>0</v>
       </c>
@@ -25215,7 +25254,7 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <f t="shared" ref="C257" si="422">SUM(D257:F257)</f>
+        <f t="shared" ref="C257" si="421">SUM(D257:F257)</f>
         <v>1673</v>
       </c>
       <c r="D257">
@@ -25231,8 +25270,8 @@
         <v>78</v>
       </c>
       <c r="H257" s="16">
-        <f t="shared" ref="H257" si="423">SUM(I257:K257)-SUM(L257:N257)</f>
-        <v>5649</v>
+        <f t="shared" ref="H257:H320" si="422">SUM(I257:K257)</f>
+        <v>7060</v>
       </c>
       <c r="I257" s="5">
         <v>5475</v>
@@ -25243,15 +25282,9 @@
       <c r="K257" s="7">
         <v>700</v>
       </c>
-      <c r="L257">
-        <v>1305</v>
-      </c>
-      <c r="M257">
-        <v>86</v>
-      </c>
-      <c r="N257">
-        <v>20</v>
-      </c>
+      <c r="L257" s="22"/>
+      <c r="M257" s="22"/>
+      <c r="N257" s="22"/>
       <c r="O257">
         <v>0</v>
       </c>
@@ -25264,7 +25297,7 @@
         <v>9</v>
       </c>
       <c r="C258">
-        <f t="shared" ref="C258" si="424">SUM(D258:F258)</f>
+        <f t="shared" ref="C258" si="423">SUM(D258:F258)</f>
         <v>1673</v>
       </c>
       <c r="D258">
@@ -25280,8 +25313,8 @@
         <v>77</v>
       </c>
       <c r="H258" s="16">
-        <f t="shared" ref="H258" si="425">SUM(I258:K258)-SUM(L258:N258)</f>
-        <v>5539</v>
+        <f t="shared" si="422"/>
+        <v>6950</v>
       </c>
       <c r="I258" s="5">
         <v>5376</v>
@@ -25292,15 +25325,9 @@
       <c r="K258" s="7">
         <v>696</v>
       </c>
-      <c r="L258">
-        <v>1305</v>
-      </c>
-      <c r="M258">
-        <v>86</v>
-      </c>
-      <c r="N258">
-        <v>20</v>
-      </c>
+      <c r="L258" s="22"/>
+      <c r="M258" s="22"/>
+      <c r="N258" s="22"/>
       <c r="O258">
         <v>0</v>
       </c>
@@ -25313,7 +25340,7 @@
         <v>9</v>
       </c>
       <c r="C259">
-        <f t="shared" ref="C259" si="426">SUM(D259:F259)</f>
+        <f t="shared" ref="C259" si="424">SUM(D259:F259)</f>
         <v>1673</v>
       </c>
       <c r="D259">
@@ -25329,8 +25356,8 @@
         <v>77</v>
       </c>
       <c r="H259" s="16">
-        <f t="shared" ref="H259" si="427">SUM(I259:K259)-SUM(L259:N259)</f>
-        <v>5542</v>
+        <f t="shared" si="422"/>
+        <v>6953</v>
       </c>
       <c r="I259" s="5">
         <v>5379</v>
@@ -25341,15 +25368,9 @@
       <c r="K259" s="7">
         <v>696</v>
       </c>
-      <c r="L259">
-        <v>1305</v>
-      </c>
-      <c r="M259">
-        <v>86</v>
-      </c>
-      <c r="N259">
-        <v>20</v>
-      </c>
+      <c r="L259" s="22"/>
+      <c r="M259" s="22"/>
+      <c r="N259" s="22"/>
       <c r="O259">
         <v>0</v>
       </c>
@@ -25362,7 +25383,7 @@
         <v>9</v>
       </c>
       <c r="C260">
-        <f t="shared" ref="C260" si="428">SUM(D260:F260)</f>
+        <f t="shared" ref="C260" si="425">SUM(D260:F260)</f>
         <v>1673</v>
       </c>
       <c r="D260">
@@ -25378,8 +25399,8 @@
         <v>77</v>
       </c>
       <c r="H260" s="16">
-        <f t="shared" ref="H260" si="429">SUM(I260:K260)-SUM(L260:N260)</f>
-        <v>5557</v>
+        <f t="shared" si="422"/>
+        <v>6968</v>
       </c>
       <c r="I260" s="5">
         <v>5392</v>
@@ -25390,15 +25411,9 @@
       <c r="K260" s="7">
         <v>698</v>
       </c>
-      <c r="L260">
-        <v>1305</v>
-      </c>
-      <c r="M260">
-        <v>86</v>
-      </c>
-      <c r="N260">
-        <v>20</v>
-      </c>
+      <c r="L260" s="22"/>
+      <c r="M260" s="22"/>
+      <c r="N260" s="22"/>
       <c r="O260">
         <v>0</v>
       </c>
@@ -25411,7 +25426,7 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <f t="shared" ref="C261" si="430">SUM(D261:F261)</f>
+        <f t="shared" ref="C261" si="426">SUM(D261:F261)</f>
         <v>1673</v>
       </c>
       <c r="D261">
@@ -25427,8 +25442,8 @@
         <v>75</v>
       </c>
       <c r="H261" s="16">
-        <f t="shared" ref="H261" si="431">SUM(I261:K261)-SUM(L261:N261)</f>
-        <v>5254</v>
+        <f t="shared" si="422"/>
+        <v>6665</v>
       </c>
       <c r="I261" s="5">
         <v>5169</v>
@@ -25439,15 +25454,9 @@
       <c r="K261" s="7">
         <v>679</v>
       </c>
-      <c r="L261">
-        <v>1305</v>
-      </c>
-      <c r="M261">
-        <v>86</v>
-      </c>
-      <c r="N261">
-        <v>20</v>
-      </c>
+      <c r="L261" s="22"/>
+      <c r="M261" s="22"/>
+      <c r="N261" s="22"/>
       <c r="O261">
         <v>0</v>
       </c>
@@ -25460,7 +25469,7 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <f t="shared" ref="C262" si="432">SUM(D262:F262)</f>
+        <f t="shared" ref="C262" si="427">SUM(D262:F262)</f>
         <v>1673</v>
       </c>
       <c r="D262">
@@ -25476,8 +25485,8 @@
         <v>75</v>
       </c>
       <c r="H262" s="16">
-        <f t="shared" ref="H262" si="433">SUM(I262:K262)-SUM(L262:N262)</f>
-        <v>5288</v>
+        <f t="shared" si="422"/>
+        <v>6699</v>
       </c>
       <c r="I262" s="5">
         <v>5188</v>
@@ -25488,15 +25497,9 @@
       <c r="K262" s="7">
         <v>683</v>
       </c>
-      <c r="L262">
-        <v>1305</v>
-      </c>
-      <c r="M262">
-        <v>86</v>
-      </c>
-      <c r="N262">
-        <v>20</v>
-      </c>
+      <c r="L262" s="22"/>
+      <c r="M262" s="22"/>
+      <c r="N262" s="22"/>
       <c r="O262">
         <v>0</v>
       </c>
@@ -25509,7 +25512,7 @@
         <v>9</v>
       </c>
       <c r="C263">
-        <f t="shared" ref="C263" si="434">SUM(D263:F263)</f>
+        <f t="shared" ref="C263" si="428">SUM(D263:F263)</f>
         <v>1673</v>
       </c>
       <c r="D263">
@@ -25525,8 +25528,8 @@
         <v>70</v>
       </c>
       <c r="H263" s="16">
-        <f t="shared" ref="H263" si="435">SUM(I263:K263)-SUM(L263:N263)</f>
-        <v>4976</v>
+        <f t="shared" si="422"/>
+        <v>6387</v>
       </c>
       <c r="I263" s="5">
         <v>4970</v>
@@ -25537,15 +25540,9 @@
       <c r="K263" s="7">
         <v>648</v>
       </c>
-      <c r="L263">
-        <v>1305</v>
-      </c>
-      <c r="M263">
-        <v>86</v>
-      </c>
-      <c r="N263">
-        <v>20</v>
-      </c>
+      <c r="L263" s="22"/>
+      <c r="M263" s="22"/>
+      <c r="N263" s="22"/>
       <c r="O263">
         <v>0</v>
       </c>
@@ -25558,7 +25555,7 @@
         <v>9</v>
       </c>
       <c r="C264">
-        <f t="shared" ref="C264" si="436">SUM(D264:F264)</f>
+        <f t="shared" ref="C264" si="429">SUM(D264:F264)</f>
         <v>1673</v>
       </c>
       <c r="D264">
@@ -25574,8 +25571,8 @@
         <v>70</v>
       </c>
       <c r="H264" s="16">
-        <f t="shared" ref="H264" si="437">SUM(I264:K264)-SUM(L264:N264)</f>
-        <v>4979</v>
+        <f t="shared" si="422"/>
+        <v>6390</v>
       </c>
       <c r="I264" s="5">
         <v>4980</v>
@@ -25586,15 +25583,9 @@
       <c r="K264" s="7">
         <v>644</v>
       </c>
-      <c r="L264">
-        <v>1305</v>
-      </c>
-      <c r="M264">
-        <v>86</v>
-      </c>
-      <c r="N264">
-        <v>20</v>
-      </c>
+      <c r="L264" s="22"/>
+      <c r="M264" s="22"/>
+      <c r="N264" s="22"/>
       <c r="O264">
         <v>0</v>
       </c>
@@ -25607,7 +25598,7 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <f t="shared" ref="C265" si="438">SUM(D265:F265)</f>
+        <f t="shared" ref="C265" si="430">SUM(D265:F265)</f>
         <v>1673</v>
       </c>
       <c r="D265">
@@ -25623,8 +25614,8 @@
         <v>70</v>
       </c>
       <c r="H265" s="16">
-        <f t="shared" ref="H265" si="439">SUM(I265:K265)-SUM(L265:N265)</f>
-        <v>4951</v>
+        <f t="shared" si="422"/>
+        <v>6362</v>
       </c>
       <c r="I265" s="5">
         <v>4955</v>
@@ -25635,15 +25626,9 @@
       <c r="K265" s="7">
         <v>642</v>
       </c>
-      <c r="L265">
-        <v>1305</v>
-      </c>
-      <c r="M265">
-        <v>86</v>
-      </c>
-      <c r="N265">
-        <v>20</v>
-      </c>
+      <c r="L265" s="22"/>
+      <c r="M265" s="22"/>
+      <c r="N265" s="22"/>
       <c r="O265">
         <v>0</v>
       </c>
@@ -25656,7 +25641,7 @@
         <v>9</v>
       </c>
       <c r="C266">
-        <f t="shared" ref="C266" si="440">SUM(D266:F266)</f>
+        <f t="shared" ref="C266" si="431">SUM(D266:F266)</f>
         <v>1673</v>
       </c>
       <c r="D266">
@@ -25672,8 +25657,8 @@
         <v>70</v>
       </c>
       <c r="H266" s="16">
-        <f t="shared" ref="H266" si="441">SUM(I266:K266)-SUM(L266:N266)</f>
-        <v>5076</v>
+        <f t="shared" si="422"/>
+        <v>6487</v>
       </c>
       <c r="I266" s="5">
         <v>5024</v>
@@ -25684,15 +25669,9 @@
       <c r="K266" s="7">
         <v>667</v>
       </c>
-      <c r="L266">
-        <v>1305</v>
-      </c>
-      <c r="M266">
-        <v>86</v>
-      </c>
-      <c r="N266">
-        <v>20</v>
-      </c>
+      <c r="L266" s="22"/>
+      <c r="M266" s="22"/>
+      <c r="N266" s="22"/>
       <c r="O266">
         <v>0</v>
       </c>
@@ -25705,7 +25684,7 @@
         <v>9</v>
       </c>
       <c r="C267">
-        <f t="shared" ref="C267" si="442">SUM(D267:F267)</f>
+        <f t="shared" ref="C267" si="432">SUM(D267:F267)</f>
         <v>1673</v>
       </c>
       <c r="D267">
@@ -25721,8 +25700,8 @@
         <v>70</v>
       </c>
       <c r="H267" s="16">
-        <f t="shared" ref="H267" si="443">SUM(I267:K267)-SUM(L267:N267)</f>
-        <v>4959</v>
+        <f t="shared" si="422"/>
+        <v>6370</v>
       </c>
       <c r="I267" s="5">
         <v>4980</v>
@@ -25733,15 +25712,9 @@
       <c r="K267" s="7">
         <v>664</v>
       </c>
-      <c r="L267">
-        <v>1305</v>
-      </c>
-      <c r="M267">
-        <v>86</v>
-      </c>
-      <c r="N267">
-        <v>20</v>
-      </c>
+      <c r="L267" s="22"/>
+      <c r="M267" s="22"/>
+      <c r="N267" s="22"/>
       <c r="O267">
         <v>0</v>
       </c>
@@ -25754,7 +25727,7 @@
         <v>9</v>
       </c>
       <c r="C268">
-        <f t="shared" ref="C268" si="444">SUM(D268:F268)</f>
+        <f t="shared" ref="C268" si="433">SUM(D268:F268)</f>
         <v>1673</v>
       </c>
       <c r="D268">
@@ -25770,8 +25743,8 @@
         <v>70</v>
       </c>
       <c r="H268" s="16">
-        <f t="shared" ref="H268" si="445">SUM(I268:K268)-SUM(L268:N268)</f>
-        <v>4959</v>
+        <f t="shared" si="422"/>
+        <v>6370</v>
       </c>
       <c r="I268" s="5">
         <v>4980</v>
@@ -25782,15 +25755,9 @@
       <c r="K268" s="7">
         <v>664</v>
       </c>
-      <c r="L268">
-        <v>1305</v>
-      </c>
-      <c r="M268">
-        <v>86</v>
-      </c>
-      <c r="N268">
-        <v>20</v>
-      </c>
+      <c r="L268" s="22"/>
+      <c r="M268" s="22"/>
+      <c r="N268" s="22"/>
       <c r="O268">
         <v>0</v>
       </c>
@@ -25803,7 +25770,7 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <f t="shared" ref="C269" si="446">SUM(D269:F269)</f>
+        <f t="shared" ref="C269" si="434">SUM(D269:F269)</f>
         <v>1673</v>
       </c>
       <c r="D269">
@@ -25819,8 +25786,8 @@
         <v>70</v>
       </c>
       <c r="H269" s="16">
-        <f t="shared" ref="H269" si="447">SUM(I269:K269)-SUM(L269:N269)</f>
-        <v>4954</v>
+        <f t="shared" si="422"/>
+        <v>6365</v>
       </c>
       <c r="I269" s="5">
         <v>4958</v>
@@ -25831,15 +25798,9 @@
       <c r="K269" s="7">
         <v>642</v>
       </c>
-      <c r="L269">
-        <v>1305</v>
-      </c>
-      <c r="M269">
-        <v>86</v>
-      </c>
-      <c r="N269">
-        <v>20</v>
-      </c>
+      <c r="L269" s="22"/>
+      <c r="M269" s="22"/>
+      <c r="N269" s="22"/>
       <c r="O269">
         <v>0</v>
       </c>
@@ -25852,7 +25813,7 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <f t="shared" ref="C270" si="448">SUM(D270:F270)</f>
+        <f t="shared" ref="C270" si="435">SUM(D270:F270)</f>
         <v>1673</v>
       </c>
       <c r="D270">
@@ -25868,8 +25829,8 @@
         <v>70</v>
       </c>
       <c r="H270" s="16">
-        <f t="shared" ref="H270" si="449">SUM(I270:K270)-SUM(L270:N270)</f>
-        <v>5085</v>
+        <f t="shared" si="422"/>
+        <v>6496</v>
       </c>
       <c r="I270" s="5">
         <v>5082</v>
@@ -25880,15 +25841,9 @@
       <c r="K270" s="7">
         <v>673</v>
       </c>
-      <c r="L270">
-        <v>1305</v>
-      </c>
-      <c r="M270">
-        <v>86</v>
-      </c>
-      <c r="N270">
-        <v>20</v>
-      </c>
+      <c r="L270" s="22"/>
+      <c r="M270" s="22"/>
+      <c r="N270" s="22"/>
       <c r="O270">
         <v>0</v>
       </c>
@@ -25901,7 +25856,7 @@
         <v>9</v>
       </c>
       <c r="C271">
-        <f t="shared" ref="C271" si="450">SUM(D271:F271)</f>
+        <f t="shared" ref="C271" si="436">SUM(D271:F271)</f>
         <v>1673</v>
       </c>
       <c r="D271">
@@ -25917,8 +25872,8 @@
         <v>70</v>
       </c>
       <c r="H271" s="16">
-        <f t="shared" ref="H271" si="451">SUM(I271:K271)-SUM(L271:N271)</f>
-        <v>4982</v>
+        <f t="shared" si="422"/>
+        <v>6393</v>
       </c>
       <c r="I271" s="5">
         <v>5037</v>
@@ -25929,15 +25884,9 @@
       <c r="K271" s="7">
         <v>652</v>
       </c>
-      <c r="L271">
-        <v>1305</v>
-      </c>
-      <c r="M271">
-        <v>86</v>
-      </c>
-      <c r="N271">
-        <v>20</v>
-      </c>
+      <c r="L271" s="22"/>
+      <c r="M271" s="22"/>
+      <c r="N271" s="22"/>
       <c r="O271">
         <v>0</v>
       </c>
@@ -25950,7 +25899,7 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <f t="shared" ref="C272" si="452">SUM(D272:F272)</f>
+        <f t="shared" ref="C272" si="437">SUM(D272:F272)</f>
         <v>1673</v>
       </c>
       <c r="D272">
@@ -25966,8 +25915,8 @@
         <v>70</v>
       </c>
       <c r="H272" s="16">
-        <f t="shared" ref="H272" si="453">SUM(I272:K272)-SUM(L272:N272)</f>
-        <v>5003</v>
+        <f t="shared" si="422"/>
+        <v>6414</v>
       </c>
       <c r="I272" s="5">
         <v>5069</v>
@@ -25978,15 +25927,9 @@
       <c r="K272" s="7">
         <v>649</v>
       </c>
-      <c r="L272">
-        <v>1305</v>
-      </c>
-      <c r="M272">
-        <v>86</v>
-      </c>
-      <c r="N272">
-        <v>20</v>
-      </c>
+      <c r="L272" s="22"/>
+      <c r="M272" s="22"/>
+      <c r="N272" s="22"/>
       <c r="O272">
         <v>0</v>
       </c>
@@ -25999,7 +25942,7 @@
         <v>9</v>
       </c>
       <c r="C273">
-        <f t="shared" ref="C273" si="454">SUM(D273:F273)</f>
+        <f t="shared" ref="C273" si="438">SUM(D273:F273)</f>
         <v>1673</v>
       </c>
       <c r="D273">
@@ -26015,8 +25958,8 @@
         <v>75</v>
       </c>
       <c r="H273" s="16">
-        <f t="shared" ref="H273" si="455">SUM(I273:K273)-SUM(L273:N273)</f>
-        <v>5023</v>
+        <f t="shared" si="422"/>
+        <v>6434</v>
       </c>
       <c r="I273" s="5">
         <v>5073</v>
@@ -26027,15 +25970,9 @@
       <c r="K273" s="7">
         <v>653</v>
       </c>
-      <c r="L273">
-        <v>1305</v>
-      </c>
-      <c r="M273">
-        <v>86</v>
-      </c>
-      <c r="N273">
-        <v>20</v>
-      </c>
+      <c r="L273" s="22"/>
+      <c r="M273" s="22"/>
+      <c r="N273" s="22"/>
       <c r="O273">
         <v>0</v>
       </c>
@@ -26048,7 +25985,7 @@
         <v>9</v>
       </c>
       <c r="C274">
-        <f t="shared" ref="C274" si="456">SUM(D274:F274)</f>
+        <f t="shared" ref="C274" si="439">SUM(D274:F274)</f>
         <v>1673</v>
       </c>
       <c r="D274">
@@ -26064,8 +26001,8 @@
         <v>82</v>
       </c>
       <c r="H274" s="16">
-        <f t="shared" ref="H274" si="457">SUM(I274:K274)-SUM(L274:N274)</f>
-        <v>5966</v>
+        <f t="shared" si="422"/>
+        <v>7377</v>
       </c>
       <c r="I274" s="5">
         <v>5831</v>
@@ -26076,15 +26013,9 @@
       <c r="K274" s="7">
         <v>743</v>
       </c>
-      <c r="L274">
-        <v>1305</v>
-      </c>
-      <c r="M274">
-        <v>86</v>
-      </c>
-      <c r="N274">
-        <v>20</v>
-      </c>
+      <c r="L274" s="22"/>
+      <c r="M274" s="22"/>
+      <c r="N274" s="22"/>
       <c r="O274">
         <v>9</v>
       </c>
@@ -26097,7 +26028,7 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <f t="shared" ref="C275" si="458">SUM(D275:F275)</f>
+        <f t="shared" ref="C275" si="440">SUM(D275:F275)</f>
         <v>1673</v>
       </c>
       <c r="D275">
@@ -26113,8 +26044,8 @@
         <v>83</v>
       </c>
       <c r="H275" s="16">
-        <f t="shared" ref="H275" si="459">SUM(I275:K275)-SUM(L275:N275)</f>
-        <v>6056</v>
+        <f t="shared" si="422"/>
+        <v>7467</v>
       </c>
       <c r="I275" s="5">
         <v>5928</v>
@@ -26125,15 +26056,9 @@
       <c r="K275" s="7">
         <v>737</v>
       </c>
-      <c r="L275">
-        <v>1305</v>
-      </c>
-      <c r="M275">
-        <v>86</v>
-      </c>
-      <c r="N275">
-        <v>20</v>
-      </c>
+      <c r="L275" s="22"/>
+      <c r="M275" s="22"/>
+      <c r="N275" s="22"/>
       <c r="O275">
         <v>12</v>
       </c>
@@ -26146,7 +26071,7 @@
         <v>9</v>
       </c>
       <c r="C276">
-        <f t="shared" ref="C276" si="460">SUM(D276:F276)</f>
+        <f t="shared" ref="C276" si="441">SUM(D276:F276)</f>
         <v>1673</v>
       </c>
       <c r="D276">
@@ -26162,8 +26087,8 @@
         <v>84</v>
       </c>
       <c r="H276" s="16">
-        <f t="shared" ref="H276" si="461">SUM(I276:K276)-SUM(L276:N276)</f>
-        <v>6273</v>
+        <f t="shared" si="422"/>
+        <v>7684</v>
       </c>
       <c r="I276" s="5">
         <v>6120</v>
@@ -26174,15 +26099,9 @@
       <c r="K276" s="7">
         <v>750</v>
       </c>
-      <c r="L276">
-        <v>1305</v>
-      </c>
-      <c r="M276">
-        <v>86</v>
-      </c>
-      <c r="N276">
-        <v>20</v>
-      </c>
+      <c r="L276" s="22"/>
+      <c r="M276" s="22"/>
+      <c r="N276" s="22"/>
       <c r="O276">
         <v>14</v>
       </c>
@@ -26195,7 +26114,7 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <f t="shared" ref="C277" si="462">SUM(D277:F277)</f>
+        <f t="shared" ref="C277" si="442">SUM(D277:F277)</f>
         <v>1673</v>
       </c>
       <c r="D277">
@@ -26211,8 +26130,8 @@
         <v>84</v>
       </c>
       <c r="H277" s="16">
-        <f t="shared" ref="H277" si="463">SUM(I277:K277)-SUM(L277:N277)</f>
-        <v>6362</v>
+        <f t="shared" si="422"/>
+        <v>7773</v>
       </c>
       <c r="I277" s="5">
         <v>6195</v>
@@ -26223,15 +26142,9 @@
       <c r="K277" s="7">
         <v>764</v>
       </c>
-      <c r="L277">
-        <v>1305</v>
-      </c>
-      <c r="M277">
-        <v>86</v>
-      </c>
-      <c r="N277">
-        <v>20</v>
-      </c>
+      <c r="L277" s="22"/>
+      <c r="M277" s="22"/>
+      <c r="N277" s="22"/>
       <c r="O277">
         <v>14</v>
       </c>
@@ -26244,7 +26157,7 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <f t="shared" ref="C278" si="464">SUM(D278:F278)</f>
+        <f t="shared" ref="C278" si="443">SUM(D278:F278)</f>
         <v>1673</v>
       </c>
       <c r="D278">
@@ -26260,8 +26173,8 @@
         <v>84</v>
       </c>
       <c r="H278" s="16">
-        <f t="shared" ref="H278" si="465">SUM(I278:K278)-SUM(L278:N278)</f>
-        <v>6370</v>
+        <f t="shared" si="422"/>
+        <v>7781</v>
       </c>
       <c r="I278" s="5">
         <v>6204</v>
@@ -26272,15 +26185,9 @@
       <c r="K278" s="7">
         <v>763</v>
       </c>
-      <c r="L278">
-        <v>1305</v>
-      </c>
-      <c r="M278">
-        <v>86</v>
-      </c>
-      <c r="N278">
-        <v>20</v>
-      </c>
+      <c r="L278" s="22"/>
+      <c r="M278" s="22"/>
+      <c r="N278" s="22"/>
       <c r="O278">
         <v>14</v>
       </c>
@@ -26293,7 +26200,7 @@
         <v>9</v>
       </c>
       <c r="C279">
-        <f t="shared" ref="C279" si="466">SUM(D279:F279)</f>
+        <f t="shared" ref="C279" si="444">SUM(D279:F279)</f>
         <v>1673</v>
       </c>
       <c r="D279">
@@ -26309,8 +26216,8 @@
         <v>85</v>
       </c>
       <c r="H279" s="16">
-        <f t="shared" ref="H279" si="467">SUM(I279:K279)-SUM(L279:N279)</f>
-        <v>6545</v>
+        <f t="shared" si="422"/>
+        <v>7956</v>
       </c>
       <c r="I279" s="5">
         <v>6351</v>
@@ -26321,15 +26228,9 @@
       <c r="K279" s="7">
         <v>777</v>
       </c>
-      <c r="L279">
-        <v>1305</v>
-      </c>
-      <c r="M279">
-        <v>86</v>
-      </c>
-      <c r="N279">
-        <v>20</v>
-      </c>
+      <c r="L279" s="22"/>
+      <c r="M279" s="22"/>
+      <c r="N279" s="22"/>
       <c r="O279">
         <v>15</v>
       </c>
@@ -26342,7 +26243,7 @@
         <v>9</v>
       </c>
       <c r="C280">
-        <f t="shared" ref="C280" si="468">SUM(D280:F280)</f>
+        <f t="shared" ref="C280" si="445">SUM(D280:F280)</f>
         <v>1673</v>
       </c>
       <c r="D280">
@@ -26358,8 +26259,8 @@
         <v>83</v>
       </c>
       <c r="H280" s="16">
-        <f t="shared" ref="H280" si="469">SUM(I280:K280)-SUM(L280:N280)</f>
-        <v>6523</v>
+        <f t="shared" si="422"/>
+        <v>7934</v>
       </c>
       <c r="I280" s="5">
         <v>6336</v>
@@ -26370,15 +26271,9 @@
       <c r="K280" s="7">
         <v>782</v>
       </c>
-      <c r="L280">
-        <v>1305</v>
-      </c>
-      <c r="M280">
-        <v>86</v>
-      </c>
-      <c r="N280">
-        <v>20</v>
-      </c>
+      <c r="L280" s="22"/>
+      <c r="M280" s="22"/>
+      <c r="N280" s="22"/>
       <c r="O280">
         <v>15</v>
       </c>
@@ -26391,7 +26286,7 @@
         <v>9</v>
       </c>
       <c r="C281">
-        <f t="shared" ref="C281" si="470">SUM(D281:F281)</f>
+        <f t="shared" ref="C281" si="446">SUM(D281:F281)</f>
         <v>1673</v>
       </c>
       <c r="D281">
@@ -26407,8 +26302,8 @@
         <v>83</v>
       </c>
       <c r="H281" s="16">
-        <f t="shared" ref="H281" si="471">SUM(I281:K281)-SUM(L281:N281)</f>
-        <v>6626</v>
+        <f t="shared" si="422"/>
+        <v>8037</v>
       </c>
       <c r="I281" s="5">
         <v>6406</v>
@@ -26419,15 +26314,9 @@
       <c r="K281" s="7">
         <v>801</v>
       </c>
-      <c r="L281">
-        <v>1305</v>
-      </c>
-      <c r="M281">
-        <v>86</v>
-      </c>
-      <c r="N281">
-        <v>20</v>
-      </c>
+      <c r="L281" s="22"/>
+      <c r="M281" s="22"/>
+      <c r="N281" s="22"/>
       <c r="O281">
         <v>17</v>
       </c>
@@ -26440,7 +26329,7 @@
         <v>9</v>
       </c>
       <c r="C282">
-        <f t="shared" ref="C282" si="472">SUM(D282:F282)</f>
+        <f t="shared" ref="C282" si="447">SUM(D282:F282)</f>
         <v>1673</v>
       </c>
       <c r="D282">
@@ -26456,8 +26345,8 @@
         <v>84</v>
       </c>
       <c r="H282" s="16">
-        <f t="shared" ref="H282" si="473">SUM(I282:K282)-SUM(L282:N282)</f>
-        <v>6869</v>
+        <f t="shared" si="422"/>
+        <v>8280</v>
       </c>
       <c r="I282" s="5">
         <v>6617</v>
@@ -26468,15 +26357,9 @@
       <c r="K282" s="7">
         <v>823</v>
       </c>
-      <c r="L282">
-        <v>1305</v>
-      </c>
-      <c r="M282">
-        <v>86</v>
-      </c>
-      <c r="N282">
-        <v>20</v>
-      </c>
+      <c r="L282" s="22"/>
+      <c r="M282" s="22"/>
+      <c r="N282" s="22"/>
       <c r="O282">
         <v>19</v>
       </c>
@@ -26489,7 +26372,7 @@
         <v>9</v>
       </c>
       <c r="C283">
-        <f t="shared" ref="C283" si="474">SUM(D283:F283)</f>
+        <f t="shared" ref="C283" si="448">SUM(D283:F283)</f>
         <v>1673</v>
       </c>
       <c r="D283">
@@ -26505,8 +26388,8 @@
         <v>84</v>
       </c>
       <c r="H283" s="16">
-        <f t="shared" ref="H283" si="475">SUM(I283:K283)-SUM(L283:N283)</f>
-        <v>6895</v>
+        <f t="shared" si="422"/>
+        <v>8306</v>
       </c>
       <c r="I283" s="5">
         <v>6643</v>
@@ -26517,15 +26400,9 @@
       <c r="K283" s="7">
         <v>823</v>
       </c>
-      <c r="L283">
-        <v>1305</v>
-      </c>
-      <c r="M283">
-        <v>86</v>
-      </c>
-      <c r="N283">
-        <v>20</v>
-      </c>
+      <c r="L283" s="22"/>
+      <c r="M283" s="22"/>
+      <c r="N283" s="22"/>
       <c r="O283">
         <v>19</v>
       </c>
@@ -26538,7 +26415,7 @@
         <v>9</v>
       </c>
       <c r="C284">
-        <f t="shared" ref="C284" si="476">SUM(D284:F284)</f>
+        <f t="shared" ref="C284" si="449">SUM(D284:F284)</f>
         <v>1673</v>
       </c>
       <c r="D284">
@@ -26554,8 +26431,8 @@
         <v>84</v>
       </c>
       <c r="H284" s="16">
-        <f t="shared" ref="H284" si="477">SUM(I284:K284)-SUM(L284:N284)</f>
-        <v>6934</v>
+        <f t="shared" si="422"/>
+        <v>8345</v>
       </c>
       <c r="I284" s="5">
         <v>6677</v>
@@ -26566,15 +26443,9 @@
       <c r="K284" s="7">
         <v>826</v>
       </c>
-      <c r="L284">
-        <v>1305</v>
-      </c>
-      <c r="M284">
-        <v>86</v>
-      </c>
-      <c r="N284">
-        <v>20</v>
-      </c>
+      <c r="L284" s="22"/>
+      <c r="M284" s="22"/>
+      <c r="N284" s="22"/>
       <c r="O284">
         <v>20</v>
       </c>
@@ -26587,7 +26458,7 @@
         <v>9</v>
       </c>
       <c r="C285">
-        <f t="shared" ref="C285:C286" si="478">SUM(D285:F285)</f>
+        <f t="shared" ref="C285:C286" si="450">SUM(D285:F285)</f>
         <v>1673</v>
       </c>
       <c r="D285">
@@ -26603,8 +26474,8 @@
         <v>84</v>
       </c>
       <c r="H285" s="16">
-        <f t="shared" ref="H285:H286" si="479">SUM(I285:K285)-SUM(L285:N285)</f>
-        <v>7042</v>
+        <f t="shared" si="422"/>
+        <v>8453</v>
       </c>
       <c r="I285" s="5">
         <v>6755</v>
@@ -26615,15 +26486,9 @@
       <c r="K285" s="7">
         <v>849</v>
       </c>
-      <c r="L285">
-        <v>1305</v>
-      </c>
-      <c r="M285">
-        <v>86</v>
-      </c>
-      <c r="N285">
-        <v>20</v>
-      </c>
+      <c r="L285" s="22"/>
+      <c r="M285" s="22"/>
+      <c r="N285" s="22"/>
       <c r="O285">
         <v>22</v>
       </c>
@@ -26636,7 +26501,7 @@
         <v>9</v>
       </c>
       <c r="C286">
-        <f t="shared" si="478"/>
+        <f t="shared" si="450"/>
         <v>1673</v>
       </c>
       <c r="D286">
@@ -26652,8 +26517,8 @@
         <v>84</v>
       </c>
       <c r="H286" s="16">
-        <f t="shared" si="479"/>
-        <v>7088</v>
+        <f t="shared" si="422"/>
+        <v>8499</v>
       </c>
       <c r="I286" s="5">
         <v>6809</v>
@@ -26664,15 +26529,9 @@
       <c r="K286" s="7">
         <v>845</v>
       </c>
-      <c r="L286">
-        <v>1305</v>
-      </c>
-      <c r="M286">
-        <v>86</v>
-      </c>
-      <c r="N286">
-        <v>20</v>
-      </c>
+      <c r="L286" s="22"/>
+      <c r="M286" s="22"/>
+      <c r="N286" s="22"/>
       <c r="O286">
         <v>22</v>
       </c>
@@ -26685,7 +26544,7 @@
         <v>9</v>
       </c>
       <c r="C287">
-        <f t="shared" ref="C287" si="480">SUM(D287:F287)</f>
+        <f t="shared" ref="C287" si="451">SUM(D287:F287)</f>
         <v>1673</v>
       </c>
       <c r="D287">
@@ -26701,8 +26560,8 @@
         <v>84</v>
       </c>
       <c r="H287" s="16">
-        <f t="shared" ref="H287" si="481">SUM(I287:K287)-SUM(L287:N287)</f>
-        <v>7158</v>
+        <f t="shared" si="422"/>
+        <v>8569</v>
       </c>
       <c r="I287" s="5">
         <v>6865</v>
@@ -26713,15 +26572,9 @@
       <c r="K287" s="7">
         <v>851</v>
       </c>
-      <c r="L287">
-        <v>1305</v>
-      </c>
-      <c r="M287">
-        <v>86</v>
-      </c>
-      <c r="N287">
-        <v>20</v>
-      </c>
+      <c r="L287" s="22"/>
+      <c r="M287" s="22"/>
+      <c r="N287" s="22"/>
       <c r="O287">
         <v>22</v>
       </c>
@@ -26734,7 +26587,7 @@
         <v>9</v>
       </c>
       <c r="C288">
-        <f t="shared" ref="C288" si="482">SUM(D288:F288)</f>
+        <f t="shared" ref="C288" si="452">SUM(D288:F288)</f>
         <v>1673</v>
       </c>
       <c r="D288">
@@ -26750,8 +26603,8 @@
         <v>85</v>
       </c>
       <c r="H288" s="16">
-        <f t="shared" ref="H288" si="483">SUM(I288:K288)-SUM(L288:N288)</f>
-        <v>7148</v>
+        <f t="shared" si="422"/>
+        <v>8559</v>
       </c>
       <c r="I288" s="5">
         <v>6848</v>
@@ -26762,15 +26615,9 @@
       <c r="K288" s="7">
         <v>856</v>
       </c>
-      <c r="L288">
-        <v>1305</v>
-      </c>
-      <c r="M288">
-        <v>86</v>
-      </c>
-      <c r="N288">
-        <v>20</v>
-      </c>
+      <c r="L288" s="22"/>
+      <c r="M288" s="22"/>
+      <c r="N288" s="22"/>
       <c r="O288">
         <v>22</v>
       </c>
@@ -26783,7 +26630,7 @@
         <v>9</v>
       </c>
       <c r="C289">
-        <f t="shared" ref="C289" si="484">SUM(D289:F289)</f>
+        <f t="shared" ref="C289" si="453">SUM(D289:F289)</f>
         <v>1673</v>
       </c>
       <c r="D289">
@@ -26799,8 +26646,8 @@
         <v>85</v>
       </c>
       <c r="H289" s="16">
-        <f t="shared" ref="H289" si="485">SUM(I289:K289)-SUM(L289:N289)</f>
-        <v>7150</v>
+        <f t="shared" si="422"/>
+        <v>8561</v>
       </c>
       <c r="I289" s="5">
         <v>6850</v>
@@ -26811,15 +26658,9 @@
       <c r="K289" s="7">
         <v>856</v>
       </c>
-      <c r="L289">
-        <v>1305</v>
-      </c>
-      <c r="M289">
-        <v>86</v>
-      </c>
-      <c r="N289">
-        <v>20</v>
-      </c>
+      <c r="L289" s="22"/>
+      <c r="M289" s="22"/>
+      <c r="N289" s="22"/>
       <c r="O289">
         <v>22</v>
       </c>
@@ -26832,7 +26673,7 @@
         <v>9</v>
       </c>
       <c r="C290">
-        <f t="shared" ref="C290" si="486">SUM(D290:F290)</f>
+        <f t="shared" ref="C290" si="454">SUM(D290:F290)</f>
         <v>1673</v>
       </c>
       <c r="D290">
@@ -26848,8 +26689,8 @@
         <v>80</v>
       </c>
       <c r="H290" s="16">
-        <f t="shared" ref="H290" si="487">SUM(I290:K290)-SUM(L290:N290)</f>
-        <v>6669</v>
+        <f t="shared" si="422"/>
+        <v>8080</v>
       </c>
       <c r="I290" s="5">
         <v>6442</v>
@@ -26860,15 +26701,9 @@
       <c r="K290" s="7">
         <v>829</v>
       </c>
-      <c r="L290">
-        <v>1305</v>
-      </c>
-      <c r="M290">
-        <v>86</v>
-      </c>
-      <c r="N290">
-        <v>20</v>
-      </c>
+      <c r="L290" s="22"/>
+      <c r="M290" s="22"/>
+      <c r="N290" s="22"/>
       <c r="O290">
         <v>23</v>
       </c>
@@ -26881,7 +26716,7 @@
         <v>9</v>
       </c>
       <c r="C291">
-        <f t="shared" ref="C291" si="488">SUM(D291:F291)</f>
+        <f t="shared" ref="C291" si="455">SUM(D291:F291)</f>
         <v>1673</v>
       </c>
       <c r="D291">
@@ -26897,8 +26732,8 @@
         <v>80</v>
       </c>
       <c r="H291" s="16">
-        <f t="shared" ref="H291" si="489">SUM(I291:K291)-SUM(L291:N291)</f>
-        <v>6718</v>
+        <f t="shared" si="422"/>
+        <v>8129</v>
       </c>
       <c r="I291" s="5">
         <v>6491</v>
@@ -26909,15 +26744,9 @@
       <c r="K291" s="7">
         <v>829</v>
       </c>
-      <c r="L291">
-        <v>1305</v>
-      </c>
-      <c r="M291">
-        <v>86</v>
-      </c>
-      <c r="N291">
-        <v>20</v>
-      </c>
+      <c r="L291" s="22"/>
+      <c r="M291" s="22"/>
+      <c r="N291" s="22"/>
       <c r="O291">
         <v>23</v>
       </c>
@@ -26930,7 +26759,7 @@
         <v>9</v>
       </c>
       <c r="C292">
-        <f t="shared" ref="C292" si="490">SUM(D292:F292)</f>
+        <f t="shared" ref="C292" si="456">SUM(D292:F292)</f>
         <v>1673</v>
       </c>
       <c r="D292">
@@ -26946,8 +26775,8 @@
         <v>81</v>
       </c>
       <c r="H292" s="16">
-        <f t="shared" ref="H292" si="491">SUM(I292:K292)-SUM(L292:N292)</f>
-        <v>6748</v>
+        <f t="shared" si="422"/>
+        <v>8159</v>
       </c>
       <c r="I292" s="5">
         <v>6486</v>
@@ -26958,15 +26787,9 @@
       <c r="K292" s="7">
         <v>844</v>
       </c>
-      <c r="L292">
-        <v>1305</v>
-      </c>
-      <c r="M292">
-        <v>86</v>
-      </c>
-      <c r="N292">
-        <v>20</v>
-      </c>
+      <c r="L292" s="22"/>
+      <c r="M292" s="22"/>
+      <c r="N292" s="22"/>
       <c r="O292">
         <v>23</v>
       </c>
@@ -26979,7 +26802,7 @@
         <v>9</v>
       </c>
       <c r="C293">
-        <f t="shared" ref="C293" si="492">SUM(D293:F293)</f>
+        <f t="shared" ref="C293" si="457">SUM(D293:F293)</f>
         <v>1673</v>
       </c>
       <c r="D293">
@@ -26995,8 +26818,8 @@
         <v>83</v>
       </c>
       <c r="H293" s="16">
-        <f t="shared" ref="H293" si="493">SUM(I293:K293)-SUM(L293:N293)</f>
-        <v>6858</v>
+        <f t="shared" si="422"/>
+        <v>8269</v>
       </c>
       <c r="I293" s="5">
         <v>6564</v>
@@ -27007,15 +26830,9 @@
       <c r="K293" s="7">
         <v>863</v>
       </c>
-      <c r="L293">
-        <v>1305</v>
-      </c>
-      <c r="M293">
-        <v>86</v>
-      </c>
-      <c r="N293">
-        <v>20</v>
-      </c>
+      <c r="L293" s="22"/>
+      <c r="M293" s="22"/>
+      <c r="N293" s="22"/>
       <c r="O293">
         <v>23</v>
       </c>
@@ -27028,7 +26845,7 @@
         <v>9</v>
       </c>
       <c r="C294">
-        <f t="shared" ref="C294" si="494">SUM(D294:F294)</f>
+        <f t="shared" ref="C294" si="458">SUM(D294:F294)</f>
         <v>1673</v>
       </c>
       <c r="D294">
@@ -27044,8 +26861,8 @@
         <v>86</v>
       </c>
       <c r="H294" s="16">
-        <f t="shared" ref="H294" si="495">SUM(I294:K294)-SUM(L294:N294)</f>
-        <v>7235</v>
+        <f t="shared" si="422"/>
+        <v>8646</v>
       </c>
       <c r="I294" s="5">
         <v>6894</v>
@@ -27056,15 +26873,9 @@
       <c r="K294" s="7">
         <v>890</v>
       </c>
-      <c r="L294">
-        <v>1305</v>
-      </c>
-      <c r="M294">
-        <v>86</v>
-      </c>
-      <c r="N294">
-        <v>20</v>
-      </c>
+      <c r="L294" s="22"/>
+      <c r="M294" s="22"/>
+      <c r="N294" s="22"/>
       <c r="O294">
         <v>23</v>
       </c>
@@ -27077,7 +26888,7 @@
         <v>9</v>
       </c>
       <c r="C295">
-        <f t="shared" ref="C295" si="496">SUM(D295:F295)</f>
+        <f t="shared" ref="C295" si="459">SUM(D295:F295)</f>
         <v>1673</v>
       </c>
       <c r="D295">
@@ -27093,8 +26904,8 @@
         <v>86</v>
       </c>
       <c r="H295" s="16">
-        <f t="shared" ref="H295" si="497">SUM(I295:K295)-SUM(L295:N295)</f>
-        <v>6913</v>
+        <f t="shared" si="422"/>
+        <v>8324</v>
       </c>
       <c r="I295" s="5">
         <v>6555</v>
@@ -27105,15 +26916,9 @@
       <c r="K295" s="7">
         <v>913</v>
       </c>
-      <c r="L295">
-        <v>1305</v>
-      </c>
-      <c r="M295">
-        <v>86</v>
-      </c>
-      <c r="N295">
-        <v>20</v>
-      </c>
+      <c r="L295" s="22"/>
+      <c r="M295" s="22"/>
+      <c r="N295" s="22"/>
       <c r="O295">
         <v>23</v>
       </c>
@@ -27126,7 +26931,7 @@
         <v>9</v>
       </c>
       <c r="C296">
-        <f t="shared" ref="C296" si="498">SUM(D296:F296)</f>
+        <f t="shared" ref="C296" si="460">SUM(D296:F296)</f>
         <v>1673</v>
       </c>
       <c r="D296">
@@ -27142,8 +26947,8 @@
         <v>86</v>
       </c>
       <c r="H296" s="16">
-        <f t="shared" ref="H296" si="499">SUM(I296:K296)-SUM(L296:N296)</f>
-        <v>7026</v>
+        <f t="shared" si="422"/>
+        <v>8437</v>
       </c>
       <c r="I296" s="5">
         <v>6645</v>
@@ -27154,15 +26959,9 @@
       <c r="K296" s="7">
         <v>924</v>
       </c>
-      <c r="L296">
-        <v>1305</v>
-      </c>
-      <c r="M296">
-        <v>86</v>
-      </c>
-      <c r="N296">
-        <v>20</v>
-      </c>
+      <c r="L296" s="22"/>
+      <c r="M296" s="22"/>
+      <c r="N296" s="22"/>
       <c r="O296">
         <v>23</v>
       </c>
@@ -27175,7 +26974,7 @@
         <v>9</v>
       </c>
       <c r="C297">
-        <f t="shared" ref="C297" si="500">SUM(D297:F297)</f>
+        <f t="shared" ref="C297" si="461">SUM(D297:F297)</f>
         <v>1673</v>
       </c>
       <c r="D297">
@@ -27191,8 +26990,8 @@
         <v>86</v>
       </c>
       <c r="H297" s="16">
-        <f t="shared" ref="H297" si="501">SUM(I297:K297)-SUM(L297:N297)</f>
-        <v>7051</v>
+        <f t="shared" si="422"/>
+        <v>8462</v>
       </c>
       <c r="I297" s="5">
         <v>6664</v>
@@ -27203,15 +27002,9 @@
       <c r="K297" s="7">
         <v>929</v>
       </c>
-      <c r="L297">
-        <v>1305</v>
-      </c>
-      <c r="M297">
-        <v>86</v>
-      </c>
-      <c r="N297">
-        <v>20</v>
-      </c>
+      <c r="L297" s="22"/>
+      <c r="M297" s="22"/>
+      <c r="N297" s="22"/>
       <c r="O297">
         <v>23</v>
       </c>
@@ -27224,7 +27017,7 @@
         <v>9</v>
       </c>
       <c r="C298">
-        <f t="shared" ref="C298" si="502">SUM(D298:F298)</f>
+        <f t="shared" ref="C298" si="462">SUM(D298:F298)</f>
         <v>1673</v>
       </c>
       <c r="D298">
@@ -27240,8 +27033,8 @@
         <v>87</v>
       </c>
       <c r="H298" s="16">
-        <f t="shared" ref="H298" si="503">SUM(I298:K298)-SUM(L298:N298)</f>
-        <v>7120</v>
+        <f t="shared" si="422"/>
+        <v>8531</v>
       </c>
       <c r="I298" s="5">
         <v>6711</v>
@@ -27252,15 +27045,9 @@
       <c r="K298" s="7">
         <v>941</v>
       </c>
-      <c r="L298">
-        <v>1305</v>
-      </c>
-      <c r="M298">
-        <v>86</v>
-      </c>
-      <c r="N298">
-        <v>20</v>
-      </c>
+      <c r="L298" s="22"/>
+      <c r="M298" s="22"/>
+      <c r="N298" s="22"/>
       <c r="O298">
         <v>23</v>
       </c>
@@ -27273,7 +27060,7 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <f t="shared" ref="C299" si="504">SUM(D299:F299)</f>
+        <f t="shared" ref="C299" si="463">SUM(D299:F299)</f>
         <v>1673</v>
       </c>
       <c r="D299">
@@ -27289,8 +27076,8 @@
         <v>88</v>
       </c>
       <c r="H299" s="16">
-        <f t="shared" ref="H299" si="505">SUM(I299:K299)-SUM(L299:N299)</f>
-        <v>7126</v>
+        <f t="shared" si="422"/>
+        <v>8537</v>
       </c>
       <c r="I299" s="5">
         <v>6708</v>
@@ -27301,15 +27088,9 @@
       <c r="K299" s="7">
         <v>946</v>
       </c>
-      <c r="L299">
-        <v>1305</v>
-      </c>
-      <c r="M299">
-        <v>86</v>
-      </c>
-      <c r="N299">
-        <v>20</v>
-      </c>
+      <c r="L299" s="22"/>
+      <c r="M299" s="22"/>
+      <c r="N299" s="22"/>
       <c r="O299">
         <v>23</v>
       </c>
@@ -27322,7 +27103,7 @@
         <v>9</v>
       </c>
       <c r="C300">
-        <f t="shared" ref="C300" si="506">SUM(D300:F300)</f>
+        <f t="shared" ref="C300" si="464">SUM(D300:F300)</f>
         <v>1673</v>
       </c>
       <c r="D300">
@@ -27338,8 +27119,8 @@
         <v>88</v>
       </c>
       <c r="H300" s="16">
-        <f t="shared" ref="H300" si="507">SUM(I300:K300)-SUM(L300:N300)</f>
-        <v>7139</v>
+        <f t="shared" si="422"/>
+        <v>8550</v>
       </c>
       <c r="I300" s="5">
         <v>6718</v>
@@ -27350,15 +27131,9 @@
       <c r="K300" s="7">
         <v>948</v>
       </c>
-      <c r="L300">
-        <v>1305</v>
-      </c>
-      <c r="M300">
-        <v>86</v>
-      </c>
-      <c r="N300">
-        <v>20</v>
-      </c>
+      <c r="L300" s="22"/>
+      <c r="M300" s="22"/>
+      <c r="N300" s="22"/>
       <c r="O300">
         <v>23</v>
       </c>
@@ -27371,7 +27146,7 @@
         <v>9</v>
       </c>
       <c r="C301">
-        <f t="shared" ref="C301" si="508">SUM(D301:F301)</f>
+        <f t="shared" ref="C301" si="465">SUM(D301:F301)</f>
         <v>1673</v>
       </c>
       <c r="D301">
@@ -27387,8 +27162,8 @@
         <v>88</v>
       </c>
       <c r="H301" s="16">
-        <f t="shared" ref="H301" si="509">SUM(I301:K301)-SUM(L301:N301)</f>
-        <v>7151</v>
+        <f t="shared" si="422"/>
+        <v>8562</v>
       </c>
       <c r="I301" s="5">
         <v>6707</v>
@@ -27399,15 +27174,9 @@
       <c r="K301" s="7">
         <v>948</v>
       </c>
-      <c r="L301">
-        <v>1305</v>
-      </c>
-      <c r="M301">
-        <v>86</v>
-      </c>
-      <c r="N301">
-        <v>20</v>
-      </c>
+      <c r="L301" s="22"/>
+      <c r="M301" s="22"/>
+      <c r="N301" s="22"/>
       <c r="O301">
         <v>23</v>
       </c>
@@ -27420,7 +27189,7 @@
         <v>9</v>
       </c>
       <c r="C302">
-        <f t="shared" ref="C302" si="510">SUM(D302:F302)</f>
+        <f t="shared" ref="C302" si="466">SUM(D302:F302)</f>
         <v>1673</v>
       </c>
       <c r="D302">
@@ -27436,8 +27205,8 @@
         <v>88</v>
       </c>
       <c r="H302" s="16">
-        <f t="shared" ref="H302" si="511">SUM(I302:K302)-SUM(L302:N302)</f>
-        <v>7151</v>
+        <f t="shared" si="422"/>
+        <v>8562</v>
       </c>
       <c r="I302" s="5">
         <v>6727</v>
@@ -27448,15 +27217,9 @@
       <c r="K302" s="7">
         <v>951</v>
       </c>
-      <c r="L302">
-        <v>1305</v>
-      </c>
-      <c r="M302">
-        <v>86</v>
-      </c>
-      <c r="N302">
-        <v>20</v>
-      </c>
+      <c r="L302" s="22"/>
+      <c r="M302" s="22"/>
+      <c r="N302" s="22"/>
       <c r="O302">
         <v>23</v>
       </c>
@@ -27469,7 +27232,7 @@
         <v>9</v>
       </c>
       <c r="C303">
-        <f t="shared" ref="C303" si="512">SUM(D303:F303)</f>
+        <f t="shared" ref="C303" si="467">SUM(D303:F303)</f>
         <v>1673</v>
       </c>
       <c r="D303">
@@ -27485,8 +27248,8 @@
         <v>89</v>
       </c>
       <c r="H303" s="16">
-        <f t="shared" ref="H303" si="513">SUM(I303:K303)-SUM(L303:N303)</f>
-        <v>7208</v>
+        <f t="shared" si="422"/>
+        <v>8619</v>
       </c>
       <c r="I303" s="5">
         <v>6764</v>
@@ -27497,15 +27260,9 @@
       <c r="K303" s="7">
         <v>962</v>
       </c>
-      <c r="L303">
-        <v>1305</v>
-      </c>
-      <c r="M303">
-        <v>86</v>
-      </c>
-      <c r="N303">
-        <v>20</v>
-      </c>
+      <c r="L303" s="22"/>
+      <c r="M303" s="22"/>
+      <c r="N303" s="22"/>
       <c r="O303">
         <v>23</v>
       </c>
@@ -27518,7 +27275,7 @@
         <v>9</v>
       </c>
       <c r="C304">
-        <f t="shared" ref="C304" si="514">SUM(D304:F304)</f>
+        <f t="shared" ref="C304" si="468">SUM(D304:F304)</f>
         <v>1673</v>
       </c>
       <c r="D304">
@@ -27534,8 +27291,8 @@
         <v>89</v>
       </c>
       <c r="H304" s="16">
-        <f t="shared" ref="H304" si="515">SUM(I304:K304)-SUM(L304:N304)</f>
-        <v>7228</v>
+        <f t="shared" si="422"/>
+        <v>8639</v>
       </c>
       <c r="I304" s="5">
         <v>6781</v>
@@ -27546,15 +27303,9 @@
       <c r="K304" s="7">
         <v>964</v>
       </c>
-      <c r="L304">
-        <v>1305</v>
-      </c>
-      <c r="M304">
-        <v>86</v>
-      </c>
-      <c r="N304">
-        <v>20</v>
-      </c>
+      <c r="L304" s="22"/>
+      <c r="M304" s="22"/>
+      <c r="N304" s="22"/>
       <c r="O304">
         <v>23</v>
       </c>
@@ -27567,7 +27318,7 @@
         <v>9</v>
       </c>
       <c r="C305">
-        <f t="shared" ref="C305" si="516">SUM(D305:F305)</f>
+        <f t="shared" ref="C305" si="469">SUM(D305:F305)</f>
         <v>1673</v>
       </c>
       <c r="D305">
@@ -27583,8 +27334,8 @@
         <v>89</v>
       </c>
       <c r="H305" s="16">
-        <f t="shared" ref="H305" si="517">SUM(I305:K305)-SUM(L305:N305)</f>
-        <v>7228</v>
+        <f t="shared" si="422"/>
+        <v>8639</v>
       </c>
       <c r="I305" s="5">
         <v>6781</v>
@@ -27595,15 +27346,9 @@
       <c r="K305" s="7">
         <v>964</v>
       </c>
-      <c r="L305">
-        <v>1305</v>
-      </c>
-      <c r="M305">
-        <v>86</v>
-      </c>
-      <c r="N305">
-        <v>20</v>
-      </c>
+      <c r="L305" s="22"/>
+      <c r="M305" s="22"/>
+      <c r="N305" s="22"/>
       <c r="O305">
         <v>23</v>
       </c>
@@ -27616,7 +27361,7 @@
         <v>9</v>
       </c>
       <c r="C306">
-        <f t="shared" ref="C306" si="518">SUM(D306:F306)</f>
+        <f t="shared" ref="C306" si="470">SUM(D306:F306)</f>
         <v>1673</v>
       </c>
       <c r="D306">
@@ -27632,8 +27377,8 @@
         <v>89</v>
       </c>
       <c r="H306" s="16">
-        <f t="shared" ref="H306" si="519">SUM(I306:K306)-SUM(L306:N306)</f>
-        <v>7240</v>
+        <f t="shared" si="422"/>
+        <v>8651</v>
       </c>
       <c r="I306" s="5">
         <v>6791</v>
@@ -27644,15 +27389,9 @@
       <c r="K306" s="7">
         <v>967</v>
       </c>
-      <c r="L306">
-        <v>1305</v>
-      </c>
-      <c r="M306">
-        <v>86</v>
-      </c>
-      <c r="N306">
-        <v>20</v>
-      </c>
+      <c r="L306" s="22"/>
+      <c r="M306" s="22"/>
+      <c r="N306" s="22"/>
       <c r="O306">
         <v>23</v>
       </c>
@@ -27665,7 +27404,7 @@
         <v>9</v>
       </c>
       <c r="C307">
-        <f t="shared" ref="C307" si="520">SUM(D307:F307)</f>
+        <f t="shared" ref="C307" si="471">SUM(D307:F307)</f>
         <v>1673</v>
       </c>
       <c r="D307">
@@ -27681,8 +27420,8 @@
         <v>89</v>
       </c>
       <c r="H307" s="16">
-        <f t="shared" ref="H307" si="521">SUM(I307:K307)-SUM(L307:N307)</f>
-        <v>7317</v>
+        <f t="shared" si="422"/>
+        <v>8728</v>
       </c>
       <c r="I307" s="5">
         <v>6859</v>
@@ -27693,15 +27432,9 @@
       <c r="K307" s="7">
         <v>973</v>
       </c>
-      <c r="L307">
-        <v>1305</v>
-      </c>
-      <c r="M307">
-        <v>86</v>
-      </c>
-      <c r="N307">
-        <v>20</v>
-      </c>
+      <c r="L307" s="22"/>
+      <c r="M307" s="22"/>
+      <c r="N307" s="22"/>
       <c r="O307">
         <v>23</v>
       </c>
@@ -27714,7 +27447,7 @@
         <v>9</v>
       </c>
       <c r="C308">
-        <f t="shared" ref="C308" si="522">SUM(D308:F308)</f>
+        <f t="shared" ref="C308" si="472">SUM(D308:F308)</f>
         <v>1673</v>
       </c>
       <c r="D308">
@@ -27730,8 +27463,8 @@
         <v>90</v>
       </c>
       <c r="H308" s="16">
-        <f t="shared" ref="H308" si="523">SUM(I308:K308)-SUM(L308:N308)</f>
-        <v>7493</v>
+        <f t="shared" si="422"/>
+        <v>8904</v>
       </c>
       <c r="I308" s="5">
         <v>6959</v>
@@ -27742,15 +27475,9 @@
       <c r="K308" s="7">
         <v>968</v>
       </c>
-      <c r="L308">
-        <v>1305</v>
-      </c>
-      <c r="M308">
-        <v>86</v>
-      </c>
-      <c r="N308">
-        <v>20</v>
-      </c>
+      <c r="L308" s="22"/>
+      <c r="M308" s="22"/>
+      <c r="N308" s="22"/>
       <c r="O308">
         <v>23</v>
       </c>
@@ -27763,7 +27490,7 @@
         <v>9</v>
       </c>
       <c r="C309">
-        <f t="shared" ref="C309" si="524">SUM(D309:F309)</f>
+        <f t="shared" ref="C309" si="473">SUM(D309:F309)</f>
         <v>1673</v>
       </c>
       <c r="D309">
@@ -27779,8 +27506,8 @@
         <v>90</v>
       </c>
       <c r="H309" s="16">
-        <f t="shared" ref="H309" si="525">SUM(I309:K309)-SUM(L309:N309)</f>
-        <v>7560</v>
+        <f t="shared" si="422"/>
+        <v>8971</v>
       </c>
       <c r="I309" s="5">
         <v>7046</v>
@@ -27791,15 +27518,9 @@
       <c r="K309" s="7">
         <v>986</v>
       </c>
-      <c r="L309">
-        <v>1305</v>
-      </c>
-      <c r="M309">
-        <v>86</v>
-      </c>
-      <c r="N309">
-        <v>20</v>
-      </c>
+      <c r="L309" s="22"/>
+      <c r="M309" s="22"/>
+      <c r="N309" s="22"/>
       <c r="O309">
         <v>24</v>
       </c>
@@ -27812,7 +27533,7 @@
         <v>9</v>
       </c>
       <c r="C310">
-        <f t="shared" ref="C310" si="526">SUM(D310:F310)</f>
+        <f t="shared" ref="C310" si="474">SUM(D310:F310)</f>
         <v>1673</v>
       </c>
       <c r="D310">
@@ -27828,8 +27549,8 @@
         <v>90</v>
       </c>
       <c r="H310" s="16">
-        <f t="shared" ref="H310" si="527">SUM(I310:K310)-SUM(L310:N310)</f>
-        <v>7629</v>
+        <f t="shared" si="422"/>
+        <v>9040</v>
       </c>
       <c r="I310" s="5">
         <v>7177</v>
@@ -27840,15 +27561,9 @@
       <c r="K310" s="7">
         <v>958</v>
       </c>
-      <c r="L310">
-        <v>1305</v>
-      </c>
-      <c r="M310">
-        <v>86</v>
-      </c>
-      <c r="N310">
-        <v>20</v>
-      </c>
+      <c r="L310" s="22"/>
+      <c r="M310" s="22"/>
+      <c r="N310" s="22"/>
       <c r="O310">
         <v>24</v>
       </c>
@@ -27861,7 +27576,7 @@
         <v>9</v>
       </c>
       <c r="C311">
-        <f t="shared" ref="C311" si="528">SUM(D311:F311)</f>
+        <f t="shared" ref="C311" si="475">SUM(D311:F311)</f>
         <v>1673</v>
       </c>
       <c r="D311">
@@ -27877,8 +27592,8 @@
         <v>99</v>
       </c>
       <c r="H311" s="16">
-        <f t="shared" ref="H311" si="529">SUM(I311:K311)-SUM(L311:N311)</f>
-        <v>9241</v>
+        <f t="shared" si="422"/>
+        <v>10652</v>
       </c>
       <c r="I311" s="5">
         <v>8630</v>
@@ -27889,15 +27604,9 @@
       <c r="K311" s="7">
         <v>1043</v>
       </c>
-      <c r="L311">
-        <v>1305</v>
-      </c>
-      <c r="M311">
-        <v>86</v>
-      </c>
-      <c r="N311">
-        <v>20</v>
-      </c>
+      <c r="L311" s="22"/>
+      <c r="M311" s="22"/>
+      <c r="N311" s="22"/>
       <c r="O311">
         <v>24</v>
       </c>
@@ -27910,7 +27619,7 @@
         <v>9</v>
       </c>
       <c r="C312">
-        <f t="shared" ref="C312" si="530">SUM(D312:F312)</f>
+        <f t="shared" ref="C312" si="476">SUM(D312:F312)</f>
         <v>1673</v>
       </c>
       <c r="D312">
@@ -27926,8 +27635,8 @@
         <v>101</v>
       </c>
       <c r="H312" s="16">
-        <f t="shared" ref="H312" si="531">SUM(I312:K312)-SUM(L312:N312)</f>
-        <v>9465</v>
+        <f t="shared" si="422"/>
+        <v>10876</v>
       </c>
       <c r="I312" s="5">
         <v>8833</v>
@@ -27938,15 +27647,9 @@
       <c r="K312" s="7">
         <v>1056</v>
       </c>
-      <c r="L312">
-        <v>1305</v>
-      </c>
-      <c r="M312">
-        <v>86</v>
-      </c>
-      <c r="N312">
-        <v>20</v>
-      </c>
+      <c r="L312" s="22"/>
+      <c r="M312" s="22"/>
+      <c r="N312" s="22"/>
       <c r="O312">
         <v>31</v>
       </c>
@@ -27959,7 +27662,7 @@
         <v>9</v>
       </c>
       <c r="C313">
-        <f t="shared" ref="C313" si="532">SUM(D313:F313)</f>
+        <f t="shared" ref="C313" si="477">SUM(D313:F313)</f>
         <v>1673</v>
       </c>
       <c r="D313">
@@ -27975,8 +27678,8 @@
         <v>101</v>
       </c>
       <c r="H313" s="16">
-        <f t="shared" ref="H313" si="533">SUM(I313:K313)-SUM(L313:N313)</f>
-        <v>9692</v>
+        <f t="shared" si="422"/>
+        <v>11103</v>
       </c>
       <c r="I313" s="5">
         <v>9036</v>
@@ -27987,15 +27690,9 @@
       <c r="K313" s="7">
         <v>1068</v>
       </c>
-      <c r="L313">
-        <v>1305</v>
-      </c>
-      <c r="M313">
-        <v>86</v>
-      </c>
-      <c r="N313">
-        <v>20</v>
-      </c>
+      <c r="L313" s="22"/>
+      <c r="M313" s="22"/>
+      <c r="N313" s="22"/>
       <c r="O313">
         <v>31</v>
       </c>
@@ -28008,7 +27705,7 @@
         <v>9</v>
       </c>
       <c r="C314">
-        <f t="shared" ref="C314" si="534">SUM(D314:F314)</f>
+        <f t="shared" ref="C314" si="478">SUM(D314:F314)</f>
         <v>1673</v>
       </c>
       <c r="D314">
@@ -28024,8 +27721,8 @@
         <v>101</v>
       </c>
       <c r="H314" s="16">
-        <f t="shared" ref="H314" si="535">SUM(I314:K314)-SUM(L314:N314)</f>
-        <v>9697</v>
+        <f t="shared" si="422"/>
+        <v>11108</v>
       </c>
       <c r="I314" s="5">
         <v>9039</v>
@@ -28036,15 +27733,9 @@
       <c r="K314" s="7">
         <v>1069</v>
       </c>
-      <c r="L314">
-        <v>1305</v>
-      </c>
-      <c r="M314">
-        <v>86</v>
-      </c>
-      <c r="N314">
-        <v>20</v>
-      </c>
+      <c r="L314" s="22"/>
+      <c r="M314" s="22"/>
+      <c r="N314" s="22"/>
       <c r="O314">
         <v>31</v>
       </c>
@@ -28057,7 +27748,7 @@
         <v>9</v>
       </c>
       <c r="C315">
-        <f t="shared" ref="C315" si="536">SUM(D315:F315)</f>
+        <f t="shared" ref="C315" si="479">SUM(D315:F315)</f>
         <v>1673</v>
       </c>
       <c r="D315">
@@ -28073,8 +27764,8 @@
         <v>101</v>
       </c>
       <c r="H315" s="16">
-        <f t="shared" ref="H315" si="537">SUM(I315:K315)-SUM(L315:N315)</f>
-        <v>9751</v>
+        <f t="shared" si="422"/>
+        <v>11162</v>
       </c>
       <c r="I315" s="5">
         <v>9132</v>
@@ -28085,15 +27776,9 @@
       <c r="K315" s="7">
         <v>1033</v>
       </c>
-      <c r="L315">
-        <v>1305</v>
-      </c>
-      <c r="M315">
-        <v>86</v>
-      </c>
-      <c r="N315">
-        <v>20</v>
-      </c>
+      <c r="L315" s="22"/>
+      <c r="M315" s="22"/>
+      <c r="N315" s="22"/>
       <c r="O315">
         <v>31</v>
       </c>
@@ -28106,7 +27791,7 @@
         <v>9</v>
       </c>
       <c r="C316">
-        <f t="shared" ref="C316" si="538">SUM(D316:F316)</f>
+        <f t="shared" ref="C316" si="480">SUM(D316:F316)</f>
         <v>1673</v>
       </c>
       <c r="D316">
@@ -28122,8 +27807,8 @@
         <v>101</v>
       </c>
       <c r="H316" s="16">
-        <f t="shared" ref="H316" si="539">SUM(I316:K316)-SUM(L316:N316)</f>
-        <v>9751</v>
+        <f t="shared" si="422"/>
+        <v>11162</v>
       </c>
       <c r="I316" s="5">
         <v>9132</v>
@@ -28134,15 +27819,9 @@
       <c r="K316" s="7">
         <v>1033</v>
       </c>
-      <c r="L316">
-        <v>1305</v>
-      </c>
-      <c r="M316">
-        <v>86</v>
-      </c>
-      <c r="N316">
-        <v>20</v>
-      </c>
+      <c r="L316" s="22"/>
+      <c r="M316" s="22"/>
+      <c r="N316" s="22"/>
       <c r="O316">
         <v>31</v>
       </c>
@@ -28155,7 +27834,7 @@
         <v>9</v>
       </c>
       <c r="C317">
-        <f t="shared" ref="C317" si="540">SUM(D317:F317)</f>
+        <f t="shared" ref="C317" si="481">SUM(D317:F317)</f>
         <v>1673</v>
       </c>
       <c r="D317">
@@ -28171,8 +27850,8 @@
         <v>103</v>
       </c>
       <c r="H317" s="16">
-        <f t="shared" ref="H317" si="541">SUM(I317:K317)-SUM(L317:N317)</f>
-        <v>9892</v>
+        <f t="shared" si="422"/>
+        <v>11303</v>
       </c>
       <c r="I317" s="5">
         <v>9236</v>
@@ -28183,15 +27862,9 @@
       <c r="K317" s="7">
         <v>1056</v>
       </c>
-      <c r="L317">
-        <v>1305</v>
-      </c>
-      <c r="M317">
-        <v>86</v>
-      </c>
-      <c r="N317">
-        <v>20</v>
-      </c>
+      <c r="L317" s="22"/>
+      <c r="M317" s="22"/>
+      <c r="N317" s="22"/>
       <c r="O317">
         <v>31</v>
       </c>
@@ -28204,7 +27877,7 @@
         <v>9</v>
       </c>
       <c r="C318">
-        <f t="shared" ref="C318" si="542">SUM(D318:F318)</f>
+        <f t="shared" ref="C318" si="482">SUM(D318:F318)</f>
         <v>1673</v>
       </c>
       <c r="D318">
@@ -28220,8 +27893,8 @@
         <v>103</v>
       </c>
       <c r="H318" s="16">
-        <f t="shared" ref="H318" si="543">SUM(I318:K318)-SUM(L318:N318)</f>
-        <v>9893</v>
+        <f t="shared" si="422"/>
+        <v>11304</v>
       </c>
       <c r="I318" s="5">
         <v>9232</v>
@@ -28232,15 +27905,9 @@
       <c r="K318" s="7">
         <v>1060</v>
       </c>
-      <c r="L318">
-        <v>1305</v>
-      </c>
-      <c r="M318">
-        <v>86</v>
-      </c>
-      <c r="N318">
-        <v>20</v>
-      </c>
+      <c r="L318" s="22"/>
+      <c r="M318" s="22"/>
+      <c r="N318" s="22"/>
       <c r="O318">
         <v>31</v>
       </c>
@@ -28253,7 +27920,7 @@
         <v>9</v>
       </c>
       <c r="C319">
-        <f t="shared" ref="C319" si="544">SUM(D319:F319)</f>
+        <f t="shared" ref="C319" si="483">SUM(D319:F319)</f>
         <v>1673</v>
       </c>
       <c r="D319">
@@ -28269,8 +27936,8 @@
         <v>103</v>
       </c>
       <c r="H319" s="16">
-        <f t="shared" ref="H319" si="545">SUM(I319:K319)-SUM(L319:N319)</f>
-        <v>9949</v>
+        <f t="shared" si="422"/>
+        <v>11360</v>
       </c>
       <c r="I319" s="5">
         <v>9263</v>
@@ -28281,15 +27948,9 @@
       <c r="K319" s="7">
         <v>1065</v>
       </c>
-      <c r="L319">
-        <v>1305</v>
-      </c>
-      <c r="M319">
-        <v>86</v>
-      </c>
-      <c r="N319">
-        <v>20</v>
-      </c>
+      <c r="L319" s="22"/>
+      <c r="M319" s="22"/>
+      <c r="N319" s="22"/>
       <c r="O319">
         <v>31</v>
       </c>
@@ -28302,7 +27963,7 @@
         <v>9</v>
       </c>
       <c r="C320">
-        <f t="shared" ref="C320" si="546">SUM(D320:F320)</f>
+        <f t="shared" ref="C320" si="484">SUM(D320:F320)</f>
         <v>1673</v>
       </c>
       <c r="D320">
@@ -28318,8 +27979,8 @@
         <v>104</v>
       </c>
       <c r="H320" s="16">
-        <f t="shared" ref="H320" si="547">SUM(I320:K320)-SUM(L320:N320)</f>
-        <v>10026</v>
+        <f t="shared" si="422"/>
+        <v>11437</v>
       </c>
       <c r="I320" s="5">
         <v>9315</v>
@@ -28330,15 +27991,9 @@
       <c r="K320" s="7">
         <v>1071</v>
       </c>
-      <c r="L320">
-        <v>1305</v>
-      </c>
-      <c r="M320">
-        <v>86</v>
-      </c>
-      <c r="N320">
-        <v>20</v>
-      </c>
+      <c r="L320" s="22"/>
+      <c r="M320" s="22"/>
+      <c r="N320" s="22"/>
       <c r="O320">
         <v>31</v>
       </c>
@@ -28351,7 +28006,7 @@
         <v>9</v>
       </c>
       <c r="C321">
-        <f t="shared" ref="C321" si="548">SUM(D321:F321)</f>
+        <f t="shared" ref="C321" si="485">SUM(D321:F321)</f>
         <v>1673</v>
       </c>
       <c r="D321">
@@ -28367,8 +28022,8 @@
         <v>104</v>
       </c>
       <c r="H321" s="16">
-        <f t="shared" ref="H321" si="549">SUM(I321:K321)-SUM(L321:N321)</f>
-        <v>10107</v>
+        <f t="shared" ref="H321:H327" si="486">SUM(I321:K321)</f>
+        <v>11518</v>
       </c>
       <c r="I321" s="5">
         <v>9340</v>
@@ -28379,15 +28034,9 @@
       <c r="K321" s="7">
         <v>1096</v>
       </c>
-      <c r="L321">
-        <v>1305</v>
-      </c>
-      <c r="M321">
-        <v>86</v>
-      </c>
-      <c r="N321">
-        <v>20</v>
-      </c>
+      <c r="L321" s="22"/>
+      <c r="M321" s="22"/>
+      <c r="N321" s="22"/>
       <c r="O321">
         <v>31</v>
       </c>
@@ -28400,7 +28049,7 @@
         <v>9</v>
       </c>
       <c r="C322">
-        <f t="shared" ref="C322" si="550">SUM(D322:F322)</f>
+        <f t="shared" ref="C322" si="487">SUM(D322:F322)</f>
         <v>1673</v>
       </c>
       <c r="D322">
@@ -28416,8 +28065,8 @@
         <v>108</v>
       </c>
       <c r="H322" s="16">
-        <f t="shared" ref="H322" si="551">SUM(I322:K322)-SUM(L322:N322)</f>
-        <v>10207</v>
+        <f t="shared" si="486"/>
+        <v>11618</v>
       </c>
       <c r="I322" s="5">
         <v>9402</v>
@@ -28428,15 +28077,9 @@
       <c r="K322" s="7">
         <v>1106</v>
       </c>
-      <c r="L322">
-        <v>1305</v>
-      </c>
-      <c r="M322">
-        <v>86</v>
-      </c>
-      <c r="N322">
-        <v>20</v>
-      </c>
+      <c r="L322" s="22"/>
+      <c r="M322" s="22"/>
+      <c r="N322" s="22"/>
       <c r="O322">
         <v>31</v>
       </c>
@@ -28449,7 +28092,7 @@
         <v>9</v>
       </c>
       <c r="C323">
-        <f t="shared" ref="C323" si="552">SUM(D323:F323)</f>
+        <f t="shared" ref="C323" si="488">SUM(D323:F323)</f>
         <v>1673</v>
       </c>
       <c r="D323">
@@ -28465,8 +28108,8 @@
         <v>109</v>
       </c>
       <c r="H323" s="16">
-        <f t="shared" ref="H323" si="553">SUM(I323:K323)-SUM(L323:N323)</f>
-        <v>10284</v>
+        <f t="shared" si="486"/>
+        <v>11695</v>
       </c>
       <c r="I323" s="5">
         <v>9460</v>
@@ -28477,15 +28120,9 @@
       <c r="K323" s="7">
         <v>1118</v>
       </c>
-      <c r="L323">
-        <v>1305</v>
-      </c>
-      <c r="M323">
-        <v>86</v>
-      </c>
-      <c r="N323">
-        <v>20</v>
-      </c>
+      <c r="L323" s="22"/>
+      <c r="M323" s="22"/>
+      <c r="N323" s="22"/>
       <c r="O323">
         <v>31</v>
       </c>
@@ -28498,7 +28135,7 @@
         <v>9</v>
       </c>
       <c r="C324">
-        <f t="shared" ref="C324" si="554">SUM(D324:F324)</f>
+        <f t="shared" ref="C324" si="489">SUM(D324:F324)</f>
         <v>1673</v>
       </c>
       <c r="D324">
@@ -28514,8 +28151,8 @@
         <v>111</v>
       </c>
       <c r="H324" s="16">
-        <f t="shared" ref="H324" si="555">SUM(I324:K324)-SUM(L324:N324)</f>
-        <v>10590</v>
+        <f t="shared" si="486"/>
+        <v>12001</v>
       </c>
       <c r="I324" s="5">
         <v>9701</v>
@@ -28526,15 +28163,9 @@
       <c r="K324" s="7">
         <v>1150</v>
       </c>
-      <c r="L324">
-        <v>1305</v>
-      </c>
-      <c r="M324">
-        <v>86</v>
-      </c>
-      <c r="N324">
-        <v>20</v>
-      </c>
+      <c r="L324" s="22"/>
+      <c r="M324" s="22"/>
+      <c r="N324" s="22"/>
       <c r="O324">
         <v>31</v>
       </c>
@@ -28547,7 +28178,7 @@
         <v>9</v>
       </c>
       <c r="C325">
-        <f t="shared" ref="C325" si="556">SUM(D325:F325)</f>
+        <f t="shared" ref="C325" si="490">SUM(D325:F325)</f>
         <v>1673</v>
       </c>
       <c r="D325">
@@ -28563,8 +28194,8 @@
         <v>112</v>
       </c>
       <c r="H325" s="16">
-        <f t="shared" ref="H325" si="557">SUM(I325:K325)-SUM(L325:N325)</f>
-        <v>10849</v>
+        <f t="shared" si="486"/>
+        <v>12260</v>
       </c>
       <c r="I325" s="5">
         <v>9942</v>
@@ -28575,15 +28206,9 @@
       <c r="K325" s="7">
         <v>1158</v>
       </c>
-      <c r="L325">
-        <v>1305</v>
-      </c>
-      <c r="M325">
-        <v>86</v>
-      </c>
-      <c r="N325">
-        <v>20</v>
-      </c>
+      <c r="L325" s="22"/>
+      <c r="M325" s="22"/>
+      <c r="N325" s="22"/>
       <c r="O325">
         <v>31</v>
       </c>
@@ -28596,7 +28221,7 @@
         <v>9</v>
       </c>
       <c r="C326">
-        <f t="shared" ref="C326" si="558">SUM(D326:F326)</f>
+        <f t="shared" ref="C326" si="491">SUM(D326:F326)</f>
         <v>1673</v>
       </c>
       <c r="D326">
@@ -28612,8 +28237,8 @@
         <v>112</v>
       </c>
       <c r="H326" s="16">
-        <f>SUM(I326:K326)-SUM(L326:N326)</f>
-        <v>10923</v>
+        <f t="shared" si="486"/>
+        <v>12334</v>
       </c>
       <c r="I326" s="5">
         <v>10000</v>
@@ -28624,15 +28249,9 @@
       <c r="K326" s="7">
         <v>1167</v>
       </c>
-      <c r="L326">
-        <v>1305</v>
-      </c>
-      <c r="M326">
-        <v>86</v>
-      </c>
-      <c r="N326">
-        <v>20</v>
-      </c>
+      <c r="L326" s="22"/>
+      <c r="M326" s="22"/>
+      <c r="N326" s="22"/>
       <c r="O326">
         <v>31</v>
       </c>
@@ -28645,7 +28264,7 @@
         <v>9</v>
       </c>
       <c r="C327">
-        <f t="shared" ref="C327" si="559">SUM(D327:F327)</f>
+        <f t="shared" ref="C327" si="492">SUM(D327:F327)</f>
         <v>1673</v>
       </c>
       <c r="D327">
@@ -28661,28 +28280,65 @@
         <v>112</v>
       </c>
       <c r="H327" s="16">
-        <f>SUM(I327:K327)-SUM(L327:N327)</f>
-        <v>11041</v>
+        <f t="shared" si="486"/>
+        <v>12452</v>
       </c>
       <c r="I327" s="5">
         <v>10069</v>
       </c>
-      <c r="J327" s="7">
+      <c r="J327" s="6">
         <v>1209</v>
       </c>
       <c r="K327" s="7">
         <v>1174</v>
       </c>
-      <c r="L327">
-        <v>1305</v>
-      </c>
-      <c r="M327">
-        <v>86</v>
-      </c>
-      <c r="N327">
-        <v>20</v>
-      </c>
+      <c r="L327" s="22"/>
+      <c r="M327" s="22"/>
+      <c r="N327" s="22"/>
       <c r="O327">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>46025</v>
+      </c>
+      <c r="B328" s="2">
+        <v>9</v>
+      </c>
+      <c r="C328">
+        <f t="shared" ref="C328" si="493">SUM(D328:F328)</f>
+        <v>1673</v>
+      </c>
+      <c r="D328">
+        <v>1105</v>
+      </c>
+      <c r="E328">
+        <v>371</v>
+      </c>
+      <c r="F328" s="3">
+        <v>197</v>
+      </c>
+      <c r="G328" s="4">
+        <v>113</v>
+      </c>
+      <c r="H328" s="16">
+        <f t="shared" ref="H328" si="494">SUM(I328:K328)</f>
+        <v>12445</v>
+      </c>
+      <c r="I328" s="5">
+        <v>10054</v>
+      </c>
+      <c r="J328" s="6">
+        <v>1214</v>
+      </c>
+      <c r="K328" s="7">
+        <v>1177</v>
+      </c>
+      <c r="L328" s="22"/>
+      <c r="M328" s="22"/>
+      <c r="N328" s="22"/>
+      <c r="O328">
         <v>31</v>
       </c>
     </row>
@@ -28705,7 +28361,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB47" sqref="AB47"/>
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactored Level1JsonReader into 2 files
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F63E3CB-8A18-E54D-853C-0F92329A926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207CE0FD-17AF-FA4A-B74F-D8E677467207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -194,6 +194,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -203,7 +204,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -1270,7 +1270,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2258,6 +2261,9 @@
                 </c:pt>
                 <c:pt idx="325" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12445</c:v>
+                </c:pt>
+                <c:pt idx="326" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3281,7 +3287,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4269,6 +4278,9 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>10054</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>10089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5294,7 +5306,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6282,6 +6297,9 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>1214</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>1209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7326,7 +7344,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8314,6 +8335,9 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>1177</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>1181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9721,7 +9745,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10709,6 +10736,9 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11735,7 +11765,10 @@
                   <c:v>46025</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>46025</c:v>
+                  <c:v>46026</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>46028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12722,6 +12755,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="325">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="326">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14550,13 +14586,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q328"/>
+  <dimension ref="A1:Q329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B296" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J332" sqref="J332"/>
+      <selection pane="bottomRight" activeCell="J330" sqref="J330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14573,25 +14609,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="19" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="19" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
       <c r="O1" s="17" t="s">
         <v>9</v>
       </c>
@@ -25239,9 +25275,9 @@
       <c r="K256" s="7">
         <v>700</v>
       </c>
-      <c r="L256" s="22"/>
-      <c r="M256" s="22"/>
-      <c r="N256" s="22"/>
+      <c r="L256" s="19"/>
+      <c r="M256" s="19"/>
+      <c r="N256" s="19"/>
       <c r="O256">
         <v>0</v>
       </c>
@@ -25282,9 +25318,9 @@
       <c r="K257" s="7">
         <v>700</v>
       </c>
-      <c r="L257" s="22"/>
-      <c r="M257" s="22"/>
-      <c r="N257" s="22"/>
+      <c r="L257" s="19"/>
+      <c r="M257" s="19"/>
+      <c r="N257" s="19"/>
       <c r="O257">
         <v>0</v>
       </c>
@@ -25325,9 +25361,9 @@
       <c r="K258" s="7">
         <v>696</v>
       </c>
-      <c r="L258" s="22"/>
-      <c r="M258" s="22"/>
-      <c r="N258" s="22"/>
+      <c r="L258" s="19"/>
+      <c r="M258" s="19"/>
+      <c r="N258" s="19"/>
       <c r="O258">
         <v>0</v>
       </c>
@@ -25368,9 +25404,9 @@
       <c r="K259" s="7">
         <v>696</v>
       </c>
-      <c r="L259" s="22"/>
-      <c r="M259" s="22"/>
-      <c r="N259" s="22"/>
+      <c r="L259" s="19"/>
+      <c r="M259" s="19"/>
+      <c r="N259" s="19"/>
       <c r="O259">
         <v>0</v>
       </c>
@@ -25411,9 +25447,9 @@
       <c r="K260" s="7">
         <v>698</v>
       </c>
-      <c r="L260" s="22"/>
-      <c r="M260" s="22"/>
-      <c r="N260" s="22"/>
+      <c r="L260" s="19"/>
+      <c r="M260" s="19"/>
+      <c r="N260" s="19"/>
       <c r="O260">
         <v>0</v>
       </c>
@@ -25454,9 +25490,9 @@
       <c r="K261" s="7">
         <v>679</v>
       </c>
-      <c r="L261" s="22"/>
-      <c r="M261" s="22"/>
-      <c r="N261" s="22"/>
+      <c r="L261" s="19"/>
+      <c r="M261" s="19"/>
+      <c r="N261" s="19"/>
       <c r="O261">
         <v>0</v>
       </c>
@@ -25497,9 +25533,9 @@
       <c r="K262" s="7">
         <v>683</v>
       </c>
-      <c r="L262" s="22"/>
-      <c r="M262" s="22"/>
-      <c r="N262" s="22"/>
+      <c r="L262" s="19"/>
+      <c r="M262" s="19"/>
+      <c r="N262" s="19"/>
       <c r="O262">
         <v>0</v>
       </c>
@@ -25540,9 +25576,9 @@
       <c r="K263" s="7">
         <v>648</v>
       </c>
-      <c r="L263" s="22"/>
-      <c r="M263" s="22"/>
-      <c r="N263" s="22"/>
+      <c r="L263" s="19"/>
+      <c r="M263" s="19"/>
+      <c r="N263" s="19"/>
       <c r="O263">
         <v>0</v>
       </c>
@@ -25583,9 +25619,9 @@
       <c r="K264" s="7">
         <v>644</v>
       </c>
-      <c r="L264" s="22"/>
-      <c r="M264" s="22"/>
-      <c r="N264" s="22"/>
+      <c r="L264" s="19"/>
+      <c r="M264" s="19"/>
+      <c r="N264" s="19"/>
       <c r="O264">
         <v>0</v>
       </c>
@@ -25626,9 +25662,9 @@
       <c r="K265" s="7">
         <v>642</v>
       </c>
-      <c r="L265" s="22"/>
-      <c r="M265" s="22"/>
-      <c r="N265" s="22"/>
+      <c r="L265" s="19"/>
+      <c r="M265" s="19"/>
+      <c r="N265" s="19"/>
       <c r="O265">
         <v>0</v>
       </c>
@@ -25669,9 +25705,9 @@
       <c r="K266" s="7">
         <v>667</v>
       </c>
-      <c r="L266" s="22"/>
-      <c r="M266" s="22"/>
-      <c r="N266" s="22"/>
+      <c r="L266" s="19"/>
+      <c r="M266" s="19"/>
+      <c r="N266" s="19"/>
       <c r="O266">
         <v>0</v>
       </c>
@@ -25712,9 +25748,9 @@
       <c r="K267" s="7">
         <v>664</v>
       </c>
-      <c r="L267" s="22"/>
-      <c r="M267" s="22"/>
-      <c r="N267" s="22"/>
+      <c r="L267" s="19"/>
+      <c r="M267" s="19"/>
+      <c r="N267" s="19"/>
       <c r="O267">
         <v>0</v>
       </c>
@@ -25755,9 +25791,9 @@
       <c r="K268" s="7">
         <v>664</v>
       </c>
-      <c r="L268" s="22"/>
-      <c r="M268" s="22"/>
-      <c r="N268" s="22"/>
+      <c r="L268" s="19"/>
+      <c r="M268" s="19"/>
+      <c r="N268" s="19"/>
       <c r="O268">
         <v>0</v>
       </c>
@@ -25798,9 +25834,9 @@
       <c r="K269" s="7">
         <v>642</v>
       </c>
-      <c r="L269" s="22"/>
-      <c r="M269" s="22"/>
-      <c r="N269" s="22"/>
+      <c r="L269" s="19"/>
+      <c r="M269" s="19"/>
+      <c r="N269" s="19"/>
       <c r="O269">
         <v>0</v>
       </c>
@@ -25841,9 +25877,9 @@
       <c r="K270" s="7">
         <v>673</v>
       </c>
-      <c r="L270" s="22"/>
-      <c r="M270" s="22"/>
-      <c r="N270" s="22"/>
+      <c r="L270" s="19"/>
+      <c r="M270" s="19"/>
+      <c r="N270" s="19"/>
       <c r="O270">
         <v>0</v>
       </c>
@@ -25884,9 +25920,9 @@
       <c r="K271" s="7">
         <v>652</v>
       </c>
-      <c r="L271" s="22"/>
-      <c r="M271" s="22"/>
-      <c r="N271" s="22"/>
+      <c r="L271" s="19"/>
+      <c r="M271" s="19"/>
+      <c r="N271" s="19"/>
       <c r="O271">
         <v>0</v>
       </c>
@@ -25927,9 +25963,9 @@
       <c r="K272" s="7">
         <v>649</v>
       </c>
-      <c r="L272" s="22"/>
-      <c r="M272" s="22"/>
-      <c r="N272" s="22"/>
+      <c r="L272" s="19"/>
+      <c r="M272" s="19"/>
+      <c r="N272" s="19"/>
       <c r="O272">
         <v>0</v>
       </c>
@@ -25970,9 +26006,9 @@
       <c r="K273" s="7">
         <v>653</v>
       </c>
-      <c r="L273" s="22"/>
-      <c r="M273" s="22"/>
-      <c r="N273" s="22"/>
+      <c r="L273" s="19"/>
+      <c r="M273" s="19"/>
+      <c r="N273" s="19"/>
       <c r="O273">
         <v>0</v>
       </c>
@@ -26013,9 +26049,9 @@
       <c r="K274" s="7">
         <v>743</v>
       </c>
-      <c r="L274" s="22"/>
-      <c r="M274" s="22"/>
-      <c r="N274" s="22"/>
+      <c r="L274" s="19"/>
+      <c r="M274" s="19"/>
+      <c r="N274" s="19"/>
       <c r="O274">
         <v>9</v>
       </c>
@@ -26056,9 +26092,9 @@
       <c r="K275" s="7">
         <v>737</v>
       </c>
-      <c r="L275" s="22"/>
-      <c r="M275" s="22"/>
-      <c r="N275" s="22"/>
+      <c r="L275" s="19"/>
+      <c r="M275" s="19"/>
+      <c r="N275" s="19"/>
       <c r="O275">
         <v>12</v>
       </c>
@@ -26099,9 +26135,9 @@
       <c r="K276" s="7">
         <v>750</v>
       </c>
-      <c r="L276" s="22"/>
-      <c r="M276" s="22"/>
-      <c r="N276" s="22"/>
+      <c r="L276" s="19"/>
+      <c r="M276" s="19"/>
+      <c r="N276" s="19"/>
       <c r="O276">
         <v>14</v>
       </c>
@@ -26142,9 +26178,9 @@
       <c r="K277" s="7">
         <v>764</v>
       </c>
-      <c r="L277" s="22"/>
-      <c r="M277" s="22"/>
-      <c r="N277" s="22"/>
+      <c r="L277" s="19"/>
+      <c r="M277" s="19"/>
+      <c r="N277" s="19"/>
       <c r="O277">
         <v>14</v>
       </c>
@@ -26185,9 +26221,9 @@
       <c r="K278" s="7">
         <v>763</v>
       </c>
-      <c r="L278" s="22"/>
-      <c r="M278" s="22"/>
-      <c r="N278" s="22"/>
+      <c r="L278" s="19"/>
+      <c r="M278" s="19"/>
+      <c r="N278" s="19"/>
       <c r="O278">
         <v>14</v>
       </c>
@@ -26228,9 +26264,9 @@
       <c r="K279" s="7">
         <v>777</v>
       </c>
-      <c r="L279" s="22"/>
-      <c r="M279" s="22"/>
-      <c r="N279" s="22"/>
+      <c r="L279" s="19"/>
+      <c r="M279" s="19"/>
+      <c r="N279" s="19"/>
       <c r="O279">
         <v>15</v>
       </c>
@@ -26271,9 +26307,9 @@
       <c r="K280" s="7">
         <v>782</v>
       </c>
-      <c r="L280" s="22"/>
-      <c r="M280" s="22"/>
-      <c r="N280" s="22"/>
+      <c r="L280" s="19"/>
+      <c r="M280" s="19"/>
+      <c r="N280" s="19"/>
       <c r="O280">
         <v>15</v>
       </c>
@@ -26314,9 +26350,9 @@
       <c r="K281" s="7">
         <v>801</v>
       </c>
-      <c r="L281" s="22"/>
-      <c r="M281" s="22"/>
-      <c r="N281" s="22"/>
+      <c r="L281" s="19"/>
+      <c r="M281" s="19"/>
+      <c r="N281" s="19"/>
       <c r="O281">
         <v>17</v>
       </c>
@@ -26357,9 +26393,9 @@
       <c r="K282" s="7">
         <v>823</v>
       </c>
-      <c r="L282" s="22"/>
-      <c r="M282" s="22"/>
-      <c r="N282" s="22"/>
+      <c r="L282" s="19"/>
+      <c r="M282" s="19"/>
+      <c r="N282" s="19"/>
       <c r="O282">
         <v>19</v>
       </c>
@@ -26400,9 +26436,9 @@
       <c r="K283" s="7">
         <v>823</v>
       </c>
-      <c r="L283" s="22"/>
-      <c r="M283" s="22"/>
-      <c r="N283" s="22"/>
+      <c r="L283" s="19"/>
+      <c r="M283" s="19"/>
+      <c r="N283" s="19"/>
       <c r="O283">
         <v>19</v>
       </c>
@@ -26443,9 +26479,9 @@
       <c r="K284" s="7">
         <v>826</v>
       </c>
-      <c r="L284" s="22"/>
-      <c r="M284" s="22"/>
-      <c r="N284" s="22"/>
+      <c r="L284" s="19"/>
+      <c r="M284" s="19"/>
+      <c r="N284" s="19"/>
       <c r="O284">
         <v>20</v>
       </c>
@@ -26486,9 +26522,9 @@
       <c r="K285" s="7">
         <v>849</v>
       </c>
-      <c r="L285" s="22"/>
-      <c r="M285" s="22"/>
-      <c r="N285" s="22"/>
+      <c r="L285" s="19"/>
+      <c r="M285" s="19"/>
+      <c r="N285" s="19"/>
       <c r="O285">
         <v>22</v>
       </c>
@@ -26529,9 +26565,9 @@
       <c r="K286" s="7">
         <v>845</v>
       </c>
-      <c r="L286" s="22"/>
-      <c r="M286" s="22"/>
-      <c r="N286" s="22"/>
+      <c r="L286" s="19"/>
+      <c r="M286" s="19"/>
+      <c r="N286" s="19"/>
       <c r="O286">
         <v>22</v>
       </c>
@@ -26572,9 +26608,9 @@
       <c r="K287" s="7">
         <v>851</v>
       </c>
-      <c r="L287" s="22"/>
-      <c r="M287" s="22"/>
-      <c r="N287" s="22"/>
+      <c r="L287" s="19"/>
+      <c r="M287" s="19"/>
+      <c r="N287" s="19"/>
       <c r="O287">
         <v>22</v>
       </c>
@@ -26615,9 +26651,9 @@
       <c r="K288" s="7">
         <v>856</v>
       </c>
-      <c r="L288" s="22"/>
-      <c r="M288" s="22"/>
-      <c r="N288" s="22"/>
+      <c r="L288" s="19"/>
+      <c r="M288" s="19"/>
+      <c r="N288" s="19"/>
       <c r="O288">
         <v>22</v>
       </c>
@@ -26658,9 +26694,9 @@
       <c r="K289" s="7">
         <v>856</v>
       </c>
-      <c r="L289" s="22"/>
-      <c r="M289" s="22"/>
-      <c r="N289" s="22"/>
+      <c r="L289" s="19"/>
+      <c r="M289" s="19"/>
+      <c r="N289" s="19"/>
       <c r="O289">
         <v>22</v>
       </c>
@@ -26701,9 +26737,9 @@
       <c r="K290" s="7">
         <v>829</v>
       </c>
-      <c r="L290" s="22"/>
-      <c r="M290" s="22"/>
-      <c r="N290" s="22"/>
+      <c r="L290" s="19"/>
+      <c r="M290" s="19"/>
+      <c r="N290" s="19"/>
       <c r="O290">
         <v>23</v>
       </c>
@@ -26744,9 +26780,9 @@
       <c r="K291" s="7">
         <v>829</v>
       </c>
-      <c r="L291" s="22"/>
-      <c r="M291" s="22"/>
-      <c r="N291" s="22"/>
+      <c r="L291" s="19"/>
+      <c r="M291" s="19"/>
+      <c r="N291" s="19"/>
       <c r="O291">
         <v>23</v>
       </c>
@@ -26787,9 +26823,9 @@
       <c r="K292" s="7">
         <v>844</v>
       </c>
-      <c r="L292" s="22"/>
-      <c r="M292" s="22"/>
-      <c r="N292" s="22"/>
+      <c r="L292" s="19"/>
+      <c r="M292" s="19"/>
+      <c r="N292" s="19"/>
       <c r="O292">
         <v>23</v>
       </c>
@@ -26830,9 +26866,9 @@
       <c r="K293" s="7">
         <v>863</v>
       </c>
-      <c r="L293" s="22"/>
-      <c r="M293" s="22"/>
-      <c r="N293" s="22"/>
+      <c r="L293" s="19"/>
+      <c r="M293" s="19"/>
+      <c r="N293" s="19"/>
       <c r="O293">
         <v>23</v>
       </c>
@@ -26873,9 +26909,9 @@
       <c r="K294" s="7">
         <v>890</v>
       </c>
-      <c r="L294" s="22"/>
-      <c r="M294" s="22"/>
-      <c r="N294" s="22"/>
+      <c r="L294" s="19"/>
+      <c r="M294" s="19"/>
+      <c r="N294" s="19"/>
       <c r="O294">
         <v>23</v>
       </c>
@@ -26916,9 +26952,9 @@
       <c r="K295" s="7">
         <v>913</v>
       </c>
-      <c r="L295" s="22"/>
-      <c r="M295" s="22"/>
-      <c r="N295" s="22"/>
+      <c r="L295" s="19"/>
+      <c r="M295" s="19"/>
+      <c r="N295" s="19"/>
       <c r="O295">
         <v>23</v>
       </c>
@@ -26959,9 +26995,9 @@
       <c r="K296" s="7">
         <v>924</v>
       </c>
-      <c r="L296" s="22"/>
-      <c r="M296" s="22"/>
-      <c r="N296" s="22"/>
+      <c r="L296" s="19"/>
+      <c r="M296" s="19"/>
+      <c r="N296" s="19"/>
       <c r="O296">
         <v>23</v>
       </c>
@@ -27002,9 +27038,9 @@
       <c r="K297" s="7">
         <v>929</v>
       </c>
-      <c r="L297" s="22"/>
-      <c r="M297" s="22"/>
-      <c r="N297" s="22"/>
+      <c r="L297" s="19"/>
+      <c r="M297" s="19"/>
+      <c r="N297" s="19"/>
       <c r="O297">
         <v>23</v>
       </c>
@@ -27045,9 +27081,9 @@
       <c r="K298" s="7">
         <v>941</v>
       </c>
-      <c r="L298" s="22"/>
-      <c r="M298" s="22"/>
-      <c r="N298" s="22"/>
+      <c r="L298" s="19"/>
+      <c r="M298" s="19"/>
+      <c r="N298" s="19"/>
       <c r="O298">
         <v>23</v>
       </c>
@@ -27088,9 +27124,9 @@
       <c r="K299" s="7">
         <v>946</v>
       </c>
-      <c r="L299" s="22"/>
-      <c r="M299" s="22"/>
-      <c r="N299" s="22"/>
+      <c r="L299" s="19"/>
+      <c r="M299" s="19"/>
+      <c r="N299" s="19"/>
       <c r="O299">
         <v>23</v>
       </c>
@@ -27131,9 +27167,9 @@
       <c r="K300" s="7">
         <v>948</v>
       </c>
-      <c r="L300" s="22"/>
-      <c r="M300" s="22"/>
-      <c r="N300" s="22"/>
+      <c r="L300" s="19"/>
+      <c r="M300" s="19"/>
+      <c r="N300" s="19"/>
       <c r="O300">
         <v>23</v>
       </c>
@@ -27174,9 +27210,9 @@
       <c r="K301" s="7">
         <v>948</v>
       </c>
-      <c r="L301" s="22"/>
-      <c r="M301" s="22"/>
-      <c r="N301" s="22"/>
+      <c r="L301" s="19"/>
+      <c r="M301" s="19"/>
+      <c r="N301" s="19"/>
       <c r="O301">
         <v>23</v>
       </c>
@@ -27217,9 +27253,9 @@
       <c r="K302" s="7">
         <v>951</v>
       </c>
-      <c r="L302" s="22"/>
-      <c r="M302" s="22"/>
-      <c r="N302" s="22"/>
+      <c r="L302" s="19"/>
+      <c r="M302" s="19"/>
+      <c r="N302" s="19"/>
       <c r="O302">
         <v>23</v>
       </c>
@@ -27260,9 +27296,9 @@
       <c r="K303" s="7">
         <v>962</v>
       </c>
-      <c r="L303" s="22"/>
-      <c r="M303" s="22"/>
-      <c r="N303" s="22"/>
+      <c r="L303" s="19"/>
+      <c r="M303" s="19"/>
+      <c r="N303" s="19"/>
       <c r="O303">
         <v>23</v>
       </c>
@@ -27303,9 +27339,9 @@
       <c r="K304" s="7">
         <v>964</v>
       </c>
-      <c r="L304" s="22"/>
-      <c r="M304" s="22"/>
-      <c r="N304" s="22"/>
+      <c r="L304" s="19"/>
+      <c r="M304" s="19"/>
+      <c r="N304" s="19"/>
       <c r="O304">
         <v>23</v>
       </c>
@@ -27346,9 +27382,9 @@
       <c r="K305" s="7">
         <v>964</v>
       </c>
-      <c r="L305" s="22"/>
-      <c r="M305" s="22"/>
-      <c r="N305" s="22"/>
+      <c r="L305" s="19"/>
+      <c r="M305" s="19"/>
+      <c r="N305" s="19"/>
       <c r="O305">
         <v>23</v>
       </c>
@@ -27389,9 +27425,9 @@
       <c r="K306" s="7">
         <v>967</v>
       </c>
-      <c r="L306" s="22"/>
-      <c r="M306" s="22"/>
-      <c r="N306" s="22"/>
+      <c r="L306" s="19"/>
+      <c r="M306" s="19"/>
+      <c r="N306" s="19"/>
       <c r="O306">
         <v>23</v>
       </c>
@@ -27432,9 +27468,9 @@
       <c r="K307" s="7">
         <v>973</v>
       </c>
-      <c r="L307" s="22"/>
-      <c r="M307" s="22"/>
-      <c r="N307" s="22"/>
+      <c r="L307" s="19"/>
+      <c r="M307" s="19"/>
+      <c r="N307" s="19"/>
       <c r="O307">
         <v>23</v>
       </c>
@@ -27475,9 +27511,9 @@
       <c r="K308" s="7">
         <v>968</v>
       </c>
-      <c r="L308" s="22"/>
-      <c r="M308" s="22"/>
-      <c r="N308" s="22"/>
+      <c r="L308" s="19"/>
+      <c r="M308" s="19"/>
+      <c r="N308" s="19"/>
       <c r="O308">
         <v>23</v>
       </c>
@@ -27518,9 +27554,9 @@
       <c r="K309" s="7">
         <v>986</v>
       </c>
-      <c r="L309" s="22"/>
-      <c r="M309" s="22"/>
-      <c r="N309" s="22"/>
+      <c r="L309" s="19"/>
+      <c r="M309" s="19"/>
+      <c r="N309" s="19"/>
       <c r="O309">
         <v>24</v>
       </c>
@@ -27561,9 +27597,9 @@
       <c r="K310" s="7">
         <v>958</v>
       </c>
-      <c r="L310" s="22"/>
-      <c r="M310" s="22"/>
-      <c r="N310" s="22"/>
+      <c r="L310" s="19"/>
+      <c r="M310" s="19"/>
+      <c r="N310" s="19"/>
       <c r="O310">
         <v>24</v>
       </c>
@@ -27604,9 +27640,9 @@
       <c r="K311" s="7">
         <v>1043</v>
       </c>
-      <c r="L311" s="22"/>
-      <c r="M311" s="22"/>
-      <c r="N311" s="22"/>
+      <c r="L311" s="19"/>
+      <c r="M311" s="19"/>
+      <c r="N311" s="19"/>
       <c r="O311">
         <v>24</v>
       </c>
@@ -27647,9 +27683,9 @@
       <c r="K312" s="7">
         <v>1056</v>
       </c>
-      <c r="L312" s="22"/>
-      <c r="M312" s="22"/>
-      <c r="N312" s="22"/>
+      <c r="L312" s="19"/>
+      <c r="M312" s="19"/>
+      <c r="N312" s="19"/>
       <c r="O312">
         <v>31</v>
       </c>
@@ -27690,9 +27726,9 @@
       <c r="K313" s="7">
         <v>1068</v>
       </c>
-      <c r="L313" s="22"/>
-      <c r="M313" s="22"/>
-      <c r="N313" s="22"/>
+      <c r="L313" s="19"/>
+      <c r="M313" s="19"/>
+      <c r="N313" s="19"/>
       <c r="O313">
         <v>31</v>
       </c>
@@ -27733,9 +27769,9 @@
       <c r="K314" s="7">
         <v>1069</v>
       </c>
-      <c r="L314" s="22"/>
-      <c r="M314" s="22"/>
-      <c r="N314" s="22"/>
+      <c r="L314" s="19"/>
+      <c r="M314" s="19"/>
+      <c r="N314" s="19"/>
       <c r="O314">
         <v>31</v>
       </c>
@@ -27776,9 +27812,9 @@
       <c r="K315" s="7">
         <v>1033</v>
       </c>
-      <c r="L315" s="22"/>
-      <c r="M315" s="22"/>
-      <c r="N315" s="22"/>
+      <c r="L315" s="19"/>
+      <c r="M315" s="19"/>
+      <c r="N315" s="19"/>
       <c r="O315">
         <v>31</v>
       </c>
@@ -27819,9 +27855,9 @@
       <c r="K316" s="7">
         <v>1033</v>
       </c>
-      <c r="L316" s="22"/>
-      <c r="M316" s="22"/>
-      <c r="N316" s="22"/>
+      <c r="L316" s="19"/>
+      <c r="M316" s="19"/>
+      <c r="N316" s="19"/>
       <c r="O316">
         <v>31</v>
       </c>
@@ -27862,9 +27898,9 @@
       <c r="K317" s="7">
         <v>1056</v>
       </c>
-      <c r="L317" s="22"/>
-      <c r="M317" s="22"/>
-      <c r="N317" s="22"/>
+      <c r="L317" s="19"/>
+      <c r="M317" s="19"/>
+      <c r="N317" s="19"/>
       <c r="O317">
         <v>31</v>
       </c>
@@ -27905,9 +27941,9 @@
       <c r="K318" s="7">
         <v>1060</v>
       </c>
-      <c r="L318" s="22"/>
-      <c r="M318" s="22"/>
-      <c r="N318" s="22"/>
+      <c r="L318" s="19"/>
+      <c r="M318" s="19"/>
+      <c r="N318" s="19"/>
       <c r="O318">
         <v>31</v>
       </c>
@@ -27948,9 +27984,9 @@
       <c r="K319" s="7">
         <v>1065</v>
       </c>
-      <c r="L319" s="22"/>
-      <c r="M319" s="22"/>
-      <c r="N319" s="22"/>
+      <c r="L319" s="19"/>
+      <c r="M319" s="19"/>
+      <c r="N319" s="19"/>
       <c r="O319">
         <v>31</v>
       </c>
@@ -27991,9 +28027,9 @@
       <c r="K320" s="7">
         <v>1071</v>
       </c>
-      <c r="L320" s="22"/>
-      <c r="M320" s="22"/>
-      <c r="N320" s="22"/>
+      <c r="L320" s="19"/>
+      <c r="M320" s="19"/>
+      <c r="N320" s="19"/>
       <c r="O320">
         <v>31</v>
       </c>
@@ -28034,9 +28070,9 @@
       <c r="K321" s="7">
         <v>1096</v>
       </c>
-      <c r="L321" s="22"/>
-      <c r="M321" s="22"/>
-      <c r="N321" s="22"/>
+      <c r="L321" s="19"/>
+      <c r="M321" s="19"/>
+      <c r="N321" s="19"/>
       <c r="O321">
         <v>31</v>
       </c>
@@ -28077,9 +28113,9 @@
       <c r="K322" s="7">
         <v>1106</v>
       </c>
-      <c r="L322" s="22"/>
-      <c r="M322" s="22"/>
-      <c r="N322" s="22"/>
+      <c r="L322" s="19"/>
+      <c r="M322" s="19"/>
+      <c r="N322" s="19"/>
       <c r="O322">
         <v>31</v>
       </c>
@@ -28120,9 +28156,9 @@
       <c r="K323" s="7">
         <v>1118</v>
       </c>
-      <c r="L323" s="22"/>
-      <c r="M323" s="22"/>
-      <c r="N323" s="22"/>
+      <c r="L323" s="19"/>
+      <c r="M323" s="19"/>
+      <c r="N323" s="19"/>
       <c r="O323">
         <v>31</v>
       </c>
@@ -28163,9 +28199,9 @@
       <c r="K324" s="7">
         <v>1150</v>
       </c>
-      <c r="L324" s="22"/>
-      <c r="M324" s="22"/>
-      <c r="N324" s="22"/>
+      <c r="L324" s="19"/>
+      <c r="M324" s="19"/>
+      <c r="N324" s="19"/>
       <c r="O324">
         <v>31</v>
       </c>
@@ -28206,9 +28242,9 @@
       <c r="K325" s="7">
         <v>1158</v>
       </c>
-      <c r="L325" s="22"/>
-      <c r="M325" s="22"/>
-      <c r="N325" s="22"/>
+      <c r="L325" s="19"/>
+      <c r="M325" s="19"/>
+      <c r="N325" s="19"/>
       <c r="O325">
         <v>31</v>
       </c>
@@ -28249,9 +28285,9 @@
       <c r="K326" s="7">
         <v>1167</v>
       </c>
-      <c r="L326" s="22"/>
-      <c r="M326" s="22"/>
-      <c r="N326" s="22"/>
+      <c r="L326" s="19"/>
+      <c r="M326" s="19"/>
+      <c r="N326" s="19"/>
       <c r="O326">
         <v>31</v>
       </c>
@@ -28292,16 +28328,16 @@
       <c r="K327" s="7">
         <v>1174</v>
       </c>
-      <c r="L327" s="22"/>
-      <c r="M327" s="22"/>
-      <c r="N327" s="22"/>
+      <c r="L327" s="19"/>
+      <c r="M327" s="19"/>
+      <c r="N327" s="19"/>
       <c r="O327">
         <v>31</v>
       </c>
     </row>
     <row r="328" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
-        <v>46025</v>
+        <v>46026</v>
       </c>
       <c r="B328" s="2">
         <v>9</v>
@@ -28335,10 +28371,53 @@
       <c r="K328" s="7">
         <v>1177</v>
       </c>
-      <c r="L328" s="22"/>
-      <c r="M328" s="22"/>
-      <c r="N328" s="22"/>
+      <c r="L328" s="19"/>
+      <c r="M328" s="19"/>
+      <c r="N328" s="19"/>
       <c r="O328">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B329" s="2">
+        <v>9</v>
+      </c>
+      <c r="C329">
+        <f t="shared" ref="C329" si="495">SUM(D329:F329)</f>
+        <v>1673</v>
+      </c>
+      <c r="D329">
+        <v>1105</v>
+      </c>
+      <c r="E329">
+        <v>371</v>
+      </c>
+      <c r="F329" s="3">
+        <v>197</v>
+      </c>
+      <c r="G329" s="4">
+        <v>114</v>
+      </c>
+      <c r="H329" s="16">
+        <f t="shared" ref="H329" si="496">SUM(I329:K329)</f>
+        <v>12479</v>
+      </c>
+      <c r="I329" s="5">
+        <v>10089</v>
+      </c>
+      <c r="J329" s="6">
+        <v>1209</v>
+      </c>
+      <c r="K329" s="7">
+        <v>1181</v>
+      </c>
+      <c r="L329" s="19"/>
+      <c r="M329" s="19"/>
+      <c r="N329" s="19"/>
+      <c r="O329">
         <v>31</v>
       </c>
     </row>
@@ -28360,7 +28439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #668 added fcVeghel (for possible future onboarding)
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207CE0FD-17AF-FA4A-B74F-D8E677467207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43F662-6C89-7347-BB57-4ACEDB04B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1275,6 +1275,9 @@
                 <c:pt idx="326">
                   <c:v>46028</c:v>
                 </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2264,6 +2267,9 @@
                 </c:pt>
                 <c:pt idx="326" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12479</c:v>
+                </c:pt>
+                <c:pt idx="327" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3291,6 +3297,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>46028</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5310,6 +5319,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>46028</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7348,6 +7360,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>46028</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9750,6 +9765,9 @@
                 <c:pt idx="326">
                   <c:v>46028</c:v>
                 </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10739,6 +10757,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11770,6 +11791,9 @@
                 <c:pt idx="326">
                   <c:v>46028</c:v>
                 </c:pt>
+                <c:pt idx="327">
+                  <c:v>46031</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12758,6 +12782,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="326">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="327">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14586,13 +14613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q329"/>
+  <dimension ref="A1:Q330"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J330" sqref="J330"/>
+      <selection pane="bottomRight" activeCell="H335" sqref="H335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28421,6 +28448,40 @@
         <v>31</v>
       </c>
     </row>
+    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B330" s="2">
+        <v>9</v>
+      </c>
+      <c r="C330">
+        <f t="shared" ref="C330" si="497">SUM(D330:F330)</f>
+        <v>1673</v>
+      </c>
+      <c r="D330">
+        <v>1105</v>
+      </c>
+      <c r="E330">
+        <v>371</v>
+      </c>
+      <c r="F330" s="3">
+        <v>197</v>
+      </c>
+      <c r="G330" s="4">
+        <v>115</v>
+      </c>
+      <c r="H330" s="16">
+        <f t="shared" ref="H330" si="498">SUM(I330:K330)</f>
+        <v>0</v>
+      </c>
+      <c r="L330" s="19"/>
+      <c r="M330" s="19"/>
+      <c r="N330" s="19"/>
+      <c r="O330">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -28439,7 +28500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #669 Added toggels for Clubs and Musueums to Preferences
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43F662-6C89-7347-BB57-4ACEDB04B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5C6D2-7143-FC4F-AFA6-B891DE959C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -2269,7 +2269,7 @@
                   <c:v>12479</c:v>
                 </c:pt>
                 <c:pt idx="327" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
-                  <c:v>0</c:v>
+                  <c:v>12611</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4290,6 +4290,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>10089</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>10185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6312,6 +6315,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>1209</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>1223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8353,6 +8359,9 @@
                 </c:pt>
                 <c:pt idx="326">
                   <c:v>1181</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>1203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14615,11 +14624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:Q330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H335" sqref="H335"/>
+      <selection pane="bottomRight" activeCell="I331" sqref="I331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28473,7 +28482,16 @@
       </c>
       <c r="H330" s="16">
         <f t="shared" ref="H330" si="498">SUM(I330:K330)</f>
-        <v>0</v>
+        <v>12611</v>
+      </c>
+      <c r="I330" s="5">
+        <v>10185</v>
+      </c>
+      <c r="J330" s="6">
+        <v>1223</v>
+      </c>
+      <c r="K330" s="7">
+        <v>1203</v>
       </c>
       <c r="L330" s="19"/>
       <c r="M330" s="19"/>
@@ -28500,7 +28518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: 672 Increased size of Preferences screen on iPad
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5C6D2-7143-FC4F-AFA6-B891DE959C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE34F8EB-1DF6-3A40-A937-5110A790B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="27780" windowHeight="26400" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1278,6 +1278,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2270,6 +2273,9 @@
                 </c:pt>
                 <c:pt idx="327" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12611</c:v>
+                </c:pt>
+                <c:pt idx="328" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3301,6 +3307,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4293,6 +4302,9 @@
                 </c:pt>
                 <c:pt idx="327">
                   <c:v>10185</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>10239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5326,6 +5338,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6318,6 +6333,9 @@
                 </c:pt>
                 <c:pt idx="327">
                   <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7370,6 +7388,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8362,6 +8383,9 @@
                 </c:pt>
                 <c:pt idx="327">
                   <c:v>1203</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9777,6 +9801,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10769,6 +10796,9 @@
                 </c:pt>
                 <c:pt idx="327">
                   <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11803,6 +11833,9 @@
                 <c:pt idx="327">
                   <c:v>46031</c:v>
                 </c:pt>
+                <c:pt idx="328">
+                  <c:v>46032</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12794,6 +12827,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="327">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="328">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14622,13 +14658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q330"/>
+  <dimension ref="A1:Q331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I331" sqref="I331"/>
+      <selection pane="bottomRight" activeCell="N341" sqref="N341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28497,6 +28533,49 @@
       <c r="M330" s="19"/>
       <c r="N330" s="19"/>
       <c r="O330">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>46032</v>
+      </c>
+      <c r="B331" s="2">
+        <v>9</v>
+      </c>
+      <c r="C331">
+        <f t="shared" ref="C331" si="499">SUM(D331:F331)</f>
+        <v>1673</v>
+      </c>
+      <c r="D331">
+        <v>1105</v>
+      </c>
+      <c r="E331">
+        <v>371</v>
+      </c>
+      <c r="F331" s="3">
+        <v>197</v>
+      </c>
+      <c r="G331" s="4">
+        <v>116</v>
+      </c>
+      <c r="H331" s="16">
+        <f t="shared" ref="H331" si="500">SUM(I331:K331)</f>
+        <v>12674</v>
+      </c>
+      <c r="I331" s="5">
+        <v>10239</v>
+      </c>
+      <c r="J331" s="6">
+        <v>1229</v>
+      </c>
+      <c r="K331" s="7">
+        <v>1206</v>
+      </c>
+      <c r="L331" s="19"/>
+      <c r="M331" s="19"/>
+      <c r="N331" s="19"/>
+      <c r="O331">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created ffcShot71.level2.json and associated Swift file.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBF5683-B85A-7B44-BC0D-94A8AE92CFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BB2FDE-7D17-FF48-A4C2-A573F5C352FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="27780" windowHeight="26400" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1281,6 +1281,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2276,6 +2279,9 @@
                 </c:pt>
                 <c:pt idx="328" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12673</c:v>
+                </c:pt>
+                <c:pt idx="329" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3310,6 +3316,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4305,6 +4314,9 @@
                 </c:pt>
                 <c:pt idx="328">
                   <c:v>10237</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>10292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5341,6 +5353,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6336,6 +6351,9 @@
                 </c:pt>
                 <c:pt idx="328">
                   <c:v>1229</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1236</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7391,6 +7409,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8386,6 +8407,9 @@
                 </c:pt>
                 <c:pt idx="328">
                   <c:v>1207</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9804,6 +9828,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10799,6 +10826,9 @@
                 </c:pt>
                 <c:pt idx="328">
                   <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11836,6 +11866,9 @@
                 <c:pt idx="328">
                   <c:v>46032</c:v>
                 </c:pt>
+                <c:pt idx="329">
+                  <c:v>46046</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12830,6 +12863,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="328">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="329">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14658,13 +14694,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q331"/>
+  <dimension ref="A1:Q332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I332" sqref="I332"/>
+      <selection pane="bottomRight" activeCell="K333" sqref="K333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28576,6 +28612,49 @@
       <c r="M331" s="19"/>
       <c r="N331" s="19"/>
       <c r="O331">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>46046</v>
+      </c>
+      <c r="B332" s="2">
+        <v>9</v>
+      </c>
+      <c r="C332">
+        <f t="shared" ref="C332" si="501">SUM(D332:F332)</f>
+        <v>1673</v>
+      </c>
+      <c r="D332">
+        <v>1105</v>
+      </c>
+      <c r="E332">
+        <v>371</v>
+      </c>
+      <c r="F332" s="3">
+        <v>197</v>
+      </c>
+      <c r="G332" s="4">
+        <v>117</v>
+      </c>
+      <c r="H332" s="16">
+        <f t="shared" ref="H332" si="502">SUM(I332:K332)</f>
+        <v>12746</v>
+      </c>
+      <c r="I332" s="5">
+        <v>10292</v>
+      </c>
+      <c r="J332" s="6">
+        <v>1236</v>
+      </c>
+      <c r="K332" s="7">
+        <v>1218</v>
+      </c>
+      <c r="L332" s="19"/>
+      <c r="M332" s="19"/>
+      <c r="N332" s="19"/>
+      <c r="O332">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Title of "Clubs and Museums" screen now adapts to whatever is being shown (e.g. "Clubs", "Museums", "Clubs and Museums").
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71866BAC-11A8-FC40-ADC1-CC47ACBBD562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3805E240-32BD-004A-993E-438564420AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="27780" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1287,6 +1287,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2288,6 +2291,9 @@
                 </c:pt>
                 <c:pt idx="330" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12818</c:v>
+                </c:pt>
+                <c:pt idx="331" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3328,6 +3334,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4329,6 +4338,9 @@
                 </c:pt>
                 <c:pt idx="330">
                   <c:v>10346</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>10387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5371,6 +5383,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6371,6 +6386,9 @@
                   <c:v>1236</c:v>
                 </c:pt>
                 <c:pt idx="330">
+                  <c:v>1243</c:v>
+                </c:pt>
+                <c:pt idx="331">
                   <c:v>1243</c:v>
                 </c:pt>
               </c:numCache>
@@ -7433,6 +7451,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8433,6 +8454,9 @@
                   <c:v>1218</c:v>
                 </c:pt>
                 <c:pt idx="330">
+                  <c:v>1229</c:v>
+                </c:pt>
+                <c:pt idx="331">
                   <c:v>1229</c:v>
                 </c:pt>
               </c:numCache>
@@ -9858,6 +9882,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10858,6 +10885,9 @@
                   <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="330">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="331">
                   <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
@@ -11902,6 +11932,9 @@
                 <c:pt idx="330">
                   <c:v>46052</c:v>
                 </c:pt>
+                <c:pt idx="331">
+                  <c:v>46053</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12902,6 +12935,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="330">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="331">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14730,13 +14766,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q333"/>
+  <dimension ref="A1:Q334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O344" sqref="O344"/>
+      <selection pane="bottomRight" activeCell="I335" sqref="I335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28737,6 +28773,49 @@
         <v>31</v>
       </c>
     </row>
+    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>46053</v>
+      </c>
+      <c r="B334" s="2">
+        <v>9</v>
+      </c>
+      <c r="C334">
+        <f t="shared" ref="C334" si="505">SUM(D334:F334)</f>
+        <v>1673</v>
+      </c>
+      <c r="D334">
+        <v>1105</v>
+      </c>
+      <c r="E334">
+        <v>371</v>
+      </c>
+      <c r="F334" s="3">
+        <v>197</v>
+      </c>
+      <c r="G334" s="4">
+        <v>119</v>
+      </c>
+      <c r="H334" s="16">
+        <f t="shared" ref="H334" si="506">SUM(I334:K334)</f>
+        <v>12859</v>
+      </c>
+      <c r="I334" s="5">
+        <v>10387</v>
+      </c>
+      <c r="J334" s="6">
+        <v>1243</v>
+      </c>
+      <c r="K334" s="7">
+        <v>1229</v>
+      </c>
+      <c r="L334" s="19"/>
+      <c r="M334" s="19"/>
+      <c r="N334" s="19"/>
+      <c r="O334">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
@@ -28755,7 +28834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Members to ElementTypeEnum. Although it is not current used.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3805E240-32BD-004A-993E-438564420AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758CA991-97D6-2849-ADCE-1D16B683C21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="27780" windowHeight="16660" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1290,6 +1290,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2294,6 +2297,9 @@
                 </c:pt>
                 <c:pt idx="331" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>12859</c:v>
+                </c:pt>
+                <c:pt idx="332" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>12855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3337,6 +3343,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4341,6 +4350,9 @@
                 </c:pt>
                 <c:pt idx="331">
                   <c:v>10387</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>10375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5386,6 +5398,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6390,6 +6405,9 @@
                 </c:pt>
                 <c:pt idx="331">
                   <c:v>1243</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7454,6 +7472,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8457,6 +8478,9 @@
                   <c:v>1229</c:v>
                 </c:pt>
                 <c:pt idx="331">
+                  <c:v>1229</c:v>
+                </c:pt>
+                <c:pt idx="332">
                   <c:v>1229</c:v>
                 </c:pt>
               </c:numCache>
@@ -9885,6 +9909,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10888,6 +10915,9 @@
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="331">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="332">
                   <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
@@ -11935,6 +11965,9 @@
                 <c:pt idx="331">
                   <c:v>46053</c:v>
                 </c:pt>
+                <c:pt idx="332">
+                  <c:v>46055</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -12938,6 +12971,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="331">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="332">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14766,13 +14802,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q334"/>
+  <dimension ref="A1:Q335"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I335" sqref="I335"/>
+      <selection pane="bottomRight" activeCell="I336" sqref="I336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28813,6 +28849,49 @@
       <c r="M334" s="19"/>
       <c r="N334" s="19"/>
       <c r="O334">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>46055</v>
+      </c>
+      <c r="B335" s="2">
+        <v>9</v>
+      </c>
+      <c r="C335">
+        <f t="shared" ref="C335" si="507">SUM(D335:F335)</f>
+        <v>1673</v>
+      </c>
+      <c r="D335">
+        <v>1105</v>
+      </c>
+      <c r="E335">
+        <v>371</v>
+      </c>
+      <c r="F335" s="3">
+        <v>197</v>
+      </c>
+      <c r="G335" s="4">
+        <v>119</v>
+      </c>
+      <c r="H335" s="16">
+        <f t="shared" ref="H335" si="508">SUM(I335:K335)</f>
+        <v>12855</v>
+      </c>
+      <c r="I335" s="5">
+        <v>10375</v>
+      </c>
+      <c r="J335" s="6">
+        <v>1251</v>
+      </c>
+      <c r="K335" s="7">
+        <v>1229</v>
+      </c>
+      <c r="L335" s="19"/>
+      <c r="M335" s="19"/>
+      <c r="N335" s="19"/>
+      <c r="O335">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: #680 Optional coloring of NL Fotobond clubs.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/LineCount.xlsx
+++ b/Photo Club Hub/Documentation/LineCount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32D5A3F-B2B9-914A-9EC5-D8D0CC2DC414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59069D03-DAB9-4E4D-A456-CD76AB836717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1296,6 +1296,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2306,6 +2309,9 @@
                 </c:pt>
                 <c:pt idx="333" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
                   <c:v>13029</c:v>
+                </c:pt>
+                <c:pt idx="334" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ ">
+                  <c:v>13044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3355,6 +3361,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4365,6 +4374,9 @@
                 </c:pt>
                 <c:pt idx="333">
                   <c:v>10492</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>10501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5416,6 +5428,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6425,6 +6440,9 @@
                   <c:v>1251</c:v>
                 </c:pt>
                 <c:pt idx="333">
+                  <c:v>1276</c:v>
+                </c:pt>
+                <c:pt idx="334">
                   <c:v>1276</c:v>
                 </c:pt>
               </c:numCache>
@@ -7496,6 +7514,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8506,6 +8527,9 @@
                 </c:pt>
                 <c:pt idx="333">
                   <c:v>1261</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>1267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9939,6 +9963,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -10948,6 +10975,9 @@
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="333">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="334">
                   <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
@@ -12001,6 +12031,9 @@
                 <c:pt idx="333">
                   <c:v>46059</c:v>
                 </c:pt>
+                <c:pt idx="334">
+                  <c:v>46067</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -13010,6 +13043,9 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="333">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="334">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -14838,13 +14874,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:Q336"/>
+  <dimension ref="A1:Q337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G337" sqref="G337"/>
+      <selection pane="bottomRight" activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28971,6 +29007,49 @@
       <c r="M336" s="19"/>
       <c r="N336" s="19"/>
       <c r="O336">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>46067</v>
+      </c>
+      <c r="B337" s="2">
+        <v>9</v>
+      </c>
+      <c r="C337">
+        <f t="shared" ref="C337" si="511">SUM(D337:F337)</f>
+        <v>1673</v>
+      </c>
+      <c r="D337">
+        <v>1105</v>
+      </c>
+      <c r="E337">
+        <v>371</v>
+      </c>
+      <c r="F337" s="3">
+        <v>197</v>
+      </c>
+      <c r="G337" s="4">
+        <v>120</v>
+      </c>
+      <c r="H337" s="16">
+        <f t="shared" ref="H337" si="512">SUM(I337:K337)</f>
+        <v>13044</v>
+      </c>
+      <c r="I337" s="5">
+        <v>10501</v>
+      </c>
+      <c r="J337" s="6">
+        <v>1276</v>
+      </c>
+      <c r="K337" s="7">
+        <v>1267</v>
+      </c>
+      <c r="L337" s="19"/>
+      <c r="M337" s="19"/>
+      <c r="N337" s="19"/>
+      <c r="O337">
         <v>31</v>
       </c>
     </row>
@@ -28993,7 +29072,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF22" sqref="AF22"/>
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>